<commit_message>
fixed: disabled buttons for - Select Professor - added: click and drag to select on delete course
</commit_message>
<xml_diff>
--- a/static/files/subject_data.xlsx
+++ b/static/files/subject_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mark Anthony Mamauag\Desktop\Scheduler\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jenze\Desktop\PROF LOADING CAPSTONE PROJECT\ClassScheduler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0F91AC0-B9B6-4133-92D0-36B5B85F5EBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CE057C6-192D-4C62-8093-D380F2AABCAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="119">
   <si>
     <t>COURSE CODE</t>
   </si>
@@ -364,13 +364,31 @@
   </si>
   <si>
     <t>10:30 AM - 12:00 PM</t>
+  </si>
+  <si>
+    <t>TEST1</t>
+  </si>
+  <si>
+    <t>TEST2</t>
+  </si>
+  <si>
+    <t>TEST3</t>
+  </si>
+  <si>
+    <t>TESTING ONLY 1</t>
+  </si>
+  <si>
+    <t>TESTING ONLY 2</t>
+  </si>
+  <si>
+    <t>TESTING ONLY 3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -411,6 +429,12 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -463,7 +487,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -498,7 +522,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -809,21 +832,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H160"/>
+  <dimension ref="A1:H161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="A141" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="G163" sqref="G163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.28515625" customWidth="1"/>
     <col min="2" max="2" width="21.85546875" style="13" customWidth="1"/>
-    <col min="3" max="3" width="43.140625" style="27" customWidth="1"/>
+    <col min="3" max="3" width="43.140625" style="26" customWidth="1"/>
     <col min="4" max="4" width="10" style="13" customWidth="1"/>
     <col min="5" max="5" width="24.28515625" customWidth="1"/>
     <col min="6" max="6" width="20.7109375" customWidth="1"/>
-    <col min="7" max="7" width="28.5703125" style="15" customWidth="1"/>
+    <col min="7" max="7" width="28.5703125" style="14" customWidth="1"/>
     <col min="8" max="8" width="9.140625" style="13"/>
   </cols>
   <sheetData>
@@ -834,7 +857,7 @@
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="16" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -853,8 +876,8 @@
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="1"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="2"/>
@@ -862,7 +885,7 @@
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="1"/>
-      <c r="C3" s="18"/>
+      <c r="C3" s="17"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -875,7 +898,7 @@
       <c r="B4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="18" t="s">
         <v>21</v>
       </c>
       <c r="D4" s="4">
@@ -894,7 +917,7 @@
       <c r="B5" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="C5" s="18" t="s">
         <v>21</v>
       </c>
       <c r="D5" s="4">
@@ -913,7 +936,7 @@
       <c r="B6" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="C6" s="18" t="s">
         <v>21</v>
       </c>
       <c r="D6" s="4">
@@ -928,7 +951,7 @@
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="4"/>
-      <c r="C7" s="19"/>
+      <c r="C7" s="18"/>
       <c r="D7" s="4"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
@@ -937,7 +960,7 @@
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="4"/>
-      <c r="C8" s="20"/>
+      <c r="C8" s="19"/>
       <c r="D8" s="4"/>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
@@ -950,7 +973,7 @@
       <c r="B9" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="19" t="s">
+      <c r="C9" s="18" t="s">
         <v>22</v>
       </c>
       <c r="D9" s="4">
@@ -969,7 +992,7 @@
       <c r="B10" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="19" t="s">
+      <c r="C10" s="18" t="s">
         <v>22</v>
       </c>
       <c r="D10" s="4">
@@ -988,7 +1011,7 @@
       <c r="B11" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="19" t="s">
+      <c r="C11" s="18" t="s">
         <v>22</v>
       </c>
       <c r="D11" s="4">
@@ -1003,7 +1026,7 @@
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="4"/>
-      <c r="C12" s="21"/>
+      <c r="C12" s="20"/>
       <c r="D12" s="4"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
@@ -1016,7 +1039,7 @@
       <c r="B13" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="19" t="s">
+      <c r="C13" s="18" t="s">
         <v>26</v>
       </c>
       <c r="D13" s="4">
@@ -1035,7 +1058,7 @@
       <c r="B14" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="19" t="s">
+      <c r="C14" s="18" t="s">
         <v>26</v>
       </c>
       <c r="D14" s="4">
@@ -1054,7 +1077,7 @@
       <c r="B15" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="19" t="s">
+      <c r="C15" s="18" t="s">
         <v>26</v>
       </c>
       <c r="D15" s="4">
@@ -1069,7 +1092,7 @@
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="4"/>
-      <c r="C16" s="21"/>
+      <c r="C16" s="20"/>
       <c r="D16" s="4"/>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
@@ -1082,7 +1105,7 @@
       <c r="B17" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C17" s="22" t="s">
+      <c r="C17" s="21" t="s">
         <v>28</v>
       </c>
       <c r="D17" s="4">
@@ -1101,7 +1124,7 @@
       <c r="B18" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="22" t="s">
+      <c r="C18" s="21" t="s">
         <v>28</v>
       </c>
       <c r="D18" s="4">
@@ -1120,7 +1143,7 @@
       <c r="B19" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C19" s="22" t="s">
+      <c r="C19" s="21" t="s">
         <v>28</v>
       </c>
       <c r="D19" s="4">
@@ -1135,7 +1158,7 @@
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="9"/>
-      <c r="C20" s="22"/>
+      <c r="C20" s="21"/>
       <c r="D20" s="4"/>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
@@ -1144,7 +1167,7 @@
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="4"/>
-      <c r="C21" s="18"/>
+      <c r="C21" s="17"/>
       <c r="D21" s="4"/>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
@@ -1157,7 +1180,7 @@
       <c r="B22" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C22" s="19" t="s">
+      <c r="C22" s="18" t="s">
         <v>82</v>
       </c>
       <c r="D22" s="4">
@@ -1178,7 +1201,7 @@
       <c r="B23" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="19" t="s">
+      <c r="C23" s="18" t="s">
         <v>82</v>
       </c>
       <c r="D23" s="4">
@@ -1195,7 +1218,7 @@
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="4"/>
-      <c r="C24" s="21"/>
+      <c r="C24" s="20"/>
       <c r="D24" s="4"/>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
@@ -1208,7 +1231,7 @@
       <c r="B25" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C25" s="19" t="s">
+      <c r="C25" s="18" t="s">
         <v>18</v>
       </c>
       <c r="D25" s="4">
@@ -1229,7 +1252,7 @@
       <c r="B26" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C26" s="19" t="s">
+      <c r="C26" s="18" t="s">
         <v>18</v>
       </c>
       <c r="D26" s="4">
@@ -1243,24 +1266,24 @@
       </c>
       <c r="G26" s="5"/>
     </row>
-    <row r="27" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
       <c r="B27" s="6"/>
-      <c r="C27" s="23"/>
+      <c r="C27" s="22"/>
       <c r="D27" s="6"/>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
-      <c r="H27" s="16"/>
-    </row>
-    <row r="28" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H27" s="15"/>
+    </row>
+    <row r="28" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <v>17</v>
       </c>
       <c r="B28" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="C28" s="19" t="s">
+      <c r="C28" s="18" t="s">
         <v>32</v>
       </c>
       <c r="D28" s="4">
@@ -1273,16 +1296,16 @@
         <v>112</v>
       </c>
       <c r="G28" s="5"/>
-      <c r="H28" s="16"/>
-    </row>
-    <row r="29" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H28" s="15"/>
+    </row>
+    <row r="29" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <v>18</v>
       </c>
       <c r="B29" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="C29" s="19" t="s">
+      <c r="C29" s="18" t="s">
         <v>32</v>
       </c>
       <c r="D29" s="4">
@@ -1295,12 +1318,12 @@
         <v>112</v>
       </c>
       <c r="G29" s="5"/>
-      <c r="H29" s="16"/>
+      <c r="H29" s="15"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
       <c r="B30" s="4"/>
-      <c r="C30" s="21"/>
+      <c r="C30" s="20"/>
       <c r="D30" s="4"/>
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
@@ -1313,7 +1336,7 @@
       <c r="B31" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="C31" s="19" t="s">
+      <c r="C31" s="18" t="s">
         <v>35</v>
       </c>
       <c r="D31" s="4">
@@ -1334,7 +1357,7 @@
       <c r="B32" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="C32" s="19" t="s">
+      <c r="C32" s="18" t="s">
         <v>35</v>
       </c>
       <c r="D32" s="4">
@@ -1351,7 +1374,7 @@
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="3"/>
       <c r="B33" s="9"/>
-      <c r="C33" s="19"/>
+      <c r="C33" s="18"/>
       <c r="D33" s="4"/>
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
@@ -1360,7 +1383,7 @@
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
       <c r="B34" s="9"/>
-      <c r="C34" s="21"/>
+      <c r="C34" s="20"/>
       <c r="D34" s="4"/>
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
@@ -1373,7 +1396,7 @@
       <c r="B35" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C35" s="19" t="s">
+      <c r="C35" s="18" t="s">
         <v>37</v>
       </c>
       <c r="D35" s="4">
@@ -1392,7 +1415,7 @@
       <c r="B36" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C36" s="19" t="s">
+      <c r="C36" s="18" t="s">
         <v>37</v>
       </c>
       <c r="D36" s="4">
@@ -1407,7 +1430,7 @@
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="3"/>
       <c r="B37" s="4"/>
-      <c r="C37" s="21"/>
+      <c r="C37" s="20"/>
       <c r="D37" s="4"/>
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
@@ -1420,7 +1443,7 @@
       <c r="B38" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C38" s="24" t="s">
+      <c r="C38" s="23" t="s">
         <v>39</v>
       </c>
       <c r="D38" s="4">
@@ -1439,7 +1462,7 @@
       <c r="B39" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C39" s="24" t="s">
+      <c r="C39" s="23" t="s">
         <v>39</v>
       </c>
       <c r="D39" s="4">
@@ -1454,7 +1477,7 @@
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="3"/>
       <c r="B40" s="10"/>
-      <c r="C40" s="24"/>
+      <c r="C40" s="23"/>
       <c r="D40" s="4"/>
       <c r="E40" s="3"/>
       <c r="F40" s="3"/>
@@ -1467,7 +1490,7 @@
       <c r="B41" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="C41" s="25" t="s">
+      <c r="C41" s="24" t="s">
         <v>64</v>
       </c>
       <c r="D41" s="4">
@@ -1486,7 +1509,7 @@
       <c r="B42" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="C42" s="25" t="s">
+      <c r="C42" s="24" t="s">
         <v>64</v>
       </c>
       <c r="D42" s="4">
@@ -1501,7 +1524,7 @@
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="3"/>
       <c r="B43" s="10"/>
-      <c r="C43" s="24"/>
+      <c r="C43" s="23"/>
       <c r="D43" s="4"/>
       <c r="E43" s="3"/>
       <c r="F43" s="3"/>
@@ -1510,7 +1533,7 @@
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="3"/>
       <c r="B44" s="4"/>
-      <c r="C44" s="20"/>
+      <c r="C44" s="19"/>
       <c r="D44" s="4"/>
       <c r="E44" s="3"/>
       <c r="F44" s="3"/>
@@ -1523,7 +1546,7 @@
       <c r="B45" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="C45" s="19" t="s">
+      <c r="C45" s="18" t="s">
         <v>41</v>
       </c>
       <c r="D45" s="4">
@@ -1542,7 +1565,7 @@
       <c r="B46" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="C46" s="19" t="s">
+      <c r="C46" s="18" t="s">
         <v>41</v>
       </c>
       <c r="D46" s="4">
@@ -1561,7 +1584,7 @@
       <c r="B47" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="C47" s="19" t="s">
+      <c r="C47" s="18" t="s">
         <v>41</v>
       </c>
       <c r="D47" s="4">
@@ -1576,7 +1599,7 @@
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="3"/>
       <c r="B48" s="4"/>
-      <c r="C48" s="21"/>
+      <c r="C48" s="20"/>
       <c r="D48" s="4"/>
       <c r="E48" s="3"/>
       <c r="F48" s="3"/>
@@ -1589,7 +1612,7 @@
       <c r="B49" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="C49" s="19" t="s">
+      <c r="C49" s="18" t="s">
         <v>43</v>
       </c>
       <c r="D49" s="4">
@@ -1608,7 +1631,7 @@
       <c r="B50" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="C50" s="19" t="s">
+      <c r="C50" s="18" t="s">
         <v>43</v>
       </c>
       <c r="D50" s="4">
@@ -1627,7 +1650,7 @@
       <c r="B51" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="C51" s="19" t="s">
+      <c r="C51" s="18" t="s">
         <v>43</v>
       </c>
       <c r="D51" s="4">
@@ -1642,7 +1665,7 @@
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="3"/>
       <c r="B52" s="4"/>
-      <c r="C52" s="21"/>
+      <c r="C52" s="20"/>
       <c r="D52" s="4"/>
       <c r="E52" s="3"/>
       <c r="F52" s="3"/>
@@ -1655,7 +1678,7 @@
       <c r="B53" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="C53" s="19" t="s">
+      <c r="C53" s="18" t="s">
         <v>45</v>
       </c>
       <c r="D53" s="4">
@@ -1674,7 +1697,7 @@
       <c r="B54" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="C54" s="19" t="s">
+      <c r="C54" s="18" t="s">
         <v>45</v>
       </c>
       <c r="D54" s="4">
@@ -1693,7 +1716,7 @@
       <c r="B55" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="C55" s="19" t="s">
+      <c r="C55" s="18" t="s">
         <v>45</v>
       </c>
       <c r="D55" s="4">
@@ -1708,7 +1731,7 @@
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="3"/>
       <c r="B56" s="4"/>
-      <c r="C56" s="21"/>
+      <c r="C56" s="20"/>
       <c r="D56" s="4"/>
       <c r="E56" s="3"/>
       <c r="F56" s="3"/>
@@ -1716,8 +1739,8 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="3"/>
-      <c r="B57" s="28"/>
-      <c r="C57" s="28"/>
+      <c r="B57" s="27"/>
+      <c r="C57" s="27"/>
       <c r="D57" s="4"/>
       <c r="E57" s="3"/>
       <c r="F57" s="3"/>
@@ -1726,7 +1749,7 @@
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="3"/>
       <c r="B58" s="4"/>
-      <c r="C58" s="20"/>
+      <c r="C58" s="19"/>
       <c r="D58" s="4"/>
       <c r="E58" s="3"/>
       <c r="F58" s="3"/>
@@ -1739,7 +1762,7 @@
       <c r="B59" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C59" s="19" t="s">
+      <c r="C59" s="18" t="s">
         <v>18</v>
       </c>
       <c r="D59" s="4">
@@ -1758,7 +1781,7 @@
       <c r="B60" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C60" s="19" t="s">
+      <c r="C60" s="18" t="s">
         <v>18</v>
       </c>
       <c r="D60" s="4">
@@ -1777,7 +1800,7 @@
       <c r="B61" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C61" s="19" t="s">
+      <c r="C61" s="18" t="s">
         <v>18</v>
       </c>
       <c r="D61" s="4">
@@ -1792,7 +1815,7 @@
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="3"/>
       <c r="B62" s="4"/>
-      <c r="C62" s="19"/>
+      <c r="C62" s="18"/>
       <c r="D62" s="4"/>
       <c r="E62" s="3"/>
       <c r="F62" s="3"/>
@@ -1801,7 +1824,7 @@
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="3"/>
       <c r="B63" s="4"/>
-      <c r="C63" s="20"/>
+      <c r="C63" s="19"/>
       <c r="D63" s="4"/>
       <c r="E63" s="3"/>
       <c r="F63" s="3"/>
@@ -1814,7 +1837,7 @@
       <c r="B64" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="C64" s="19" t="s">
+      <c r="C64" s="18" t="s">
         <v>51</v>
       </c>
       <c r="D64" s="4">
@@ -1833,7 +1856,7 @@
       <c r="B65" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="C65" s="19" t="s">
+      <c r="C65" s="18" t="s">
         <v>51</v>
       </c>
       <c r="D65" s="4">
@@ -1852,7 +1875,7 @@
       <c r="B66" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="C66" s="19" t="s">
+      <c r="C66" s="18" t="s">
         <v>51</v>
       </c>
       <c r="D66" s="4">
@@ -1867,7 +1890,7 @@
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="3"/>
       <c r="B67" s="9"/>
-      <c r="C67" s="19"/>
+      <c r="C67" s="18"/>
       <c r="D67" s="4"/>
       <c r="E67" s="3"/>
       <c r="F67" s="3"/>
@@ -1876,7 +1899,7 @@
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="3"/>
       <c r="B68" s="4"/>
-      <c r="C68" s="21"/>
+      <c r="C68" s="20"/>
       <c r="D68" s="4"/>
       <c r="E68" s="3"/>
       <c r="F68" s="3"/>
@@ -1889,7 +1912,7 @@
       <c r="B69" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C69" s="19" t="s">
+      <c r="C69" s="18" t="s">
         <v>20</v>
       </c>
       <c r="D69" s="4">
@@ -1908,7 +1931,7 @@
       <c r="B70" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C70" s="19" t="s">
+      <c r="C70" s="18" t="s">
         <v>20</v>
       </c>
       <c r="D70" s="4">
@@ -1927,7 +1950,7 @@
       <c r="B71" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C71" s="19" t="s">
+      <c r="C71" s="18" t="s">
         <v>20</v>
       </c>
       <c r="D71" s="4">
@@ -1942,7 +1965,7 @@
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="3"/>
       <c r="B72" s="4"/>
-      <c r="C72" s="19"/>
+      <c r="C72" s="18"/>
       <c r="D72" s="4"/>
       <c r="E72" s="3"/>
       <c r="F72" s="3"/>
@@ -1955,7 +1978,7 @@
       <c r="B73" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="C73" s="19" t="s">
+      <c r="C73" s="18" t="s">
         <v>56</v>
       </c>
       <c r="D73" s="4">
@@ -1974,7 +1997,7 @@
       <c r="B74" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="C74" s="19" t="s">
+      <c r="C74" s="18" t="s">
         <v>56</v>
       </c>
       <c r="D74" s="4">
@@ -1993,7 +2016,7 @@
       <c r="B75" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="C75" s="19" t="s">
+      <c r="C75" s="18" t="s">
         <v>56</v>
       </c>
       <c r="D75" s="4">
@@ -2008,7 +2031,7 @@
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="3"/>
       <c r="B76" s="4"/>
-      <c r="C76" s="21"/>
+      <c r="C76" s="20"/>
       <c r="D76" s="4"/>
       <c r="E76" s="3"/>
       <c r="F76" s="3"/>
@@ -2017,7 +2040,7 @@
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="3"/>
       <c r="B77" s="4"/>
-      <c r="C77" s="20"/>
+      <c r="C77" s="19"/>
       <c r="D77" s="4"/>
       <c r="E77" s="3"/>
       <c r="F77" s="3"/>
@@ -2030,7 +2053,7 @@
       <c r="B78" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="C78" s="19" t="s">
+      <c r="C78" s="18" t="s">
         <v>58</v>
       </c>
       <c r="D78" s="4">
@@ -2049,7 +2072,7 @@
       <c r="B79" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="C79" s="19" t="s">
+      <c r="C79" s="18" t="s">
         <v>58</v>
       </c>
       <c r="D79" s="4">
@@ -2068,7 +2091,7 @@
       <c r="B80" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="C80" s="19" t="s">
+      <c r="C80" s="18" t="s">
         <v>58</v>
       </c>
       <c r="D80" s="4">
@@ -2087,7 +2110,7 @@
       <c r="B81" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="C81" s="19" t="s">
+      <c r="C81" s="18" t="s">
         <v>58</v>
       </c>
       <c r="D81" s="4">
@@ -2102,7 +2125,7 @@
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="3"/>
       <c r="B82" s="4"/>
-      <c r="C82" s="21"/>
+      <c r="C82" s="20"/>
       <c r="D82" s="4"/>
       <c r="E82" s="3"/>
       <c r="F82" s="3"/>
@@ -2115,7 +2138,7 @@
       <c r="B83" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="C83" s="19" t="s">
+      <c r="C83" s="18" t="s">
         <v>60</v>
       </c>
       <c r="D83" s="4">
@@ -2134,7 +2157,7 @@
       <c r="B84" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="C84" s="19" t="s">
+      <c r="C84" s="18" t="s">
         <v>60</v>
       </c>
       <c r="D84" s="4">
@@ -2153,7 +2176,7 @@
       <c r="B85" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="C85" s="19" t="s">
+      <c r="C85" s="18" t="s">
         <v>60</v>
       </c>
       <c r="D85" s="4">
@@ -2172,7 +2195,7 @@
       <c r="B86" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="C86" s="19" t="s">
+      <c r="C86" s="18" t="s">
         <v>60</v>
       </c>
       <c r="D86" s="4">
@@ -2187,7 +2210,7 @@
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="3"/>
       <c r="B87" s="4"/>
-      <c r="C87" s="21"/>
+      <c r="C87" s="20"/>
       <c r="D87" s="4"/>
       <c r="E87" s="3"/>
       <c r="F87" s="3"/>
@@ -2200,7 +2223,7 @@
       <c r="B88" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="C88" s="19" t="s">
+      <c r="C88" s="18" t="s">
         <v>62</v>
       </c>
       <c r="D88" s="4">
@@ -2219,7 +2242,7 @@
       <c r="B89" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="C89" s="19" t="s">
+      <c r="C89" s="18" t="s">
         <v>62</v>
       </c>
       <c r="D89" s="4">
@@ -2238,7 +2261,7 @@
       <c r="B90" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="C90" s="19" t="s">
+      <c r="C90" s="18" t="s">
         <v>62</v>
       </c>
       <c r="D90" s="4">
@@ -2257,7 +2280,7 @@
       <c r="B91" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="C91" s="19" t="s">
+      <c r="C91" s="18" t="s">
         <v>62</v>
       </c>
       <c r="D91" s="4">
@@ -2272,7 +2295,7 @@
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="3"/>
       <c r="B92" s="4"/>
-      <c r="C92" s="21"/>
+      <c r="C92" s="20"/>
       <c r="D92" s="4"/>
       <c r="E92" s="3"/>
       <c r="F92" s="3"/>
@@ -2285,7 +2308,7 @@
       <c r="B93" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="C93" s="19" t="s">
+      <c r="C93" s="18" t="s">
         <v>64</v>
       </c>
       <c r="D93" s="4">
@@ -2304,7 +2327,7 @@
       <c r="B94" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="C94" s="19" t="s">
+      <c r="C94" s="18" t="s">
         <v>64</v>
       </c>
       <c r="D94" s="4">
@@ -2323,7 +2346,7 @@
       <c r="B95" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="C95" s="19" t="s">
+      <c r="C95" s="18" t="s">
         <v>64</v>
       </c>
       <c r="D95" s="4">
@@ -2342,7 +2365,7 @@
       <c r="B96" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="C96" s="19" t="s">
+      <c r="C96" s="18" t="s">
         <v>64</v>
       </c>
       <c r="D96" s="4">
@@ -2357,7 +2380,7 @@
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="3"/>
       <c r="B97" s="4"/>
-      <c r="C97" s="21"/>
+      <c r="C97" s="20"/>
       <c r="D97" s="4"/>
       <c r="E97" s="3"/>
       <c r="F97" s="3"/>
@@ -2370,7 +2393,7 @@
       <c r="B98" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="C98" s="19" t="s">
+      <c r="C98" s="18" t="s">
         <v>66</v>
       </c>
       <c r="D98" s="4">
@@ -2389,7 +2412,7 @@
       <c r="B99" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="C99" s="19" t="s">
+      <c r="C99" s="18" t="s">
         <v>66</v>
       </c>
       <c r="D99" s="4">
@@ -2408,7 +2431,7 @@
       <c r="B100" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="C100" s="19" t="s">
+      <c r="C100" s="18" t="s">
         <v>66</v>
       </c>
       <c r="D100" s="4">
@@ -2427,7 +2450,7 @@
       <c r="B101" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="C101" s="19" t="s">
+      <c r="C101" s="18" t="s">
         <v>66</v>
       </c>
       <c r="D101" s="4">
@@ -2442,7 +2465,7 @@
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" s="3"/>
       <c r="B102" s="4"/>
-      <c r="C102" s="21"/>
+      <c r="C102" s="20"/>
       <c r="D102" s="4"/>
       <c r="E102" s="3"/>
       <c r="F102" s="3"/>
@@ -2455,7 +2478,7 @@
       <c r="B103" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="C103" s="19" t="s">
+      <c r="C103" s="18" t="s">
         <v>68</v>
       </c>
       <c r="D103" s="4">
@@ -2474,7 +2497,7 @@
       <c r="B104" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="C104" s="19" t="s">
+      <c r="C104" s="18" t="s">
         <v>68</v>
       </c>
       <c r="D104" s="4">
@@ -2493,7 +2516,7 @@
       <c r="B105" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="C105" s="19" t="s">
+      <c r="C105" s="18" t="s">
         <v>68</v>
       </c>
       <c r="D105" s="4">
@@ -2512,7 +2535,7 @@
       <c r="B106" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="C106" s="19" t="s">
+      <c r="C106" s="18" t="s">
         <v>68</v>
       </c>
       <c r="D106" s="4">
@@ -2527,7 +2550,7 @@
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" s="3"/>
       <c r="B107" s="4"/>
-      <c r="C107" s="21"/>
+      <c r="C107" s="20"/>
       <c r="D107" s="4"/>
       <c r="E107" s="3"/>
       <c r="F107" s="3"/>
@@ -2536,7 +2559,7 @@
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" s="3"/>
       <c r="B108" s="4"/>
-      <c r="C108" s="20"/>
+      <c r="C108" s="19"/>
       <c r="D108" s="4"/>
       <c r="E108" s="3"/>
       <c r="F108" s="3"/>
@@ -2549,7 +2572,7 @@
       <c r="B109" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="C109" s="23" t="s">
+      <c r="C109" s="22" t="s">
         <v>73</v>
       </c>
       <c r="D109" s="4">
@@ -2568,7 +2591,7 @@
       <c r="B110" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="C110" s="23" t="s">
+      <c r="C110" s="22" t="s">
         <v>73</v>
       </c>
       <c r="D110" s="4">
@@ -2587,7 +2610,7 @@
       <c r="B111" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="C111" s="23" t="s">
+      <c r="C111" s="22" t="s">
         <v>73</v>
       </c>
       <c r="D111" s="4">
@@ -2602,7 +2625,7 @@
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" s="3"/>
       <c r="B112" s="4"/>
-      <c r="C112" s="21"/>
+      <c r="C112" s="20"/>
       <c r="D112" s="4"/>
       <c r="E112" s="3"/>
       <c r="F112" s="5"/>
@@ -2615,7 +2638,7 @@
       <c r="B113" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="C113" s="25" t="s">
+      <c r="C113" s="24" t="s">
         <v>75</v>
       </c>
       <c r="D113" s="4">
@@ -2634,7 +2657,7 @@
       <c r="B114" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="C114" s="25" t="s">
+      <c r="C114" s="24" t="s">
         <v>75</v>
       </c>
       <c r="D114" s="4">
@@ -2653,7 +2676,7 @@
       <c r="B115" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="C115" s="25" t="s">
+      <c r="C115" s="24" t="s">
         <v>75</v>
       </c>
       <c r="D115" s="4">
@@ -2668,7 +2691,7 @@
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" s="3"/>
       <c r="B116" s="4"/>
-      <c r="C116" s="21"/>
+      <c r="C116" s="20"/>
       <c r="D116" s="4"/>
       <c r="E116" s="3"/>
       <c r="F116" s="3"/>
@@ -2681,7 +2704,7 @@
       <c r="B117" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="C117" s="25" t="s">
+      <c r="C117" s="24" t="s">
         <v>77</v>
       </c>
       <c r="D117" s="4">
@@ -2700,7 +2723,7 @@
       <c r="B118" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="C118" s="25" t="s">
+      <c r="C118" s="24" t="s">
         <v>77</v>
       </c>
       <c r="D118" s="4">
@@ -2719,7 +2742,7 @@
       <c r="B119" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="C119" s="25" t="s">
+      <c r="C119" s="24" t="s">
         <v>77</v>
       </c>
       <c r="D119" s="4">
@@ -2734,7 +2757,7 @@
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" s="3"/>
       <c r="B120" s="4"/>
-      <c r="C120" s="21"/>
+      <c r="C120" s="20"/>
       <c r="D120" s="4"/>
       <c r="E120" s="3"/>
       <c r="F120" s="3"/>
@@ -2747,7 +2770,7 @@
       <c r="B121" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C121" s="26" t="s">
+      <c r="C121" s="25" t="s">
         <v>79</v>
       </c>
       <c r="D121" s="4">
@@ -2766,7 +2789,7 @@
       <c r="B122" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C122" s="26" t="s">
+      <c r="C122" s="25" t="s">
         <v>79</v>
       </c>
       <c r="D122" s="4">
@@ -2785,7 +2808,7 @@
       <c r="B123" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C123" s="26" t="s">
+      <c r="C123" s="25" t="s">
         <v>79</v>
       </c>
       <c r="D123" s="4">
@@ -2804,7 +2827,7 @@
       <c r="B124" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C124" s="26" t="s">
+      <c r="C124" s="25" t="s">
         <v>79</v>
       </c>
       <c r="D124" s="4">
@@ -2819,7 +2842,7 @@
     <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" s="3"/>
       <c r="B125" s="4"/>
-      <c r="C125" s="26"/>
+      <c r="C125" s="25"/>
       <c r="D125" s="4"/>
       <c r="E125" s="3"/>
       <c r="F125" s="3"/>
@@ -2827,8 +2850,8 @@
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" s="3"/>
-      <c r="B126" s="28"/>
-      <c r="C126" s="28"/>
+      <c r="B126" s="27"/>
+      <c r="C126" s="27"/>
       <c r="D126" s="4"/>
       <c r="E126" s="3"/>
       <c r="F126" s="3"/>
@@ -2837,7 +2860,7 @@
     <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" s="3"/>
       <c r="B127" s="1"/>
-      <c r="C127" s="17"/>
+      <c r="C127" s="16"/>
       <c r="D127" s="4"/>
       <c r="E127" s="3"/>
       <c r="F127" s="3"/>
@@ -2850,7 +2873,7 @@
       <c r="B128" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="C128" s="19" t="s">
+      <c r="C128" s="18" t="s">
         <v>68</v>
       </c>
       <c r="D128" s="4">
@@ -2869,7 +2892,7 @@
       <c r="B129" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="C129" s="19" t="s">
+      <c r="C129" s="18" t="s">
         <v>68</v>
       </c>
       <c r="D129" s="4">
@@ -2888,7 +2911,7 @@
       <c r="B130" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="C130" s="19" t="s">
+      <c r="C130" s="18" t="s">
         <v>68</v>
       </c>
       <c r="D130" s="4">
@@ -2907,7 +2930,7 @@
       <c r="B131" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="C131" s="19" t="s">
+      <c r="C131" s="18" t="s">
         <v>68</v>
       </c>
       <c r="D131" s="4">
@@ -2922,7 +2945,7 @@
     <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132" s="3"/>
       <c r="B132" s="9"/>
-      <c r="C132" s="19"/>
+      <c r="C132" s="18"/>
       <c r="D132" s="4"/>
       <c r="E132" s="7"/>
       <c r="F132" s="3"/>
@@ -2935,7 +2958,7 @@
       <c r="B133" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="C133" s="19" t="s">
+      <c r="C133" s="18" t="s">
         <v>56</v>
       </c>
       <c r="D133" s="4">
@@ -2954,7 +2977,7 @@
       <c r="B134" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="C134" s="19" t="s">
+      <c r="C134" s="18" t="s">
         <v>56</v>
       </c>
       <c r="D134" s="4">
@@ -2973,7 +2996,7 @@
       <c r="B135" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="C135" s="19" t="s">
+      <c r="C135" s="18" t="s">
         <v>56</v>
       </c>
       <c r="D135" s="4">
@@ -2992,7 +3015,7 @@
       <c r="B136" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="C136" s="19" t="s">
+      <c r="C136" s="18" t="s">
         <v>56</v>
       </c>
       <c r="D136" s="4">
@@ -3011,7 +3034,7 @@
       <c r="B137" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="C137" s="19" t="s">
+      <c r="C137" s="18" t="s">
         <v>56</v>
       </c>
       <c r="D137" s="4">
@@ -3030,7 +3053,7 @@
       <c r="B138" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="C138" s="19" t="s">
+      <c r="C138" s="18" t="s">
         <v>56</v>
       </c>
       <c r="D138" s="4">
@@ -3049,7 +3072,7 @@
       <c r="B139" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="C139" s="19" t="s">
+      <c r="C139" s="18" t="s">
         <v>56</v>
       </c>
       <c r="D139" s="4">
@@ -3068,7 +3091,7 @@
       <c r="B140" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="C140" s="19" t="s">
+      <c r="C140" s="18" t="s">
         <v>56</v>
       </c>
       <c r="D140" s="4">
@@ -3087,7 +3110,7 @@
       <c r="B141" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="C141" s="19" t="s">
+      <c r="C141" s="18" t="s">
         <v>56</v>
       </c>
       <c r="D141" s="4">
@@ -3106,7 +3129,7 @@
       <c r="B142" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="C142" s="19" t="s">
+      <c r="C142" s="18" t="s">
         <v>56</v>
       </c>
       <c r="D142" s="4">
@@ -3125,7 +3148,7 @@
       <c r="B143" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="C143" s="19" t="s">
+      <c r="C143" s="18" t="s">
         <v>56</v>
       </c>
       <c r="D143" s="4">
@@ -3144,7 +3167,7 @@
       <c r="B144" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="C144" s="19" t="s">
+      <c r="C144" s="18" t="s">
         <v>56</v>
       </c>
       <c r="D144" s="4">
@@ -3163,7 +3186,7 @@
       <c r="B145" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="C145" s="19" t="s">
+      <c r="C145" s="18" t="s">
         <v>56</v>
       </c>
       <c r="D145" s="4">
@@ -3178,7 +3201,7 @@
     <row r="146" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A146" s="3"/>
       <c r="B146" s="1"/>
-      <c r="C146" s="17"/>
+      <c r="C146" s="16"/>
       <c r="D146" s="4"/>
       <c r="E146" s="3"/>
       <c r="F146" s="3"/>
@@ -3191,7 +3214,7 @@
       <c r="B147" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C147" s="21" t="s">
+      <c r="C147" s="20" t="s">
         <v>18</v>
       </c>
       <c r="D147" s="4">
@@ -3210,7 +3233,7 @@
       <c r="B148" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C148" s="21" t="s">
+      <c r="C148" s="20" t="s">
         <v>18</v>
       </c>
       <c r="D148" s="4">
@@ -3229,7 +3252,7 @@
       <c r="B149" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C149" s="21" t="s">
+      <c r="C149" s="20" t="s">
         <v>18</v>
       </c>
       <c r="D149" s="4">
@@ -3248,7 +3271,7 @@
       <c r="B150" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C150" s="21" t="s">
+      <c r="C150" s="20" t="s">
         <v>18</v>
       </c>
       <c r="D150" s="4">
@@ -3267,7 +3290,7 @@
       <c r="B151" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C151" s="21" t="s">
+      <c r="C151" s="20" t="s">
         <v>18</v>
       </c>
       <c r="D151" s="4">
@@ -3286,7 +3309,7 @@
       <c r="B152" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C152" s="21" t="s">
+      <c r="C152" s="20" t="s">
         <v>18</v>
       </c>
       <c r="D152" s="4">
@@ -3301,7 +3324,7 @@
     <row r="153" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A153" s="3"/>
       <c r="B153" s="4"/>
-      <c r="C153" s="21"/>
+      <c r="C153" s="20"/>
       <c r="D153" s="4"/>
       <c r="E153" s="3"/>
       <c r="F153" s="3"/>
@@ -3314,7 +3337,7 @@
       <c r="B154" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C154" s="19" t="s">
+      <c r="C154" s="18" t="s">
         <v>20</v>
       </c>
       <c r="D154" s="4">
@@ -3333,7 +3356,7 @@
       <c r="B155" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C155" s="19" t="s">
+      <c r="C155" s="18" t="s">
         <v>20</v>
       </c>
       <c r="D155" s="4">
@@ -3352,7 +3375,7 @@
       <c r="B156" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C156" s="19" t="s">
+      <c r="C156" s="18" t="s">
         <v>20</v>
       </c>
       <c r="D156" s="4">
@@ -3371,7 +3394,7 @@
       <c r="B157" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C157" s="19" t="s">
+      <c r="C157" s="18" t="s">
         <v>20</v>
       </c>
       <c r="D157" s="4">
@@ -3390,7 +3413,7 @@
       <c r="B158" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C158" s="19" t="s">
+      <c r="C158" s="18" t="s">
         <v>20</v>
       </c>
       <c r="D158" s="4">
@@ -3403,16 +3426,68 @@
       <c r="G158" s="5"/>
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E159" s="14"/>
+      <c r="A159" s="3">
+        <v>29</v>
+      </c>
+      <c r="B159" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="C159" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="D159" s="4">
+        <v>4</v>
+      </c>
+      <c r="E159" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="F159" s="3"/>
+      <c r="G159" s="5"/>
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E160" s="14"/>
+      <c r="A160" s="3">
+        <v>30</v>
+      </c>
+      <c r="B160" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C160" s="18" t="s">
+        <v>117</v>
+      </c>
+      <c r="D160" s="4">
+        <v>5</v>
+      </c>
+      <c r="E160" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="F160" s="3"/>
+      <c r="G160" s="5"/>
+    </row>
+    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A161" s="3">
+        <v>31</v>
+      </c>
+      <c r="B161" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C161" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="D161" s="4">
+        <v>6</v>
+      </c>
+      <c r="E161" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="F161" s="3"/>
+      <c r="G161" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B57:C57"/>
     <mergeCell ref="B126:C126"/>
   </mergeCells>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="14" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
added: courses added now appears in mainscreen added: Year Level in process_excel: and displayed changed: some window titles and button names
</commit_message>
<xml_diff>
--- a/static/files/subject_data.xlsx
+++ b/static/files/subject_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jenze\Desktop\PROF LOADING CAPSTONE PROJECT\ClassScheduler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CE057C6-192D-4C62-8093-D380F2AABCAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8DB5433-C63B-4161-9F90-AF7D47763914}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="118">
   <si>
     <t>COURSE CODE</t>
   </si>
@@ -36,12 +36,6 @@
     <t>COURSE &amp; SEC.</t>
   </si>
   <si>
-    <t>DAY AND TIME</t>
-  </si>
-  <si>
-    <t>FACULTY</t>
-  </si>
-  <si>
     <t>NO.</t>
   </si>
   <si>
@@ -354,18 +348,6 @@
     <t>I-D BSFM (ABM)</t>
   </si>
   <si>
-    <t>7:30 AM - 9:00 AM</t>
-  </si>
-  <si>
-    <t>9:00 AM - 10:30 AM</t>
-  </si>
-  <si>
-    <t>10:30 AM -12:00 PM</t>
-  </si>
-  <si>
-    <t>10:30 AM - 12:00 PM</t>
-  </si>
-  <si>
     <t>TEST1</t>
   </si>
   <si>
@@ -382,6 +364,21 @@
   </si>
   <si>
     <t>TESTING ONLY 3</t>
+  </si>
+  <si>
+    <t>YEAR LEVEL</t>
+  </si>
+  <si>
+    <t>FIRST YEAR</t>
+  </si>
+  <si>
+    <t>SECOND YEAR</t>
+  </si>
+  <si>
+    <t>THIRD YEAR</t>
+  </si>
+  <si>
+    <t>FOURTH YEAR</t>
   </si>
 </sst>
 </file>
@@ -487,7 +484,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -551,6 +548,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -834,8 +834,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A141" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="G163" sqref="G163"/>
+    <sheetView tabSelected="1" topLeftCell="A142" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="C152" sqref="C152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -843,7 +843,7 @@
     <col min="1" max="1" width="5.28515625" customWidth="1"/>
     <col min="2" max="2" width="21.85546875" style="13" customWidth="1"/>
     <col min="3" max="3" width="43.140625" style="26" customWidth="1"/>
-    <col min="4" max="4" width="10" style="13" customWidth="1"/>
+    <col min="4" max="4" width="23" style="13" customWidth="1"/>
     <col min="5" max="5" width="24.28515625" customWidth="1"/>
     <col min="6" max="6" width="20.7109375" customWidth="1"/>
     <col min="7" max="7" width="28.5703125" style="14" customWidth="1"/>
@@ -852,7 +852,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -860,25 +860,23 @@
       <c r="C1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>10</v>
+      <c r="D1" s="16" t="s">
+        <v>113</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>4</v>
-      </c>
+      <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="1"/>
       <c r="C2" s="19"/>
       <c r="D2" s="19"/>
-      <c r="E2" s="1"/>
+      <c r="E2" s="19"/>
       <c r="F2" s="1"/>
       <c r="G2" s="2"/>
     </row>
@@ -896,18 +894,20 @@
         <v>1</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="4">
+        <v>19</v>
+      </c>
+      <c r="D4" s="28" t="s">
+        <v>114</v>
+      </c>
+      <c r="E4" s="4">
         <v>6</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" s="3"/>
+      <c r="F4" s="3" t="s">
+        <v>4</v>
+      </c>
       <c r="G4" s="5"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -915,18 +915,20 @@
         <v>2</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="4">
+        <v>19</v>
+      </c>
+      <c r="D5" s="28" t="s">
+        <v>114</v>
+      </c>
+      <c r="E5" s="4">
         <v>6</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="F5" s="3"/>
+      <c r="F5" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="G5" s="5"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -934,26 +936,28 @@
         <v>3</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="4">
+        <v>19</v>
+      </c>
+      <c r="D6" s="28" t="s">
+        <v>114</v>
+      </c>
+      <c r="E6" s="4">
         <v>6</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="F6" s="3"/>
+      <c r="F6" s="3" t="s">
+        <v>79</v>
+      </c>
       <c r="G6" s="5"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="4"/>
       <c r="C7" s="18"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="3"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="4"/>
       <c r="F7" s="3"/>
       <c r="G7" s="5"/>
     </row>
@@ -961,8 +965,8 @@
       <c r="A8" s="3"/>
       <c r="B8" s="4"/>
       <c r="C8" s="19"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="3"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="4"/>
       <c r="F8" s="3"/>
       <c r="G8" s="5"/>
     </row>
@@ -971,18 +975,20 @@
         <v>4</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="4">
+        <v>20</v>
+      </c>
+      <c r="D9" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="E9" s="4">
         <v>6</v>
       </c>
-      <c r="E9" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F9" s="3"/>
+      <c r="F9" s="3" t="s">
+        <v>5</v>
+      </c>
       <c r="G9" s="5"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -990,18 +996,20 @@
         <v>5</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="4">
+        <v>20</v>
+      </c>
+      <c r="D10" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="E10" s="4">
         <v>6</v>
       </c>
-      <c r="E10" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F10" s="3"/>
+      <c r="F10" s="3" t="s">
+        <v>28</v>
+      </c>
       <c r="G10" s="5"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1009,26 +1017,28 @@
         <v>6</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="4">
+        <v>20</v>
+      </c>
+      <c r="D11" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="E11" s="4">
         <v>6</v>
       </c>
-      <c r="E11" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F11" s="3"/>
+      <c r="F11" s="3" t="s">
+        <v>29</v>
+      </c>
       <c r="G11" s="5"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="4"/>
       <c r="C12" s="20"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="3"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="4"/>
       <c r="F12" s="3"/>
       <c r="G12" s="5"/>
     </row>
@@ -1037,18 +1047,20 @@
         <v>7</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="D13" s="4">
-        <v>3</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F13" s="3"/>
+        <v>24</v>
+      </c>
+      <c r="D13" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="E13" s="4">
+        <v>3</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>5</v>
+      </c>
       <c r="G13" s="5"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -1056,18 +1068,20 @@
         <v>8</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="D14" s="4">
-        <v>3</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F14" s="3"/>
+        <v>24</v>
+      </c>
+      <c r="D14" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="E14" s="4">
+        <v>3</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>28</v>
+      </c>
       <c r="G14" s="5"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -1075,26 +1089,28 @@
         <v>9</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="D15" s="4">
-        <v>3</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F15" s="3"/>
+        <v>24</v>
+      </c>
+      <c r="D15" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="E15" s="4">
+        <v>3</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>29</v>
+      </c>
       <c r="G15" s="5"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="4"/>
       <c r="C16" s="20"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="3"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="4"/>
       <c r="F16" s="3"/>
       <c r="G16" s="5"/>
     </row>
@@ -1103,18 +1119,20 @@
         <v>10</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C17" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="D17" s="4">
-        <v>3</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F17" s="4"/>
+        <v>26</v>
+      </c>
+      <c r="D17" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="E17" s="4">
+        <v>3</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>5</v>
+      </c>
       <c r="G17" s="6"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -1122,18 +1140,20 @@
         <v>11</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C18" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="E18" s="4">
+        <v>3</v>
+      </c>
+      <c r="F18" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D18" s="4">
-        <v>3</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F18" s="3"/>
       <c r="G18" s="5"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -1141,26 +1161,28 @@
         <v>12</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C19" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="D19" s="4">
-        <v>3</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F19" s="3"/>
+        <v>26</v>
+      </c>
+      <c r="D19" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="E19" s="4">
+        <v>3</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>29</v>
+      </c>
       <c r="G19" s="5"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="9"/>
       <c r="C20" s="21"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="3"/>
+      <c r="D20" s="28"/>
+      <c r="E20" s="4"/>
       <c r="F20" s="3"/>
       <c r="G20" s="5"/>
     </row>
@@ -1168,8 +1190,8 @@
       <c r="A21" s="3"/>
       <c r="B21" s="4"/>
       <c r="C21" s="17"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="3"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="4"/>
       <c r="F21" s="3"/>
       <c r="G21" s="5"/>
     </row>
@@ -1178,19 +1200,19 @@
         <v>13</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C22" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="D22" s="4">
+        <v>80</v>
+      </c>
+      <c r="D22" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="E22" s="4">
         <v>4</v>
       </c>
-      <c r="E22" s="3" t="s">
-        <v>8</v>
-      </c>
       <c r="F22" s="3" t="s">
-        <v>109</v>
+        <v>6</v>
       </c>
       <c r="G22" s="5"/>
     </row>
@@ -1199,19 +1221,19 @@
         <v>14</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="D23" s="4">
+        <v>80</v>
+      </c>
+      <c r="D23" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="E23" s="4">
         <v>4</v>
       </c>
-      <c r="E23" s="3" t="s">
-        <v>46</v>
-      </c>
       <c r="F23" s="3" t="s">
-        <v>110</v>
+        <v>44</v>
       </c>
       <c r="G23" s="5"/>
     </row>
@@ -1219,8 +1241,8 @@
       <c r="A24" s="3"/>
       <c r="B24" s="4"/>
       <c r="C24" s="20"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="3"/>
+      <c r="D24" s="28"/>
+      <c r="E24" s="4"/>
       <c r="F24" s="3"/>
       <c r="G24" s="5"/>
     </row>
@@ -1229,19 +1251,19 @@
         <v>15</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="D25" s="4">
-        <v>3</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>8</v>
+        <v>16</v>
+      </c>
+      <c r="D25" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="E25" s="4">
+        <v>3</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>110</v>
+        <v>6</v>
       </c>
       <c r="G25" s="5"/>
     </row>
@@ -1250,19 +1272,19 @@
         <v>16</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C26" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="D26" s="4">
-        <v>3</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>46</v>
+        <v>16</v>
+      </c>
+      <c r="D26" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="E26" s="4">
+        <v>3</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>109</v>
+        <v>44</v>
       </c>
       <c r="G26" s="5"/>
     </row>
@@ -1270,8 +1292,8 @@
       <c r="A27" s="5"/>
       <c r="B27" s="6"/>
       <c r="C27" s="22"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="5"/>
+      <c r="D27" s="28"/>
+      <c r="E27" s="6"/>
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
       <c r="H27" s="15"/>
@@ -1281,19 +1303,19 @@
         <v>17</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C28" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="D28" s="4">
-        <v>3</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>8</v>
+        <v>30</v>
+      </c>
+      <c r="D28" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="E28" s="4">
+        <v>3</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>112</v>
+        <v>6</v>
       </c>
       <c r="G28" s="5"/>
       <c r="H28" s="15"/>
@@ -1303,19 +1325,19 @@
         <v>18</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C29" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="D29" s="4">
-        <v>3</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>46</v>
+        <v>30</v>
+      </c>
+      <c r="D29" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="E29" s="4">
+        <v>3</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>112</v>
+        <v>44</v>
       </c>
       <c r="G29" s="5"/>
       <c r="H29" s="15"/>
@@ -1324,8 +1346,8 @@
       <c r="A30" s="3"/>
       <c r="B30" s="4"/>
       <c r="C30" s="20"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="3"/>
+      <c r="D30" s="28"/>
+      <c r="E30" s="4"/>
       <c r="F30" s="3"/>
       <c r="G30" s="5"/>
     </row>
@@ -1334,19 +1356,19 @@
         <v>19</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C31" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="D31" s="4">
-        <v>3</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>8</v>
+        <v>33</v>
+      </c>
+      <c r="D31" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="E31" s="4">
+        <v>3</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>111</v>
+        <v>6</v>
       </c>
       <c r="G31" s="5"/>
     </row>
@@ -1355,19 +1377,19 @@
         <v>20</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C32" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="D32" s="4">
-        <v>3</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>46</v>
+        <v>33</v>
+      </c>
+      <c r="D32" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="E32" s="4">
+        <v>3</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>109</v>
+        <v>44</v>
       </c>
       <c r="G32" s="5"/>
     </row>
@@ -1375,8 +1397,8 @@
       <c r="A33" s="3"/>
       <c r="B33" s="9"/>
       <c r="C33" s="18"/>
-      <c r="D33" s="4"/>
-      <c r="E33" s="3"/>
+      <c r="D33" s="28"/>
+      <c r="E33" s="4"/>
       <c r="F33" s="3"/>
       <c r="G33" s="5"/>
     </row>
@@ -1384,8 +1406,8 @@
       <c r="A34" s="3"/>
       <c r="B34" s="9"/>
       <c r="C34" s="20"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="3"/>
+      <c r="D34" s="28"/>
+      <c r="E34" s="4"/>
       <c r="F34" s="3"/>
       <c r="G34" s="5"/>
     </row>
@@ -1394,18 +1416,20 @@
         <v>21</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C35" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="D35" s="4">
-        <v>3</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F35" s="3"/>
+        <v>35</v>
+      </c>
+      <c r="D35" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="E35" s="4">
+        <v>3</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="G35" s="5"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -1413,26 +1437,28 @@
         <v>22</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C36" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="D36" s="4">
-        <v>3</v>
-      </c>
-      <c r="E36" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="F36" s="3"/>
+        <v>35</v>
+      </c>
+      <c r="D36" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="E36" s="4">
+        <v>3</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="G36" s="5"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="3"/>
       <c r="B37" s="4"/>
       <c r="C37" s="20"/>
-      <c r="D37" s="4"/>
-      <c r="E37" s="3"/>
+      <c r="D37" s="28"/>
+      <c r="E37" s="4"/>
       <c r="F37" s="3"/>
       <c r="G37" s="5"/>
     </row>
@@ -1441,18 +1467,20 @@
         <v>23</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C38" s="23" t="s">
-        <v>39</v>
-      </c>
-      <c r="D38" s="4">
-        <v>3</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F38" s="3"/>
+        <v>37</v>
+      </c>
+      <c r="D38" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="E38" s="4">
+        <v>3</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="G38" s="5"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -1460,26 +1488,28 @@
         <v>24</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C39" s="23" t="s">
-        <v>39</v>
-      </c>
-      <c r="D39" s="4">
-        <v>3</v>
-      </c>
-      <c r="E39" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="F39" s="3"/>
+        <v>37</v>
+      </c>
+      <c r="D39" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="E39" s="4">
+        <v>3</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="G39" s="5"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="3"/>
       <c r="B40" s="10"/>
       <c r="C40" s="23"/>
-      <c r="D40" s="4"/>
-      <c r="E40" s="3"/>
+      <c r="D40" s="28"/>
+      <c r="E40" s="4"/>
       <c r="F40" s="3"/>
       <c r="G40" s="5"/>
     </row>
@@ -1488,18 +1518,20 @@
         <v>25</v>
       </c>
       <c r="B41" s="12" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C41" s="24" t="s">
-        <v>64</v>
-      </c>
-      <c r="D41" s="4">
-        <v>3</v>
-      </c>
-      <c r="E41" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F41" s="3"/>
+        <v>62</v>
+      </c>
+      <c r="D41" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="E41" s="4">
+        <v>3</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="G41" s="5"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -1507,26 +1539,28 @@
         <v>26</v>
       </c>
       <c r="B42" s="12" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C42" s="24" t="s">
-        <v>64</v>
-      </c>
-      <c r="D42" s="4">
-        <v>3</v>
-      </c>
-      <c r="E42" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="F42" s="3"/>
+        <v>62</v>
+      </c>
+      <c r="D42" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="E42" s="4">
+        <v>3</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="G42" s="5"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="3"/>
       <c r="B43" s="10"/>
       <c r="C43" s="23"/>
-      <c r="D43" s="4"/>
-      <c r="E43" s="3"/>
+      <c r="D43" s="28"/>
+      <c r="E43" s="4"/>
       <c r="F43" s="3"/>
       <c r="G43" s="5"/>
     </row>
@@ -1534,8 +1568,8 @@
       <c r="A44" s="3"/>
       <c r="B44" s="4"/>
       <c r="C44" s="19"/>
-      <c r="D44" s="4"/>
-      <c r="E44" s="3"/>
+      <c r="D44" s="28"/>
+      <c r="E44" s="4"/>
       <c r="F44" s="3"/>
       <c r="G44" s="5"/>
     </row>
@@ -1544,18 +1578,20 @@
         <v>27</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C45" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="D45" s="4">
-        <v>3</v>
-      </c>
-      <c r="E45" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F45" s="3"/>
+        <v>39</v>
+      </c>
+      <c r="D45" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="E45" s="4">
+        <v>3</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="G45" s="5"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
@@ -1563,18 +1599,20 @@
         <v>28</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C46" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="D46" s="4">
-        <v>3</v>
-      </c>
-      <c r="E46" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="F46" s="3"/>
+        <v>39</v>
+      </c>
+      <c r="D46" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="E46" s="4">
+        <v>3</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>47</v>
+      </c>
       <c r="G46" s="5"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
@@ -1582,26 +1620,28 @@
         <v>29</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C47" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="D47" s="4">
-        <v>3</v>
-      </c>
-      <c r="E47" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="F47" s="3"/>
+        <v>39</v>
+      </c>
+      <c r="D47" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="E47" s="4">
+        <v>3</v>
+      </c>
+      <c r="F47" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="G47" s="5"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="3"/>
       <c r="B48" s="4"/>
       <c r="C48" s="20"/>
-      <c r="D48" s="4"/>
-      <c r="E48" s="3"/>
+      <c r="D48" s="28"/>
+      <c r="E48" s="4"/>
       <c r="F48" s="3"/>
       <c r="G48" s="5"/>
     </row>
@@ -1610,18 +1650,20 @@
         <v>30</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C49" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="D49" s="4">
-        <v>3</v>
-      </c>
-      <c r="E49" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F49" s="3"/>
+        <v>41</v>
+      </c>
+      <c r="D49" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="E49" s="4">
+        <v>3</v>
+      </c>
+      <c r="F49" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="G49" s="5"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
@@ -1629,18 +1671,20 @@
         <v>31</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C50" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="D50" s="4">
-        <v>3</v>
-      </c>
-      <c r="E50" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="F50" s="3"/>
+        <v>41</v>
+      </c>
+      <c r="D50" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="E50" s="4">
+        <v>3</v>
+      </c>
+      <c r="F50" s="3" t="s">
+        <v>47</v>
+      </c>
       <c r="G50" s="5"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
@@ -1648,26 +1692,28 @@
         <v>32</v>
       </c>
       <c r="B51" s="9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C51" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="D51" s="4">
-        <v>3</v>
-      </c>
-      <c r="E51" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="F51" s="3"/>
+        <v>41</v>
+      </c>
+      <c r="D51" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="E51" s="4">
+        <v>3</v>
+      </c>
+      <c r="F51" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="G51" s="5"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="3"/>
       <c r="B52" s="4"/>
       <c r="C52" s="20"/>
-      <c r="D52" s="4"/>
-      <c r="E52" s="3"/>
+      <c r="D52" s="28"/>
+      <c r="E52" s="4"/>
       <c r="F52" s="3"/>
       <c r="G52" s="5"/>
     </row>
@@ -1676,18 +1722,20 @@
         <v>33</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C53" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="D53" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="E53" s="4">
+        <v>3</v>
+      </c>
+      <c r="F53" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D53" s="4">
-        <v>3</v>
-      </c>
-      <c r="E53" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F53" s="3"/>
       <c r="G53" s="5"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
@@ -1695,18 +1743,20 @@
         <v>34</v>
       </c>
       <c r="B54" s="9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C54" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="D54" s="4">
-        <v>3</v>
-      </c>
-      <c r="E54" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="F54" s="3"/>
+        <v>43</v>
+      </c>
+      <c r="D54" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="E54" s="4">
+        <v>3</v>
+      </c>
+      <c r="F54" s="3" t="s">
+        <v>47</v>
+      </c>
       <c r="G54" s="5"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
@@ -1714,26 +1764,28 @@
         <v>36</v>
       </c>
       <c r="B55" s="9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C55" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="D55" s="4">
-        <v>3</v>
-      </c>
-      <c r="E55" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="F55" s="3"/>
+        <v>43</v>
+      </c>
+      <c r="D55" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="E55" s="4">
+        <v>3</v>
+      </c>
+      <c r="F55" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="G55" s="5"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="3"/>
       <c r="B56" s="4"/>
       <c r="C56" s="20"/>
-      <c r="D56" s="4"/>
-      <c r="E56" s="3"/>
+      <c r="D56" s="28"/>
+      <c r="E56" s="4"/>
       <c r="F56" s="3"/>
       <c r="G56" s="5"/>
     </row>
@@ -1741,8 +1793,8 @@
       <c r="A57" s="3"/>
       <c r="B57" s="27"/>
       <c r="C57" s="27"/>
-      <c r="D57" s="4"/>
-      <c r="E57" s="3"/>
+      <c r="D57" s="28"/>
+      <c r="E57" s="4"/>
       <c r="F57" s="3"/>
       <c r="G57" s="5"/>
     </row>
@@ -1750,8 +1802,8 @@
       <c r="A58" s="3"/>
       <c r="B58" s="4"/>
       <c r="C58" s="19"/>
-      <c r="D58" s="4"/>
-      <c r="E58" s="3"/>
+      <c r="D58" s="28"/>
+      <c r="E58" s="4"/>
       <c r="F58" s="3"/>
       <c r="G58" s="5"/>
     </row>
@@ -1760,18 +1812,20 @@
         <v>37</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C59" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="D59" s="4">
-        <v>3</v>
-      </c>
-      <c r="E59" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F59" s="3"/>
+        <v>16</v>
+      </c>
+      <c r="D59" s="28" t="s">
+        <v>114</v>
+      </c>
+      <c r="E59" s="4">
+        <v>3</v>
+      </c>
+      <c r="F59" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="G59" s="5"/>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
@@ -1779,18 +1833,20 @@
         <v>38</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C60" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="D60" s="4">
-        <v>3</v>
-      </c>
-      <c r="E60" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F60" s="3"/>
+        <v>16</v>
+      </c>
+      <c r="D60" s="28" t="s">
+        <v>114</v>
+      </c>
+      <c r="E60" s="4">
+        <v>3</v>
+      </c>
+      <c r="F60" s="3" t="s">
+        <v>10</v>
+      </c>
       <c r="G60" s="5"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
@@ -1798,26 +1854,28 @@
         <v>39</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C61" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="D61" s="4">
-        <v>3</v>
-      </c>
-      <c r="E61" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F61" s="3"/>
+        <v>16</v>
+      </c>
+      <c r="D61" s="28" t="s">
+        <v>114</v>
+      </c>
+      <c r="E61" s="4">
+        <v>3</v>
+      </c>
+      <c r="F61" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="G61" s="5"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="3"/>
       <c r="B62" s="4"/>
       <c r="C62" s="18"/>
-      <c r="D62" s="4"/>
-      <c r="E62" s="3"/>
+      <c r="D62" s="28"/>
+      <c r="E62" s="4"/>
       <c r="F62" s="3"/>
       <c r="G62" s="5"/>
     </row>
@@ -1825,8 +1883,8 @@
       <c r="A63" s="3"/>
       <c r="B63" s="4"/>
       <c r="C63" s="19"/>
-      <c r="D63" s="4"/>
-      <c r="E63" s="3"/>
+      <c r="D63" s="28"/>
+      <c r="E63" s="4"/>
       <c r="F63" s="3"/>
       <c r="G63" s="5"/>
     </row>
@@ -1835,18 +1893,20 @@
         <v>40</v>
       </c>
       <c r="B64" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C64" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="D64" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="E64" s="4">
+        <v>3</v>
+      </c>
+      <c r="F64" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C64" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="D64" s="4">
-        <v>3</v>
-      </c>
-      <c r="E64" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="F64" s="3"/>
       <c r="G64" s="5"/>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
@@ -1854,18 +1914,20 @@
         <v>41</v>
       </c>
       <c r="B65" s="9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C65" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="D65" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="E65" s="4">
+        <v>3</v>
+      </c>
+      <c r="F65" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D65" s="4">
-        <v>3</v>
-      </c>
-      <c r="E65" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F65" s="3"/>
       <c r="G65" s="5"/>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
@@ -1873,26 +1935,28 @@
         <v>42</v>
       </c>
       <c r="B66" s="9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C66" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="D66" s="4">
-        <v>3</v>
-      </c>
-      <c r="E66" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="F66" s="3"/>
+        <v>49</v>
+      </c>
+      <c r="D66" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="E66" s="4">
+        <v>3</v>
+      </c>
+      <c r="F66" s="3" t="s">
+        <v>52</v>
+      </c>
       <c r="G66" s="5"/>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="3"/>
       <c r="B67" s="9"/>
       <c r="C67" s="18"/>
-      <c r="D67" s="4"/>
-      <c r="E67" s="3"/>
+      <c r="D67" s="28"/>
+      <c r="E67" s="4"/>
       <c r="F67" s="3"/>
       <c r="G67" s="5"/>
     </row>
@@ -1900,8 +1964,8 @@
       <c r="A68" s="3"/>
       <c r="B68" s="4"/>
       <c r="C68" s="20"/>
-      <c r="D68" s="4"/>
-      <c r="E68" s="3"/>
+      <c r="D68" s="28"/>
+      <c r="E68" s="4"/>
       <c r="F68" s="3"/>
       <c r="G68" s="5"/>
     </row>
@@ -1910,18 +1974,20 @@
         <v>43</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C69" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="D69" s="4">
-        <v>3</v>
-      </c>
-      <c r="E69" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="F69" s="3"/>
+        <v>18</v>
+      </c>
+      <c r="D69" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="E69" s="4">
+        <v>3</v>
+      </c>
+      <c r="F69" s="3" t="s">
+        <v>50</v>
+      </c>
       <c r="G69" s="5"/>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
@@ -1929,18 +1995,20 @@
         <v>44</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C70" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="D70" s="4">
-        <v>3</v>
-      </c>
-      <c r="E70" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F70" s="3"/>
+        <v>18</v>
+      </c>
+      <c r="D70" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="E70" s="4">
+        <v>3</v>
+      </c>
+      <c r="F70" s="3" t="s">
+        <v>51</v>
+      </c>
       <c r="G70" s="5"/>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
@@ -1948,26 +2016,28 @@
         <v>45</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C71" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="D71" s="4">
-        <v>3</v>
-      </c>
-      <c r="E71" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="F71" s="3"/>
+        <v>18</v>
+      </c>
+      <c r="D71" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="E71" s="4">
+        <v>3</v>
+      </c>
+      <c r="F71" s="3" t="s">
+        <v>52</v>
+      </c>
       <c r="G71" s="5"/>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="3"/>
       <c r="B72" s="4"/>
       <c r="C72" s="18"/>
-      <c r="D72" s="4"/>
-      <c r="E72" s="3"/>
+      <c r="D72" s="28"/>
+      <c r="E72" s="4"/>
       <c r="F72" s="3"/>
       <c r="G72" s="5"/>
     </row>
@@ -1976,18 +2046,20 @@
         <v>46</v>
       </c>
       <c r="B73" s="9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C73" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="D73" s="4">
-        <v>3</v>
-      </c>
-      <c r="E73" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="F73" s="3"/>
+        <v>54</v>
+      </c>
+      <c r="D73" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="E73" s="4">
+        <v>3</v>
+      </c>
+      <c r="F73" s="3" t="s">
+        <v>50</v>
+      </c>
       <c r="G73" s="5"/>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
@@ -1995,18 +2067,20 @@
         <v>47</v>
       </c>
       <c r="B74" s="9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C74" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="D74" s="4">
-        <v>3</v>
-      </c>
-      <c r="E74" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F74" s="3"/>
+        <v>54</v>
+      </c>
+      <c r="D74" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="E74" s="4">
+        <v>3</v>
+      </c>
+      <c r="F74" s="3" t="s">
+        <v>51</v>
+      </c>
       <c r="G74" s="5"/>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
@@ -2014,26 +2088,28 @@
         <v>48</v>
       </c>
       <c r="B75" s="9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C75" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="D75" s="4">
-        <v>3</v>
-      </c>
-      <c r="E75" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="F75" s="3"/>
+      <c r="D75" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="E75" s="4">
+        <v>3</v>
+      </c>
+      <c r="F75" s="3" t="s">
+        <v>52</v>
+      </c>
       <c r="G75" s="5"/>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="3"/>
       <c r="B76" s="4"/>
       <c r="C76" s="20"/>
-      <c r="D76" s="4"/>
-      <c r="E76" s="3"/>
+      <c r="D76" s="28"/>
+      <c r="E76" s="4"/>
       <c r="F76" s="3"/>
       <c r="G76" s="5"/>
     </row>
@@ -2041,8 +2117,8 @@
       <c r="A77" s="3"/>
       <c r="B77" s="4"/>
       <c r="C77" s="19"/>
-      <c r="D77" s="4"/>
-      <c r="E77" s="3"/>
+      <c r="D77" s="28"/>
+      <c r="E77" s="4"/>
       <c r="F77" s="3"/>
       <c r="G77" s="5"/>
     </row>
@@ -2051,18 +2127,20 @@
         <v>49</v>
       </c>
       <c r="B78" s="9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C78" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="D78" s="4">
-        <v>3</v>
-      </c>
-      <c r="E78" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F78" s="3"/>
+        <v>56</v>
+      </c>
+      <c r="D78" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="E78" s="4">
+        <v>3</v>
+      </c>
+      <c r="F78" s="3" t="s">
+        <v>12</v>
+      </c>
       <c r="G78" s="5"/>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
@@ -2070,18 +2148,20 @@
         <v>50</v>
       </c>
       <c r="B79" s="9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C79" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="D79" s="4">
-        <v>3</v>
-      </c>
-      <c r="E79" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F79" s="3"/>
+        <v>56</v>
+      </c>
+      <c r="D79" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="E79" s="4">
+        <v>3</v>
+      </c>
+      <c r="F79" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="G79" s="5"/>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
@@ -2089,18 +2169,20 @@
         <v>51</v>
       </c>
       <c r="B80" s="9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C80" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="D80" s="4">
-        <v>3</v>
-      </c>
-      <c r="E80" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F80" s="3"/>
+        <v>56</v>
+      </c>
+      <c r="D80" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="E80" s="4">
+        <v>3</v>
+      </c>
+      <c r="F80" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="G80" s="5"/>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
@@ -2108,26 +2190,28 @@
         <v>52</v>
       </c>
       <c r="B81" s="9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C81" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="D81" s="4">
-        <v>3</v>
-      </c>
-      <c r="E81" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="F81" s="3"/>
+        <v>56</v>
+      </c>
+      <c r="D81" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="E81" s="4">
+        <v>3</v>
+      </c>
+      <c r="F81" s="3" t="s">
+        <v>96</v>
+      </c>
       <c r="G81" s="5"/>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="3"/>
       <c r="B82" s="4"/>
       <c r="C82" s="20"/>
-      <c r="D82" s="4"/>
-      <c r="E82" s="3"/>
+      <c r="D82" s="28"/>
+      <c r="E82" s="4"/>
       <c r="F82" s="3"/>
       <c r="G82" s="5"/>
     </row>
@@ -2136,18 +2220,20 @@
         <v>53</v>
       </c>
       <c r="B83" s="9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C83" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="D83" s="4">
-        <v>3</v>
-      </c>
-      <c r="E83" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F83" s="3"/>
+        <v>58</v>
+      </c>
+      <c r="D83" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="E83" s="4">
+        <v>3</v>
+      </c>
+      <c r="F83" s="3" t="s">
+        <v>12</v>
+      </c>
       <c r="G83" s="5"/>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
@@ -2155,18 +2241,20 @@
         <v>54</v>
       </c>
       <c r="B84" s="9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C84" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="D84" s="4">
-        <v>3</v>
-      </c>
-      <c r="E84" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F84" s="3"/>
+        <v>58</v>
+      </c>
+      <c r="D84" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="E84" s="4">
+        <v>3</v>
+      </c>
+      <c r="F84" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="G84" s="5"/>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
@@ -2174,18 +2262,20 @@
         <v>55</v>
       </c>
       <c r="B85" s="9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C85" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="D85" s="4">
-        <v>3</v>
-      </c>
-      <c r="E85" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F85" s="3"/>
+        <v>58</v>
+      </c>
+      <c r="D85" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="E85" s="4">
+        <v>3</v>
+      </c>
+      <c r="F85" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="G85" s="5"/>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
@@ -2193,26 +2283,28 @@
         <v>56</v>
       </c>
       <c r="B86" s="9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C86" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="D86" s="4">
-        <v>3</v>
-      </c>
-      <c r="E86" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="F86" s="3"/>
+        <v>58</v>
+      </c>
+      <c r="D86" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="E86" s="4">
+        <v>3</v>
+      </c>
+      <c r="F86" s="3" t="s">
+        <v>96</v>
+      </c>
       <c r="G86" s="5"/>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="3"/>
       <c r="B87" s="4"/>
       <c r="C87" s="20"/>
-      <c r="D87" s="4"/>
-      <c r="E87" s="3"/>
+      <c r="D87" s="28"/>
+      <c r="E87" s="4"/>
       <c r="F87" s="3"/>
       <c r="G87" s="5"/>
     </row>
@@ -2221,18 +2313,20 @@
         <v>57</v>
       </c>
       <c r="B88" s="9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C88" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="D88" s="4">
-        <v>3</v>
-      </c>
-      <c r="E88" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F88" s="3"/>
+        <v>60</v>
+      </c>
+      <c r="D88" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="E88" s="4">
+        <v>3</v>
+      </c>
+      <c r="F88" s="3" t="s">
+        <v>12</v>
+      </c>
       <c r="G88" s="5"/>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
@@ -2240,18 +2334,20 @@
         <v>58</v>
       </c>
       <c r="B89" s="9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C89" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="D89" s="4">
-        <v>3</v>
-      </c>
-      <c r="E89" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F89" s="3"/>
+        <v>60</v>
+      </c>
+      <c r="D89" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="E89" s="4">
+        <v>3</v>
+      </c>
+      <c r="F89" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="G89" s="5"/>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
@@ -2259,18 +2355,20 @@
         <v>59</v>
       </c>
       <c r="B90" s="9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C90" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="D90" s="4">
-        <v>3</v>
-      </c>
-      <c r="E90" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F90" s="3"/>
+        <v>60</v>
+      </c>
+      <c r="D90" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="E90" s="4">
+        <v>3</v>
+      </c>
+      <c r="F90" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="G90" s="5"/>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
@@ -2278,26 +2376,28 @@
         <v>60</v>
       </c>
       <c r="B91" s="9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C91" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="D91" s="4">
-        <v>3</v>
-      </c>
-      <c r="E91" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="F91" s="3"/>
+        <v>60</v>
+      </c>
+      <c r="D91" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="E91" s="4">
+        <v>3</v>
+      </c>
+      <c r="F91" s="3" t="s">
+        <v>96</v>
+      </c>
       <c r="G91" s="5"/>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="3"/>
       <c r="B92" s="4"/>
       <c r="C92" s="20"/>
-      <c r="D92" s="4"/>
-      <c r="E92" s="3"/>
+      <c r="D92" s="28"/>
+      <c r="E92" s="4"/>
       <c r="F92" s="3"/>
       <c r="G92" s="5"/>
     </row>
@@ -2306,18 +2406,20 @@
         <v>61</v>
       </c>
       <c r="B93" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C93" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="D93" s="4">
-        <v>3</v>
-      </c>
-      <c r="E93" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F93" s="3"/>
+        <v>62</v>
+      </c>
+      <c r="D93" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="E93" s="4">
+        <v>3</v>
+      </c>
+      <c r="F93" s="3" t="s">
+        <v>12</v>
+      </c>
       <c r="G93" s="5"/>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
@@ -2325,18 +2427,20 @@
         <v>62</v>
       </c>
       <c r="B94" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C94" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="D94" s="4">
-        <v>3</v>
-      </c>
-      <c r="E94" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F94" s="3"/>
+        <v>62</v>
+      </c>
+      <c r="D94" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="E94" s="4">
+        <v>3</v>
+      </c>
+      <c r="F94" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="G94" s="5"/>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
@@ -2344,18 +2448,20 @@
         <v>63</v>
       </c>
       <c r="B95" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C95" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="D95" s="4">
-        <v>3</v>
-      </c>
-      <c r="E95" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F95" s="3"/>
+        <v>62</v>
+      </c>
+      <c r="D95" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="E95" s="4">
+        <v>3</v>
+      </c>
+      <c r="F95" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="G95" s="5"/>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
@@ -2363,26 +2469,28 @@
         <v>64</v>
       </c>
       <c r="B96" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C96" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="D96" s="4">
-        <v>3</v>
-      </c>
-      <c r="E96" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="F96" s="3"/>
+        <v>62</v>
+      </c>
+      <c r="D96" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="E96" s="4">
+        <v>3</v>
+      </c>
+      <c r="F96" s="3" t="s">
+        <v>96</v>
+      </c>
       <c r="G96" s="5"/>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="3"/>
       <c r="B97" s="4"/>
       <c r="C97" s="20"/>
-      <c r="D97" s="4"/>
-      <c r="E97" s="3"/>
+      <c r="D97" s="28"/>
+      <c r="E97" s="4"/>
       <c r="F97" s="3"/>
       <c r="G97" s="5"/>
     </row>
@@ -2391,18 +2499,20 @@
         <v>65</v>
       </c>
       <c r="B98" s="9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C98" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="D98" s="4">
-        <v>3</v>
-      </c>
-      <c r="E98" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F98" s="3"/>
+        <v>64</v>
+      </c>
+      <c r="D98" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="E98" s="4">
+        <v>3</v>
+      </c>
+      <c r="F98" s="3" t="s">
+        <v>12</v>
+      </c>
       <c r="G98" s="5"/>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
@@ -2410,18 +2520,20 @@
         <v>66</v>
       </c>
       <c r="B99" s="9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C99" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="D99" s="4">
-        <v>3</v>
-      </c>
-      <c r="E99" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F99" s="3"/>
+        <v>64</v>
+      </c>
+      <c r="D99" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="E99" s="4">
+        <v>3</v>
+      </c>
+      <c r="F99" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="G99" s="5"/>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
@@ -2429,18 +2541,20 @@
         <v>67</v>
       </c>
       <c r="B100" s="9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C100" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="D100" s="4">
-        <v>3</v>
-      </c>
-      <c r="E100" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F100" s="3"/>
+        <v>64</v>
+      </c>
+      <c r="D100" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="E100" s="4">
+        <v>3</v>
+      </c>
+      <c r="F100" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="G100" s="5"/>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
@@ -2448,26 +2562,28 @@
         <v>68</v>
       </c>
       <c r="B101" s="9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C101" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="D101" s="4">
-        <v>3</v>
-      </c>
-      <c r="E101" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="F101" s="3"/>
+        <v>64</v>
+      </c>
+      <c r="D101" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="E101" s="4">
+        <v>3</v>
+      </c>
+      <c r="F101" s="3" t="s">
+        <v>96</v>
+      </c>
       <c r="G101" s="5"/>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" s="3"/>
       <c r="B102" s="4"/>
       <c r="C102" s="20"/>
-      <c r="D102" s="4"/>
-      <c r="E102" s="3"/>
+      <c r="D102" s="28"/>
+      <c r="E102" s="4"/>
       <c r="F102" s="3"/>
       <c r="G102" s="5"/>
     </row>
@@ -2476,18 +2592,20 @@
         <v>69</v>
       </c>
       <c r="B103" s="9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C103" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="D103" s="4">
-        <v>3</v>
-      </c>
-      <c r="E103" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F103" s="3"/>
+        <v>66</v>
+      </c>
+      <c r="D103" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="E103" s="4">
+        <v>3</v>
+      </c>
+      <c r="F103" s="3" t="s">
+        <v>12</v>
+      </c>
       <c r="G103" s="5"/>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
@@ -2495,18 +2613,20 @@
         <v>70</v>
       </c>
       <c r="B104" s="9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C104" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="D104" s="4">
-        <v>3</v>
-      </c>
-      <c r="E104" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F104" s="3"/>
+        <v>66</v>
+      </c>
+      <c r="D104" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="E104" s="4">
+        <v>3</v>
+      </c>
+      <c r="F104" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="G104" s="5"/>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
@@ -2514,18 +2634,20 @@
         <v>71</v>
       </c>
       <c r="B105" s="9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C105" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="D105" s="4">
-        <v>3</v>
-      </c>
-      <c r="E105" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F105" s="3"/>
+        <v>66</v>
+      </c>
+      <c r="D105" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="E105" s="4">
+        <v>3</v>
+      </c>
+      <c r="F105" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="G105" s="5"/>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
@@ -2533,26 +2655,28 @@
         <v>72</v>
       </c>
       <c r="B106" s="9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C106" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="D106" s="4">
-        <v>3</v>
-      </c>
-      <c r="E106" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="F106" s="3"/>
+        <v>66</v>
+      </c>
+      <c r="D106" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="E106" s="4">
+        <v>3</v>
+      </c>
+      <c r="F106" s="3" t="s">
+        <v>96</v>
+      </c>
       <c r="G106" s="5"/>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" s="3"/>
       <c r="B107" s="4"/>
       <c r="C107" s="20"/>
-      <c r="D107" s="4"/>
-      <c r="E107" s="3"/>
+      <c r="D107" s="28"/>
+      <c r="E107" s="4"/>
       <c r="F107" s="3"/>
       <c r="G107" s="5"/>
     </row>
@@ -2560,8 +2684,8 @@
       <c r="A108" s="3"/>
       <c r="B108" s="4"/>
       <c r="C108" s="19"/>
-      <c r="D108" s="4"/>
-      <c r="E108" s="3"/>
+      <c r="D108" s="28"/>
+      <c r="E108" s="4"/>
       <c r="F108" s="3"/>
       <c r="G108" s="5"/>
     </row>
@@ -2570,18 +2694,20 @@
         <v>73</v>
       </c>
       <c r="B109" s="12" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C109" s="22" t="s">
-        <v>73</v>
-      </c>
-      <c r="D109" s="4">
-        <v>3</v>
-      </c>
-      <c r="E109" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="F109" s="5"/>
+        <v>71</v>
+      </c>
+      <c r="D109" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="E109" s="4">
+        <v>3</v>
+      </c>
+      <c r="F109" s="3" t="s">
+        <v>97</v>
+      </c>
       <c r="G109" s="5"/>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
@@ -2589,18 +2715,20 @@
         <v>74</v>
       </c>
       <c r="B110" s="12" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C110" s="22" t="s">
-        <v>73</v>
-      </c>
-      <c r="D110" s="4">
-        <v>3</v>
-      </c>
-      <c r="E110" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="F110" s="5"/>
+        <v>71</v>
+      </c>
+      <c r="D110" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="E110" s="4">
+        <v>3</v>
+      </c>
+      <c r="F110" s="3" t="s">
+        <v>98</v>
+      </c>
       <c r="G110" s="5"/>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
@@ -2608,27 +2736,29 @@
         <v>75</v>
       </c>
       <c r="B111" s="12" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C111" s="22" t="s">
-        <v>73</v>
-      </c>
-      <c r="D111" s="4">
-        <v>3</v>
-      </c>
-      <c r="E111" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="F111" s="5"/>
+        <v>71</v>
+      </c>
+      <c r="D111" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="E111" s="4">
+        <v>3</v>
+      </c>
+      <c r="F111" s="3" t="s">
+        <v>99</v>
+      </c>
       <c r="G111" s="5"/>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" s="3"/>
       <c r="B112" s="4"/>
       <c r="C112" s="20"/>
-      <c r="D112" s="4"/>
-      <c r="E112" s="3"/>
-      <c r="F112" s="5"/>
+      <c r="D112" s="28"/>
+      <c r="E112" s="4"/>
+      <c r="F112" s="3"/>
       <c r="G112" s="5"/>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
@@ -2636,18 +2766,20 @@
         <v>76</v>
       </c>
       <c r="B113" s="12" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C113" s="24" t="s">
-        <v>75</v>
-      </c>
-      <c r="D113" s="4">
-        <v>3</v>
-      </c>
-      <c r="E113" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="F113" s="5"/>
+        <v>73</v>
+      </c>
+      <c r="D113" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="E113" s="4">
+        <v>3</v>
+      </c>
+      <c r="F113" s="3" t="s">
+        <v>97</v>
+      </c>
       <c r="G113" s="5"/>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
@@ -2655,18 +2787,20 @@
         <v>77</v>
       </c>
       <c r="B114" s="12" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C114" s="24" t="s">
-        <v>75</v>
-      </c>
-      <c r="D114" s="4">
-        <v>3</v>
-      </c>
-      <c r="E114" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="F114" s="3"/>
+        <v>73</v>
+      </c>
+      <c r="D114" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="E114" s="4">
+        <v>3</v>
+      </c>
+      <c r="F114" s="3" t="s">
+        <v>98</v>
+      </c>
       <c r="G114" s="5"/>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
@@ -2674,26 +2808,28 @@
         <v>78</v>
       </c>
       <c r="B115" s="12" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C115" s="24" t="s">
-        <v>75</v>
-      </c>
-      <c r="D115" s="4">
-        <v>3</v>
-      </c>
-      <c r="E115" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="F115" s="3"/>
+        <v>73</v>
+      </c>
+      <c r="D115" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="E115" s="4">
+        <v>3</v>
+      </c>
+      <c r="F115" s="3" t="s">
+        <v>99</v>
+      </c>
       <c r="G115" s="5"/>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" s="3"/>
       <c r="B116" s="4"/>
       <c r="C116" s="20"/>
-      <c r="D116" s="4"/>
-      <c r="E116" s="3"/>
+      <c r="D116" s="28"/>
+      <c r="E116" s="4"/>
       <c r="F116" s="3"/>
       <c r="G116" s="5"/>
     </row>
@@ -2702,18 +2838,20 @@
         <v>79</v>
       </c>
       <c r="B117" s="12" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C117" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="D117" s="4">
-        <v>3</v>
-      </c>
-      <c r="E117" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="F117" s="3"/>
+        <v>75</v>
+      </c>
+      <c r="D117" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="E117" s="4">
+        <v>3</v>
+      </c>
+      <c r="F117" s="3" t="s">
+        <v>97</v>
+      </c>
       <c r="G117" s="5"/>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
@@ -2721,18 +2859,20 @@
         <v>80</v>
       </c>
       <c r="B118" s="12" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C118" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="D118" s="4">
-        <v>3</v>
-      </c>
-      <c r="E118" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="F118" s="3"/>
+        <v>75</v>
+      </c>
+      <c r="D118" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="E118" s="4">
+        <v>3</v>
+      </c>
+      <c r="F118" s="3" t="s">
+        <v>98</v>
+      </c>
       <c r="G118" s="5"/>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
@@ -2740,26 +2880,28 @@
         <v>81</v>
       </c>
       <c r="B119" s="12" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C119" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="D119" s="4">
-        <v>3</v>
-      </c>
-      <c r="E119" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="F119" s="3"/>
+        <v>75</v>
+      </c>
+      <c r="D119" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="E119" s="4">
+        <v>3</v>
+      </c>
+      <c r="F119" s="3" t="s">
+        <v>99</v>
+      </c>
       <c r="G119" s="5"/>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" s="3"/>
       <c r="B120" s="4"/>
       <c r="C120" s="20"/>
-      <c r="D120" s="4"/>
-      <c r="E120" s="3"/>
+      <c r="D120" s="28"/>
+      <c r="E120" s="4"/>
       <c r="F120" s="3"/>
       <c r="G120" s="5"/>
     </row>
@@ -2768,18 +2910,20 @@
         <v>82</v>
       </c>
       <c r="B121" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C121" s="25" t="s">
-        <v>79</v>
-      </c>
-      <c r="D121" s="4">
-        <v>3</v>
-      </c>
-      <c r="E121" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F121" s="3"/>
+        <v>77</v>
+      </c>
+      <c r="D121" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="E121" s="4">
+        <v>3</v>
+      </c>
+      <c r="F121" s="3" t="s">
+        <v>12</v>
+      </c>
       <c r="G121" s="5"/>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
@@ -2787,18 +2931,20 @@
         <v>83</v>
       </c>
       <c r="B122" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C122" s="25" t="s">
-        <v>79</v>
-      </c>
-      <c r="D122" s="4">
-        <v>3</v>
-      </c>
-      <c r="E122" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F122" s="3"/>
+        <v>77</v>
+      </c>
+      <c r="D122" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="E122" s="4">
+        <v>3</v>
+      </c>
+      <c r="F122" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="G122" s="5"/>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.25">
@@ -2806,18 +2952,20 @@
         <v>84</v>
       </c>
       <c r="B123" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C123" s="25" t="s">
-        <v>79</v>
-      </c>
-      <c r="D123" s="4">
-        <v>3</v>
-      </c>
-      <c r="E123" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F123" s="3"/>
+        <v>77</v>
+      </c>
+      <c r="D123" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="E123" s="4">
+        <v>3</v>
+      </c>
+      <c r="F123" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="G123" s="5"/>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.25">
@@ -2825,26 +2973,28 @@
         <v>85</v>
       </c>
       <c r="B124" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C124" s="25" t="s">
-        <v>79</v>
-      </c>
-      <c r="D124" s="4">
-        <v>3</v>
-      </c>
-      <c r="E124" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="F124" s="3"/>
+        <v>77</v>
+      </c>
+      <c r="D124" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="E124" s="4">
+        <v>3</v>
+      </c>
+      <c r="F124" s="3" t="s">
+        <v>96</v>
+      </c>
       <c r="G124" s="5"/>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" s="3"/>
       <c r="B125" s="4"/>
       <c r="C125" s="25"/>
-      <c r="D125" s="4"/>
-      <c r="E125" s="3"/>
+      <c r="D125" s="28"/>
+      <c r="E125" s="4"/>
       <c r="F125" s="3"/>
       <c r="G125" s="5"/>
     </row>
@@ -2852,8 +3002,8 @@
       <c r="A126" s="3"/>
       <c r="B126" s="27"/>
       <c r="C126" s="27"/>
-      <c r="D126" s="4"/>
-      <c r="E126" s="3"/>
+      <c r="D126" s="28"/>
+      <c r="E126" s="4"/>
       <c r="F126" s="3"/>
       <c r="G126" s="5"/>
     </row>
@@ -2861,8 +3011,8 @@
       <c r="A127" s="3"/>
       <c r="B127" s="1"/>
       <c r="C127" s="16"/>
-      <c r="D127" s="4"/>
-      <c r="E127" s="3"/>
+      <c r="D127" s="28"/>
+      <c r="E127" s="4"/>
       <c r="F127" s="3"/>
       <c r="G127" s="5"/>
     </row>
@@ -2871,18 +3021,18 @@
         <v>1</v>
       </c>
       <c r="B128" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C128" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="D128" s="28"/>
+      <c r="E128" s="4">
+        <v>3</v>
+      </c>
+      <c r="F128" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="C128" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="D128" s="4">
-        <v>3</v>
-      </c>
-      <c r="E128" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="F128" s="3"/>
       <c r="G128" s="5"/>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.25">
@@ -2890,18 +3040,18 @@
         <v>2</v>
       </c>
       <c r="B129" s="9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C129" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="D129" s="28"/>
+      <c r="E129" s="4">
+        <v>3</v>
+      </c>
+      <c r="F129" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="D129" s="4">
-        <v>3</v>
-      </c>
-      <c r="E129" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="F129" s="3"/>
       <c r="G129" s="5"/>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.25">
@@ -2909,18 +3059,18 @@
         <v>3</v>
       </c>
       <c r="B130" s="9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C130" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="D130" s="4">
-        <v>3</v>
-      </c>
-      <c r="E130" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="F130" s="3"/>
+        <v>66</v>
+      </c>
+      <c r="D130" s="28"/>
+      <c r="E130" s="4">
+        <v>3</v>
+      </c>
+      <c r="F130" s="8" t="s">
+        <v>69</v>
+      </c>
       <c r="G130" s="5"/>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.25">
@@ -2928,27 +3078,27 @@
         <v>4</v>
       </c>
       <c r="B131" s="9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C131" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="D131" s="4">
-        <v>3</v>
-      </c>
-      <c r="E131" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="F131" s="3"/>
+        <v>66</v>
+      </c>
+      <c r="D131" s="28"/>
+      <c r="E131" s="4">
+        <v>3</v>
+      </c>
+      <c r="F131" s="7" t="s">
+        <v>17</v>
+      </c>
       <c r="G131" s="5"/>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132" s="3"/>
       <c r="B132" s="9"/>
       <c r="C132" s="18"/>
-      <c r="D132" s="4"/>
-      <c r="E132" s="7"/>
-      <c r="F132" s="3"/>
+      <c r="D132" s="28"/>
+      <c r="E132" s="4"/>
+      <c r="F132" s="7"/>
       <c r="G132" s="5"/>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.25">
@@ -2956,18 +3106,18 @@
         <v>5</v>
       </c>
       <c r="B133" s="9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C133" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="D133" s="4">
-        <v>3</v>
-      </c>
-      <c r="E133" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="F133" s="3"/>
+        <v>54</v>
+      </c>
+      <c r="D133" s="28"/>
+      <c r="E133" s="4">
+        <v>3</v>
+      </c>
+      <c r="F133" s="8" t="s">
+        <v>87</v>
+      </c>
       <c r="G133" s="5"/>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.25">
@@ -2975,18 +3125,18 @@
         <v>6</v>
       </c>
       <c r="B134" s="9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C134" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="D134" s="4">
-        <v>3</v>
-      </c>
-      <c r="E134" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="F134" s="3"/>
+        <v>54</v>
+      </c>
+      <c r="D134" s="28"/>
+      <c r="E134" s="4">
+        <v>3</v>
+      </c>
+      <c r="F134" s="8" t="s">
+        <v>88</v>
+      </c>
       <c r="G134" s="5"/>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.25">
@@ -2994,18 +3144,18 @@
         <v>7</v>
       </c>
       <c r="B135" s="9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C135" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="D135" s="4">
-        <v>3</v>
-      </c>
-      <c r="E135" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="F135" s="3"/>
+        <v>54</v>
+      </c>
+      <c r="D135" s="28"/>
+      <c r="E135" s="4">
+        <v>3</v>
+      </c>
+      <c r="F135" s="8" t="s">
+        <v>89</v>
+      </c>
       <c r="G135" s="5"/>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.25">
@@ -3013,18 +3163,18 @@
         <v>8</v>
       </c>
       <c r="B136" s="9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C136" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="D136" s="4">
-        <v>3</v>
-      </c>
-      <c r="E136" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="F136" s="11"/>
+        <v>54</v>
+      </c>
+      <c r="D136" s="28"/>
+      <c r="E136" s="4">
+        <v>3</v>
+      </c>
+      <c r="F136" s="11" t="s">
+        <v>90</v>
+      </c>
       <c r="G136" s="5"/>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.25">
@@ -3032,18 +3182,18 @@
         <v>9</v>
       </c>
       <c r="B137" s="9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C137" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="D137" s="4">
+        <v>54</v>
+      </c>
+      <c r="D137" s="28"/>
+      <c r="E137" s="4">
         <v>4</v>
       </c>
-      <c r="E137" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="F137" s="11"/>
+      <c r="F137" s="8" t="s">
+        <v>93</v>
+      </c>
       <c r="G137" s="5"/>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.25">
@@ -3051,18 +3201,18 @@
         <v>10</v>
       </c>
       <c r="B138" s="9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C138" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="D138" s="4">
-        <v>3</v>
-      </c>
-      <c r="E138" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="F138" s="3"/>
+        <v>54</v>
+      </c>
+      <c r="D138" s="28"/>
+      <c r="E138" s="4">
+        <v>3</v>
+      </c>
+      <c r="F138" s="8" t="s">
+        <v>102</v>
+      </c>
       <c r="G138" s="5"/>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.25">
@@ -3070,18 +3220,18 @@
         <v>11</v>
       </c>
       <c r="B139" s="9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C139" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="D139" s="4">
-        <v>3</v>
-      </c>
-      <c r="E139" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="F139" s="3"/>
+        <v>54</v>
+      </c>
+      <c r="D139" s="28"/>
+      <c r="E139" s="4">
+        <v>3</v>
+      </c>
+      <c r="F139" s="7" t="s">
+        <v>91</v>
+      </c>
       <c r="G139" s="5"/>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.25">
@@ -3089,18 +3239,18 @@
         <v>12</v>
       </c>
       <c r="B140" s="9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C140" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="D140" s="4">
-        <v>3</v>
-      </c>
-      <c r="E140" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="F140" s="3"/>
+        <v>54</v>
+      </c>
+      <c r="D140" s="28"/>
+      <c r="E140" s="4">
+        <v>3</v>
+      </c>
+      <c r="F140" s="8" t="s">
+        <v>103</v>
+      </c>
       <c r="G140" s="5"/>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.25">
@@ -3108,18 +3258,18 @@
         <v>13</v>
       </c>
       <c r="B141" s="9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C141" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="D141" s="4">
-        <v>3</v>
-      </c>
-      <c r="E141" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="F141" s="3"/>
+        <v>54</v>
+      </c>
+      <c r="D141" s="28"/>
+      <c r="E141" s="4">
+        <v>3</v>
+      </c>
+      <c r="F141" s="8" t="s">
+        <v>106</v>
+      </c>
       <c r="G141" s="5"/>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.25">
@@ -3127,18 +3277,18 @@
         <v>14</v>
       </c>
       <c r="B142" s="9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C142" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="D142" s="4">
-        <v>3</v>
-      </c>
-      <c r="E142" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="F142" s="3"/>
+        <v>54</v>
+      </c>
+      <c r="D142" s="28"/>
+      <c r="E142" s="4">
+        <v>3</v>
+      </c>
+      <c r="F142" s="8" t="s">
+        <v>92</v>
+      </c>
       <c r="G142" s="5"/>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.25">
@@ -3146,18 +3296,18 @@
         <v>15</v>
       </c>
       <c r="B143" s="9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C143" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="D143" s="4">
-        <v>3</v>
-      </c>
-      <c r="E143" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="F143" s="3"/>
+        <v>54</v>
+      </c>
+      <c r="D143" s="28"/>
+      <c r="E143" s="4">
+        <v>3</v>
+      </c>
+      <c r="F143" s="8" t="s">
+        <v>104</v>
+      </c>
       <c r="G143" s="5"/>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.25">
@@ -3165,18 +3315,18 @@
         <v>16</v>
       </c>
       <c r="B144" s="9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C144" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="D144" s="4">
+        <v>54</v>
+      </c>
+      <c r="D144" s="28"/>
+      <c r="E144" s="4">
         <v>4</v>
       </c>
-      <c r="E144" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="F144" s="3"/>
+      <c r="F144" s="8" t="s">
+        <v>104</v>
+      </c>
       <c r="G144" s="5"/>
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.25">
@@ -3184,26 +3334,26 @@
         <v>17</v>
       </c>
       <c r="B145" s="9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C145" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="D145" s="4">
-        <v>3</v>
-      </c>
-      <c r="E145" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="F145" s="3"/>
+        <v>54</v>
+      </c>
+      <c r="D145" s="28"/>
+      <c r="E145" s="4">
+        <v>3</v>
+      </c>
+      <c r="F145" s="8" t="s">
+        <v>105</v>
+      </c>
       <c r="G145" s="5"/>
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A146" s="3"/>
       <c r="B146" s="1"/>
       <c r="C146" s="16"/>
-      <c r="D146" s="4"/>
-      <c r="E146" s="3"/>
+      <c r="D146" s="28"/>
+      <c r="E146" s="4"/>
       <c r="F146" s="3"/>
       <c r="G146" s="5"/>
     </row>
@@ -3212,18 +3362,18 @@
         <v>18</v>
       </c>
       <c r="B147" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C147" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="D147" s="4">
-        <v>3</v>
-      </c>
-      <c r="E147" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="F147" s="3"/>
+        <v>16</v>
+      </c>
+      <c r="D147" s="28"/>
+      <c r="E147" s="4">
+        <v>3</v>
+      </c>
+      <c r="F147" s="8" t="s">
+        <v>82</v>
+      </c>
       <c r="G147" s="5"/>
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.25">
@@ -3231,18 +3381,18 @@
         <v>19</v>
       </c>
       <c r="B148" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C148" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="D148" s="4">
-        <v>3</v>
-      </c>
-      <c r="E148" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="F148" s="3"/>
+        <v>16</v>
+      </c>
+      <c r="D148" s="28"/>
+      <c r="E148" s="4">
+        <v>3</v>
+      </c>
+      <c r="F148" s="8" t="s">
+        <v>81</v>
+      </c>
       <c r="G148" s="5"/>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.25">
@@ -3250,18 +3400,18 @@
         <v>20</v>
       </c>
       <c r="B149" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C149" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="D149" s="4">
-        <v>3</v>
-      </c>
-      <c r="E149" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="F149" s="3"/>
+        <v>16</v>
+      </c>
+      <c r="D149" s="28"/>
+      <c r="E149" s="4">
+        <v>3</v>
+      </c>
+      <c r="F149" s="8" t="s">
+        <v>84</v>
+      </c>
       <c r="G149" s="5"/>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.25">
@@ -3269,18 +3419,18 @@
         <v>21</v>
       </c>
       <c r="B150" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C150" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="D150" s="4">
-        <v>3</v>
-      </c>
-      <c r="E150" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="F150" s="3"/>
+        <v>16</v>
+      </c>
+      <c r="D150" s="28"/>
+      <c r="E150" s="4">
+        <v>3</v>
+      </c>
+      <c r="F150" s="8" t="s">
+        <v>83</v>
+      </c>
       <c r="G150" s="5"/>
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.25">
@@ -3288,18 +3438,18 @@
         <v>22</v>
       </c>
       <c r="B151" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C151" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="D151" s="4">
-        <v>3</v>
-      </c>
-      <c r="E151" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="F151" s="3"/>
+        <v>16</v>
+      </c>
+      <c r="D151" s="28"/>
+      <c r="E151" s="4">
+        <v>3</v>
+      </c>
+      <c r="F151" s="8" t="s">
+        <v>85</v>
+      </c>
       <c r="G151" s="5"/>
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.25">
@@ -3307,26 +3457,26 @@
         <v>23</v>
       </c>
       <c r="B152" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C152" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="D152" s="4">
-        <v>3</v>
-      </c>
-      <c r="E152" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="F152" s="3"/>
+        <v>16</v>
+      </c>
+      <c r="D152" s="28"/>
+      <c r="E152" s="4">
+        <v>3</v>
+      </c>
+      <c r="F152" s="8" t="s">
+        <v>86</v>
+      </c>
       <c r="G152" s="5"/>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A153" s="3"/>
       <c r="B153" s="4"/>
       <c r="C153" s="20"/>
-      <c r="D153" s="4"/>
-      <c r="E153" s="3"/>
+      <c r="D153" s="28"/>
+      <c r="E153" s="4"/>
       <c r="F153" s="3"/>
       <c r="G153" s="5"/>
     </row>
@@ -3335,18 +3485,18 @@
         <v>24</v>
       </c>
       <c r="B154" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C154" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="D154" s="4">
-        <v>3</v>
-      </c>
-      <c r="E154" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="F154" s="3"/>
+        <v>18</v>
+      </c>
+      <c r="D154" s="28"/>
+      <c r="E154" s="4">
+        <v>3</v>
+      </c>
+      <c r="F154" s="11" t="s">
+        <v>67</v>
+      </c>
       <c r="G154" s="5"/>
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.25">
@@ -3354,18 +3504,18 @@
         <v>25</v>
       </c>
       <c r="B155" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C155" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="D155" s="4">
-        <v>3</v>
-      </c>
-      <c r="E155" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="F155" s="3"/>
+        <v>18</v>
+      </c>
+      <c r="D155" s="28"/>
+      <c r="E155" s="4">
+        <v>3</v>
+      </c>
+      <c r="F155" s="11" t="s">
+        <v>68</v>
+      </c>
       <c r="G155" s="5"/>
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.25">
@@ -3373,18 +3523,18 @@
         <v>26</v>
       </c>
       <c r="B156" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C156" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="D156" s="4">
-        <v>3</v>
-      </c>
-      <c r="E156" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="F156" s="3"/>
+        <v>18</v>
+      </c>
+      <c r="D156" s="28"/>
+      <c r="E156" s="4">
+        <v>3</v>
+      </c>
+      <c r="F156" s="11" t="s">
+        <v>69</v>
+      </c>
       <c r="G156" s="5"/>
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.25">
@@ -3392,18 +3542,18 @@
         <v>27</v>
       </c>
       <c r="B157" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C157" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="D157" s="4">
-        <v>3</v>
-      </c>
-      <c r="E157" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="F157" s="3"/>
+        <v>18</v>
+      </c>
+      <c r="D157" s="28"/>
+      <c r="E157" s="4">
+        <v>3</v>
+      </c>
+      <c r="F157" s="8" t="s">
+        <v>94</v>
+      </c>
       <c r="G157" s="5"/>
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.25">
@@ -3411,18 +3561,18 @@
         <v>28</v>
       </c>
       <c r="B158" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C158" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="D158" s="4">
-        <v>3</v>
-      </c>
-      <c r="E158" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="F158" s="3"/>
+        <v>18</v>
+      </c>
+      <c r="D158" s="28"/>
+      <c r="E158" s="4">
+        <v>3</v>
+      </c>
+      <c r="F158" s="8" t="s">
+        <v>95</v>
+      </c>
       <c r="G158" s="5"/>
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.25">
@@ -3430,18 +3580,20 @@
         <v>29</v>
       </c>
       <c r="B159" s="4" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="C159" s="18" t="s">
-        <v>116</v>
-      </c>
-      <c r="D159" s="4">
-        <v>4</v>
-      </c>
-      <c r="E159" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="F159" s="3"/>
+        <v>110</v>
+      </c>
+      <c r="D159" s="28" t="s">
+        <v>114</v>
+      </c>
+      <c r="E159" s="4">
+        <v>2</v>
+      </c>
+      <c r="F159" s="8" t="s">
+        <v>95</v>
+      </c>
       <c r="G159" s="5"/>
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.25">
@@ -3449,18 +3601,20 @@
         <v>30</v>
       </c>
       <c r="B160" s="4" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="C160" s="18" t="s">
-        <v>117</v>
-      </c>
-      <c r="D160" s="4">
-        <v>5</v>
-      </c>
-      <c r="E160" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="F160" s="3"/>
+        <v>111</v>
+      </c>
+      <c r="D160" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="E160" s="4">
+        <v>4</v>
+      </c>
+      <c r="F160" s="8" t="s">
+        <v>95</v>
+      </c>
       <c r="G160" s="5"/>
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.25">
@@ -3468,18 +3622,20 @@
         <v>31</v>
       </c>
       <c r="B161" s="4" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="C161" s="18" t="s">
-        <v>118</v>
-      </c>
-      <c r="D161" s="4">
+        <v>112</v>
+      </c>
+      <c r="D161" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="E161" s="4">
         <v>6</v>
       </c>
-      <c r="E161" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="F161" s="3"/>
+      <c r="F161" s="8" t="s">
+        <v>95</v>
+      </c>
       <c r="G161" s="5"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added: YEAR LEVEL column: YEARLEVEL w/ Department
</commit_message>
<xml_diff>
--- a/static/files/subject_data.xlsx
+++ b/static/files/subject_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jenze\Desktop\PROF LOADING CAPSTONE PROJECT\ClassScheduler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CE057C6-192D-4C62-8093-D380F2AABCAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7252A988-409C-4835-9030-E0BD99764322}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21990" windowHeight="13395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,9 +30,6 @@
     <t>COURSE CODE</t>
   </si>
   <si>
-    <t>DESCRIPTION</t>
-  </si>
-  <si>
     <t>COURSE &amp; SEC.</t>
   </si>
   <si>
@@ -382,6 +379,9 @@
   </si>
   <si>
     <t>TESTING ONLY 3</t>
+  </si>
+  <si>
+    <t>COURSE NAME</t>
   </si>
 </sst>
 </file>
@@ -834,8 +834,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A141" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="G163" sqref="G163"/>
+    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -852,25 +852,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
-      </c>
       <c r="G1" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -896,16 +896,16 @@
         <v>1</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D4" s="4">
         <v>6</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="5"/>
@@ -915,16 +915,16 @@
         <v>2</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D5" s="4">
         <v>6</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="5"/>
@@ -934,16 +934,16 @@
         <v>3</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D6" s="4">
         <v>6</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="5"/>
@@ -971,16 +971,16 @@
         <v>4</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D9" s="4">
         <v>6</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="5"/>
@@ -990,16 +990,16 @@
         <v>5</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D10" s="4">
         <v>6</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="5"/>
@@ -1009,16 +1009,16 @@
         <v>6</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D11" s="4">
         <v>6</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="5"/>
@@ -1037,16 +1037,16 @@
         <v>7</v>
       </c>
       <c r="B13" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="18" t="s">
-        <v>26</v>
-      </c>
       <c r="D13" s="4">
         <v>3</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F13" s="3"/>
       <c r="G13" s="5"/>
@@ -1056,16 +1056,16 @@
         <v>8</v>
       </c>
       <c r="B14" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="18" t="s">
-        <v>26</v>
-      </c>
       <c r="D14" s="4">
         <v>3</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F14" s="3"/>
       <c r="G14" s="5"/>
@@ -1075,16 +1075,16 @@
         <v>9</v>
       </c>
       <c r="B15" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="18" t="s">
-        <v>26</v>
-      </c>
       <c r="D15" s="4">
         <v>3</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F15" s="3"/>
       <c r="G15" s="5"/>
@@ -1103,16 +1103,16 @@
         <v>10</v>
       </c>
       <c r="B17" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="C17" s="21" t="s">
-        <v>28</v>
-      </c>
       <c r="D17" s="4">
         <v>3</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F17" s="4"/>
       <c r="G17" s="6"/>
@@ -1122,16 +1122,16 @@
         <v>11</v>
       </c>
       <c r="B18" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="21" t="s">
-        <v>28</v>
-      </c>
       <c r="D18" s="4">
         <v>3</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F18" s="3"/>
       <c r="G18" s="5"/>
@@ -1141,16 +1141,16 @@
         <v>12</v>
       </c>
       <c r="B19" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="C19" s="21" t="s">
-        <v>28</v>
-      </c>
       <c r="D19" s="4">
         <v>3</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F19" s="3"/>
       <c r="G19" s="5"/>
@@ -1178,19 +1178,19 @@
         <v>13</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C22" s="18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D22" s="4">
         <v>4</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G22" s="5"/>
     </row>
@@ -1199,19 +1199,19 @@
         <v>14</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D23" s="4">
         <v>4</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G23" s="5"/>
     </row>
@@ -1229,19 +1229,19 @@
         <v>15</v>
       </c>
       <c r="B25" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C25" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="C25" s="18" t="s">
-        <v>18</v>
-      </c>
       <c r="D25" s="4">
         <v>3</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G25" s="5"/>
     </row>
@@ -1250,19 +1250,19 @@
         <v>16</v>
       </c>
       <c r="B26" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C26" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="C26" s="18" t="s">
-        <v>18</v>
-      </c>
       <c r="D26" s="4">
         <v>3</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G26" s="5"/>
     </row>
@@ -1281,19 +1281,19 @@
         <v>17</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C28" s="18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D28" s="4">
         <v>3</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G28" s="5"/>
       <c r="H28" s="15"/>
@@ -1303,19 +1303,19 @@
         <v>18</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C29" s="18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D29" s="4">
         <v>3</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G29" s="5"/>
       <c r="H29" s="15"/>
@@ -1334,19 +1334,19 @@
         <v>19</v>
       </c>
       <c r="B31" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C31" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="C31" s="18" t="s">
-        <v>35</v>
-      </c>
       <c r="D31" s="4">
         <v>3</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G31" s="5"/>
     </row>
@@ -1355,19 +1355,19 @@
         <v>20</v>
       </c>
       <c r="B32" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C32" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="C32" s="18" t="s">
-        <v>35</v>
-      </c>
       <c r="D32" s="4">
         <v>3</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G32" s="5"/>
     </row>
@@ -1394,16 +1394,16 @@
         <v>21</v>
       </c>
       <c r="B35" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C35" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="C35" s="18" t="s">
-        <v>37</v>
-      </c>
       <c r="D35" s="4">
         <v>3</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F35" s="3"/>
       <c r="G35" s="5"/>
@@ -1413,16 +1413,16 @@
         <v>22</v>
       </c>
       <c r="B36" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C36" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="C36" s="18" t="s">
-        <v>37</v>
-      </c>
       <c r="D36" s="4">
         <v>3</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F36" s="3"/>
       <c r="G36" s="5"/>
@@ -1441,16 +1441,16 @@
         <v>23</v>
       </c>
       <c r="B38" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C38" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="C38" s="23" t="s">
-        <v>39</v>
-      </c>
       <c r="D38" s="4">
         <v>3</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F38" s="3"/>
       <c r="G38" s="5"/>
@@ -1460,16 +1460,16 @@
         <v>24</v>
       </c>
       <c r="B39" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C39" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="C39" s="23" t="s">
-        <v>39</v>
-      </c>
       <c r="D39" s="4">
         <v>3</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F39" s="3"/>
       <c r="G39" s="5"/>
@@ -1488,16 +1488,16 @@
         <v>25</v>
       </c>
       <c r="B41" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C41" s="24" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D41" s="4">
         <v>3</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F41" s="3"/>
       <c r="G41" s="5"/>
@@ -1507,16 +1507,16 @@
         <v>26</v>
       </c>
       <c r="B42" s="12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C42" s="24" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D42" s="4">
         <v>3</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F42" s="3"/>
       <c r="G42" s="5"/>
@@ -1544,16 +1544,16 @@
         <v>27</v>
       </c>
       <c r="B45" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C45" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="C45" s="18" t="s">
-        <v>41</v>
-      </c>
       <c r="D45" s="4">
         <v>3</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F45" s="3"/>
       <c r="G45" s="5"/>
@@ -1563,16 +1563,16 @@
         <v>28</v>
       </c>
       <c r="B46" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C46" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="C46" s="18" t="s">
-        <v>41</v>
-      </c>
       <c r="D46" s="4">
         <v>3</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F46" s="3"/>
       <c r="G46" s="5"/>
@@ -1582,16 +1582,16 @@
         <v>29</v>
       </c>
       <c r="B47" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C47" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="C47" s="18" t="s">
-        <v>41</v>
-      </c>
       <c r="D47" s="4">
         <v>3</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F47" s="3"/>
       <c r="G47" s="5"/>
@@ -1610,16 +1610,16 @@
         <v>30</v>
       </c>
       <c r="B49" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C49" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="C49" s="18" t="s">
-        <v>43</v>
-      </c>
       <c r="D49" s="4">
         <v>3</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F49" s="3"/>
       <c r="G49" s="5"/>
@@ -1629,16 +1629,16 @@
         <v>31</v>
       </c>
       <c r="B50" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C50" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="C50" s="18" t="s">
-        <v>43</v>
-      </c>
       <c r="D50" s="4">
         <v>3</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F50" s="3"/>
       <c r="G50" s="5"/>
@@ -1648,16 +1648,16 @@
         <v>32</v>
       </c>
       <c r="B51" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C51" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="C51" s="18" t="s">
-        <v>43</v>
-      </c>
       <c r="D51" s="4">
         <v>3</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F51" s="3"/>
       <c r="G51" s="5"/>
@@ -1676,16 +1676,16 @@
         <v>33</v>
       </c>
       <c r="B53" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C53" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="C53" s="18" t="s">
-        <v>45</v>
-      </c>
       <c r="D53" s="4">
         <v>3</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F53" s="3"/>
       <c r="G53" s="5"/>
@@ -1695,16 +1695,16 @@
         <v>34</v>
       </c>
       <c r="B54" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C54" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="C54" s="18" t="s">
-        <v>45</v>
-      </c>
       <c r="D54" s="4">
         <v>3</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F54" s="3"/>
       <c r="G54" s="5"/>
@@ -1714,16 +1714,16 @@
         <v>36</v>
       </c>
       <c r="B55" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C55" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="C55" s="18" t="s">
-        <v>45</v>
-      </c>
       <c r="D55" s="4">
         <v>3</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F55" s="3"/>
       <c r="G55" s="5"/>
@@ -1760,16 +1760,16 @@
         <v>37</v>
       </c>
       <c r="B59" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C59" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="C59" s="18" t="s">
-        <v>18</v>
-      </c>
       <c r="D59" s="4">
         <v>3</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F59" s="3"/>
       <c r="G59" s="5"/>
@@ -1779,16 +1779,16 @@
         <v>38</v>
       </c>
       <c r="B60" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C60" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="C60" s="18" t="s">
-        <v>18</v>
-      </c>
       <c r="D60" s="4">
         <v>3</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F60" s="3"/>
       <c r="G60" s="5"/>
@@ -1798,16 +1798,16 @@
         <v>39</v>
       </c>
       <c r="B61" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C61" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="C61" s="18" t="s">
-        <v>18</v>
-      </c>
       <c r="D61" s="4">
         <v>3</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F61" s="3"/>
       <c r="G61" s="5"/>
@@ -1835,16 +1835,16 @@
         <v>40</v>
       </c>
       <c r="B64" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C64" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="C64" s="18" t="s">
+      <c r="D64" s="4">
+        <v>3</v>
+      </c>
+      <c r="E64" s="3" t="s">
         <v>51</v>
-      </c>
-      <c r="D64" s="4">
-        <v>3</v>
-      </c>
-      <c r="E64" s="3" t="s">
-        <v>52</v>
       </c>
       <c r="F64" s="3"/>
       <c r="G64" s="5"/>
@@ -1854,16 +1854,16 @@
         <v>41</v>
       </c>
       <c r="B65" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C65" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="C65" s="18" t="s">
-        <v>51</v>
-      </c>
       <c r="D65" s="4">
         <v>3</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F65" s="3"/>
       <c r="G65" s="5"/>
@@ -1873,16 +1873,16 @@
         <v>42</v>
       </c>
       <c r="B66" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C66" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="C66" s="18" t="s">
-        <v>51</v>
-      </c>
       <c r="D66" s="4">
         <v>3</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F66" s="3"/>
       <c r="G66" s="5"/>
@@ -1910,16 +1910,16 @@
         <v>43</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C69" s="18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D69" s="4">
         <v>3</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F69" s="3"/>
       <c r="G69" s="5"/>
@@ -1929,16 +1929,16 @@
         <v>44</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C70" s="18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D70" s="4">
         <v>3</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F70" s="3"/>
       <c r="G70" s="5"/>
@@ -1948,16 +1948,16 @@
         <v>45</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C71" s="18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D71" s="4">
         <v>3</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F71" s="3"/>
       <c r="G71" s="5"/>
@@ -1976,16 +1976,16 @@
         <v>46</v>
       </c>
       <c r="B73" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C73" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="C73" s="18" t="s">
-        <v>56</v>
-      </c>
       <c r="D73" s="4">
         <v>3</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F73" s="3"/>
       <c r="G73" s="5"/>
@@ -1995,16 +1995,16 @@
         <v>47</v>
       </c>
       <c r="B74" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C74" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="C74" s="18" t="s">
-        <v>56</v>
-      </c>
       <c r="D74" s="4">
         <v>3</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F74" s="3"/>
       <c r="G74" s="5"/>
@@ -2014,16 +2014,16 @@
         <v>48</v>
       </c>
       <c r="B75" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C75" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="C75" s="18" t="s">
-        <v>56</v>
-      </c>
       <c r="D75" s="4">
         <v>3</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F75" s="3"/>
       <c r="G75" s="5"/>
@@ -2051,16 +2051,16 @@
         <v>49</v>
       </c>
       <c r="B78" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C78" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="C78" s="18" t="s">
-        <v>58</v>
-      </c>
       <c r="D78" s="4">
         <v>3</v>
       </c>
       <c r="E78" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F78" s="3"/>
       <c r="G78" s="5"/>
@@ -2070,16 +2070,16 @@
         <v>50</v>
       </c>
       <c r="B79" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C79" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="C79" s="18" t="s">
-        <v>58</v>
-      </c>
       <c r="D79" s="4">
         <v>3</v>
       </c>
       <c r="E79" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F79" s="3"/>
       <c r="G79" s="5"/>
@@ -2089,16 +2089,16 @@
         <v>51</v>
       </c>
       <c r="B80" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C80" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="C80" s="18" t="s">
-        <v>58</v>
-      </c>
       <c r="D80" s="4">
         <v>3</v>
       </c>
       <c r="E80" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F80" s="3"/>
       <c r="G80" s="5"/>
@@ -2108,16 +2108,16 @@
         <v>52</v>
       </c>
       <c r="B81" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C81" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="C81" s="18" t="s">
-        <v>58</v>
-      </c>
       <c r="D81" s="4">
         <v>3</v>
       </c>
       <c r="E81" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F81" s="3"/>
       <c r="G81" s="5"/>
@@ -2136,16 +2136,16 @@
         <v>53</v>
       </c>
       <c r="B83" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C83" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="C83" s="18" t="s">
-        <v>60</v>
-      </c>
       <c r="D83" s="4">
         <v>3</v>
       </c>
       <c r="E83" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F83" s="3"/>
       <c r="G83" s="5"/>
@@ -2155,16 +2155,16 @@
         <v>54</v>
       </c>
       <c r="B84" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C84" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="C84" s="18" t="s">
-        <v>60</v>
-      </c>
       <c r="D84" s="4">
         <v>3</v>
       </c>
       <c r="E84" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F84" s="3"/>
       <c r="G84" s="5"/>
@@ -2174,16 +2174,16 @@
         <v>55</v>
       </c>
       <c r="B85" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C85" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="C85" s="18" t="s">
-        <v>60</v>
-      </c>
       <c r="D85" s="4">
         <v>3</v>
       </c>
       <c r="E85" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F85" s="3"/>
       <c r="G85" s="5"/>
@@ -2193,16 +2193,16 @@
         <v>56</v>
       </c>
       <c r="B86" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C86" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="C86" s="18" t="s">
-        <v>60</v>
-      </c>
       <c r="D86" s="4">
         <v>3</v>
       </c>
       <c r="E86" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F86" s="3"/>
       <c r="G86" s="5"/>
@@ -2221,16 +2221,16 @@
         <v>57</v>
       </c>
       <c r="B88" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="C88" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="C88" s="18" t="s">
-        <v>62</v>
-      </c>
       <c r="D88" s="4">
         <v>3</v>
       </c>
       <c r="E88" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F88" s="3"/>
       <c r="G88" s="5"/>
@@ -2240,16 +2240,16 @@
         <v>58</v>
       </c>
       <c r="B89" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="C89" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="C89" s="18" t="s">
-        <v>62</v>
-      </c>
       <c r="D89" s="4">
         <v>3</v>
       </c>
       <c r="E89" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F89" s="3"/>
       <c r="G89" s="5"/>
@@ -2259,16 +2259,16 @@
         <v>59</v>
       </c>
       <c r="B90" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="C90" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="C90" s="18" t="s">
-        <v>62</v>
-      </c>
       <c r="D90" s="4">
         <v>3</v>
       </c>
       <c r="E90" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F90" s="3"/>
       <c r="G90" s="5"/>
@@ -2278,16 +2278,16 @@
         <v>60</v>
       </c>
       <c r="B91" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="C91" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="C91" s="18" t="s">
-        <v>62</v>
-      </c>
       <c r="D91" s="4">
         <v>3</v>
       </c>
       <c r="E91" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F91" s="3"/>
       <c r="G91" s="5"/>
@@ -2306,16 +2306,16 @@
         <v>61</v>
       </c>
       <c r="B93" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C93" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="C93" s="18" t="s">
-        <v>64</v>
-      </c>
       <c r="D93" s="4">
         <v>3</v>
       </c>
       <c r="E93" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F93" s="3"/>
       <c r="G93" s="5"/>
@@ -2325,16 +2325,16 @@
         <v>62</v>
       </c>
       <c r="B94" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C94" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="C94" s="18" t="s">
-        <v>64</v>
-      </c>
       <c r="D94" s="4">
         <v>3</v>
       </c>
       <c r="E94" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F94" s="3"/>
       <c r="G94" s="5"/>
@@ -2344,16 +2344,16 @@
         <v>63</v>
       </c>
       <c r="B95" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C95" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="C95" s="18" t="s">
-        <v>64</v>
-      </c>
       <c r="D95" s="4">
         <v>3</v>
       </c>
       <c r="E95" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F95" s="3"/>
       <c r="G95" s="5"/>
@@ -2363,16 +2363,16 @@
         <v>64</v>
       </c>
       <c r="B96" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C96" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="C96" s="18" t="s">
-        <v>64</v>
-      </c>
       <c r="D96" s="4">
         <v>3</v>
       </c>
       <c r="E96" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F96" s="3"/>
       <c r="G96" s="5"/>
@@ -2391,16 +2391,16 @@
         <v>65</v>
       </c>
       <c r="B98" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C98" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="C98" s="18" t="s">
-        <v>66</v>
-      </c>
       <c r="D98" s="4">
         <v>3</v>
       </c>
       <c r="E98" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F98" s="3"/>
       <c r="G98" s="5"/>
@@ -2410,16 +2410,16 @@
         <v>66</v>
       </c>
       <c r="B99" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C99" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="C99" s="18" t="s">
-        <v>66</v>
-      </c>
       <c r="D99" s="4">
         <v>3</v>
       </c>
       <c r="E99" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F99" s="3"/>
       <c r="G99" s="5"/>
@@ -2429,16 +2429,16 @@
         <v>67</v>
       </c>
       <c r="B100" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C100" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="C100" s="18" t="s">
-        <v>66</v>
-      </c>
       <c r="D100" s="4">
         <v>3</v>
       </c>
       <c r="E100" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F100" s="3"/>
       <c r="G100" s="5"/>
@@ -2448,16 +2448,16 @@
         <v>68</v>
       </c>
       <c r="B101" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C101" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="C101" s="18" t="s">
-        <v>66</v>
-      </c>
       <c r="D101" s="4">
         <v>3</v>
       </c>
       <c r="E101" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F101" s="3"/>
       <c r="G101" s="5"/>
@@ -2476,16 +2476,16 @@
         <v>69</v>
       </c>
       <c r="B103" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="C103" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="C103" s="18" t="s">
-        <v>68</v>
-      </c>
       <c r="D103" s="4">
         <v>3</v>
       </c>
       <c r="E103" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F103" s="3"/>
       <c r="G103" s="5"/>
@@ -2495,16 +2495,16 @@
         <v>70</v>
       </c>
       <c r="B104" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="C104" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="C104" s="18" t="s">
-        <v>68</v>
-      </c>
       <c r="D104" s="4">
         <v>3</v>
       </c>
       <c r="E104" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F104" s="3"/>
       <c r="G104" s="5"/>
@@ -2514,16 +2514,16 @@
         <v>71</v>
       </c>
       <c r="B105" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="C105" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="C105" s="18" t="s">
-        <v>68</v>
-      </c>
       <c r="D105" s="4">
         <v>3</v>
       </c>
       <c r="E105" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F105" s="3"/>
       <c r="G105" s="5"/>
@@ -2533,16 +2533,16 @@
         <v>72</v>
       </c>
       <c r="B106" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="C106" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="C106" s="18" t="s">
-        <v>68</v>
-      </c>
       <c r="D106" s="4">
         <v>3</v>
       </c>
       <c r="E106" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F106" s="3"/>
       <c r="G106" s="5"/>
@@ -2570,16 +2570,16 @@
         <v>73</v>
       </c>
       <c r="B109" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="C109" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="C109" s="22" t="s">
-        <v>73</v>
-      </c>
       <c r="D109" s="4">
         <v>3</v>
       </c>
       <c r="E109" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F109" s="5"/>
       <c r="G109" s="5"/>
@@ -2589,16 +2589,16 @@
         <v>74</v>
       </c>
       <c r="B110" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="C110" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="C110" s="22" t="s">
-        <v>73</v>
-      </c>
       <c r="D110" s="4">
         <v>3</v>
       </c>
       <c r="E110" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F110" s="5"/>
       <c r="G110" s="5"/>
@@ -2608,16 +2608,16 @@
         <v>75</v>
       </c>
       <c r="B111" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="C111" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="C111" s="22" t="s">
-        <v>73</v>
-      </c>
       <c r="D111" s="4">
         <v>3</v>
       </c>
       <c r="E111" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F111" s="5"/>
       <c r="G111" s="5"/>
@@ -2636,16 +2636,16 @@
         <v>76</v>
       </c>
       <c r="B113" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="C113" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="C113" s="24" t="s">
-        <v>75</v>
-      </c>
       <c r="D113" s="4">
         <v>3</v>
       </c>
       <c r="E113" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F113" s="5"/>
       <c r="G113" s="5"/>
@@ -2655,16 +2655,16 @@
         <v>77</v>
       </c>
       <c r="B114" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="C114" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="C114" s="24" t="s">
-        <v>75</v>
-      </c>
       <c r="D114" s="4">
         <v>3</v>
       </c>
       <c r="E114" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F114" s="3"/>
       <c r="G114" s="5"/>
@@ -2674,16 +2674,16 @@
         <v>78</v>
       </c>
       <c r="B115" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="C115" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="C115" s="24" t="s">
-        <v>75</v>
-      </c>
       <c r="D115" s="4">
         <v>3</v>
       </c>
       <c r="E115" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F115" s="3"/>
       <c r="G115" s="5"/>
@@ -2702,16 +2702,16 @@
         <v>79</v>
       </c>
       <c r="B117" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="C117" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="C117" s="24" t="s">
-        <v>77</v>
-      </c>
       <c r="D117" s="4">
         <v>3</v>
       </c>
       <c r="E117" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F117" s="3"/>
       <c r="G117" s="5"/>
@@ -2721,16 +2721,16 @@
         <v>80</v>
       </c>
       <c r="B118" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="C118" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="C118" s="24" t="s">
-        <v>77</v>
-      </c>
       <c r="D118" s="4">
         <v>3</v>
       </c>
       <c r="E118" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F118" s="3"/>
       <c r="G118" s="5"/>
@@ -2740,16 +2740,16 @@
         <v>81</v>
       </c>
       <c r="B119" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="C119" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="C119" s="24" t="s">
-        <v>77</v>
-      </c>
       <c r="D119" s="4">
         <v>3</v>
       </c>
       <c r="E119" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F119" s="3"/>
       <c r="G119" s="5"/>
@@ -2768,16 +2768,16 @@
         <v>82</v>
       </c>
       <c r="B121" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C121" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="C121" s="25" t="s">
-        <v>79</v>
-      </c>
       <c r="D121" s="4">
         <v>3</v>
       </c>
       <c r="E121" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F121" s="3"/>
       <c r="G121" s="5"/>
@@ -2787,16 +2787,16 @@
         <v>83</v>
       </c>
       <c r="B122" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C122" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="C122" s="25" t="s">
-        <v>79</v>
-      </c>
       <c r="D122" s="4">
         <v>3</v>
       </c>
       <c r="E122" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F122" s="3"/>
       <c r="G122" s="5"/>
@@ -2806,16 +2806,16 @@
         <v>84</v>
       </c>
       <c r="B123" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C123" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="C123" s="25" t="s">
-        <v>79</v>
-      </c>
       <c r="D123" s="4">
         <v>3</v>
       </c>
       <c r="E123" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F123" s="3"/>
       <c r="G123" s="5"/>
@@ -2825,16 +2825,16 @@
         <v>85</v>
       </c>
       <c r="B124" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C124" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="C124" s="25" t="s">
-        <v>79</v>
-      </c>
       <c r="D124" s="4">
         <v>3</v>
       </c>
       <c r="E124" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F124" s="3"/>
       <c r="G124" s="5"/>
@@ -2871,16 +2871,16 @@
         <v>1</v>
       </c>
       <c r="B128" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="C128" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="C128" s="18" t="s">
+      <c r="D128" s="4">
+        <v>3</v>
+      </c>
+      <c r="E128" s="8" t="s">
         <v>68</v>
-      </c>
-      <c r="D128" s="4">
-        <v>3</v>
-      </c>
-      <c r="E128" s="8" t="s">
-        <v>69</v>
       </c>
       <c r="F128" s="3"/>
       <c r="G128" s="5"/>
@@ -2890,16 +2890,16 @@
         <v>2</v>
       </c>
       <c r="B129" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="C129" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="C129" s="18" t="s">
-        <v>68</v>
-      </c>
       <c r="D129" s="4">
         <v>3</v>
       </c>
       <c r="E129" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F129" s="3"/>
       <c r="G129" s="5"/>
@@ -2909,16 +2909,16 @@
         <v>3</v>
       </c>
       <c r="B130" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="C130" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="C130" s="18" t="s">
-        <v>68</v>
-      </c>
       <c r="D130" s="4">
         <v>3</v>
       </c>
       <c r="E130" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F130" s="3"/>
       <c r="G130" s="5"/>
@@ -2928,16 +2928,16 @@
         <v>4</v>
       </c>
       <c r="B131" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="C131" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="C131" s="18" t="s">
-        <v>68</v>
-      </c>
       <c r="D131" s="4">
         <v>3</v>
       </c>
       <c r="E131" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F131" s="3"/>
       <c r="G131" s="5"/>
@@ -2956,16 +2956,16 @@
         <v>5</v>
       </c>
       <c r="B133" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C133" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="C133" s="18" t="s">
-        <v>56</v>
-      </c>
       <c r="D133" s="4">
         <v>3</v>
       </c>
       <c r="E133" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F133" s="3"/>
       <c r="G133" s="5"/>
@@ -2975,16 +2975,16 @@
         <v>6</v>
       </c>
       <c r="B134" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C134" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="C134" s="18" t="s">
-        <v>56</v>
-      </c>
       <c r="D134" s="4">
         <v>3</v>
       </c>
       <c r="E134" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F134" s="3"/>
       <c r="G134" s="5"/>
@@ -2994,16 +2994,16 @@
         <v>7</v>
       </c>
       <c r="B135" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C135" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="C135" s="18" t="s">
-        <v>56</v>
-      </c>
       <c r="D135" s="4">
         <v>3</v>
       </c>
       <c r="E135" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F135" s="3"/>
       <c r="G135" s="5"/>
@@ -3013,16 +3013,16 @@
         <v>8</v>
       </c>
       <c r="B136" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C136" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="C136" s="18" t="s">
-        <v>56</v>
-      </c>
       <c r="D136" s="4">
         <v>3</v>
       </c>
       <c r="E136" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F136" s="11"/>
       <c r="G136" s="5"/>
@@ -3032,16 +3032,16 @@
         <v>9</v>
       </c>
       <c r="B137" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C137" s="18" t="s">
         <v>55</v>
-      </c>
-      <c r="C137" s="18" t="s">
-        <v>56</v>
       </c>
       <c r="D137" s="4">
         <v>4</v>
       </c>
       <c r="E137" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F137" s="11"/>
       <c r="G137" s="5"/>
@@ -3051,16 +3051,16 @@
         <v>10</v>
       </c>
       <c r="B138" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C138" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="C138" s="18" t="s">
-        <v>56</v>
-      </c>
       <c r="D138" s="4">
         <v>3</v>
       </c>
       <c r="E138" s="8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F138" s="3"/>
       <c r="G138" s="5"/>
@@ -3070,16 +3070,16 @@
         <v>11</v>
       </c>
       <c r="B139" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C139" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="C139" s="18" t="s">
-        <v>56</v>
-      </c>
       <c r="D139" s="4">
         <v>3</v>
       </c>
       <c r="E139" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F139" s="3"/>
       <c r="G139" s="5"/>
@@ -3089,16 +3089,16 @@
         <v>12</v>
       </c>
       <c r="B140" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C140" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="C140" s="18" t="s">
-        <v>56</v>
-      </c>
       <c r="D140" s="4">
         <v>3</v>
       </c>
       <c r="E140" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F140" s="3"/>
       <c r="G140" s="5"/>
@@ -3108,16 +3108,16 @@
         <v>13</v>
       </c>
       <c r="B141" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C141" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="C141" s="18" t="s">
-        <v>56</v>
-      </c>
       <c r="D141" s="4">
         <v>3</v>
       </c>
       <c r="E141" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F141" s="3"/>
       <c r="G141" s="5"/>
@@ -3127,16 +3127,16 @@
         <v>14</v>
       </c>
       <c r="B142" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C142" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="C142" s="18" t="s">
-        <v>56</v>
-      </c>
       <c r="D142" s="4">
         <v>3</v>
       </c>
       <c r="E142" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F142" s="3"/>
       <c r="G142" s="5"/>
@@ -3146,16 +3146,16 @@
         <v>15</v>
       </c>
       <c r="B143" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C143" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="C143" s="18" t="s">
-        <v>56</v>
-      </c>
       <c r="D143" s="4">
         <v>3</v>
       </c>
       <c r="E143" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F143" s="3"/>
       <c r="G143" s="5"/>
@@ -3165,16 +3165,16 @@
         <v>16</v>
       </c>
       <c r="B144" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C144" s="18" t="s">
         <v>55</v>
-      </c>
-      <c r="C144" s="18" t="s">
-        <v>56</v>
       </c>
       <c r="D144" s="4">
         <v>4</v>
       </c>
       <c r="E144" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F144" s="3"/>
       <c r="G144" s="5"/>
@@ -3184,16 +3184,16 @@
         <v>17</v>
       </c>
       <c r="B145" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C145" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="C145" s="18" t="s">
-        <v>56</v>
-      </c>
       <c r="D145" s="4">
         <v>3</v>
       </c>
       <c r="E145" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F145" s="3"/>
       <c r="G145" s="5"/>
@@ -3212,16 +3212,16 @@
         <v>18</v>
       </c>
       <c r="B147" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C147" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="C147" s="20" t="s">
-        <v>18</v>
-      </c>
       <c r="D147" s="4">
         <v>3</v>
       </c>
       <c r="E147" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F147" s="3"/>
       <c r="G147" s="5"/>
@@ -3231,16 +3231,16 @@
         <v>19</v>
       </c>
       <c r="B148" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C148" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="C148" s="20" t="s">
-        <v>18</v>
-      </c>
       <c r="D148" s="4">
         <v>3</v>
       </c>
       <c r="E148" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F148" s="3"/>
       <c r="G148" s="5"/>
@@ -3250,16 +3250,16 @@
         <v>20</v>
       </c>
       <c r="B149" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C149" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="C149" s="20" t="s">
-        <v>18</v>
-      </c>
       <c r="D149" s="4">
         <v>3</v>
       </c>
       <c r="E149" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F149" s="3"/>
       <c r="G149" s="5"/>
@@ -3269,16 +3269,16 @@
         <v>21</v>
       </c>
       <c r="B150" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C150" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="C150" s="20" t="s">
-        <v>18</v>
-      </c>
       <c r="D150" s="4">
         <v>3</v>
       </c>
       <c r="E150" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F150" s="3"/>
       <c r="G150" s="5"/>
@@ -3288,16 +3288,16 @@
         <v>22</v>
       </c>
       <c r="B151" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C151" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="C151" s="20" t="s">
-        <v>18</v>
-      </c>
       <c r="D151" s="4">
         <v>3</v>
       </c>
       <c r="E151" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F151" s="3"/>
       <c r="G151" s="5"/>
@@ -3307,16 +3307,16 @@
         <v>23</v>
       </c>
       <c r="B152" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C152" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="C152" s="20" t="s">
-        <v>18</v>
-      </c>
       <c r="D152" s="4">
         <v>3</v>
       </c>
       <c r="E152" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F152" s="3"/>
       <c r="G152" s="5"/>
@@ -3335,16 +3335,16 @@
         <v>24</v>
       </c>
       <c r="B154" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C154" s="18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D154" s="4">
         <v>3</v>
       </c>
       <c r="E154" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F154" s="3"/>
       <c r="G154" s="5"/>
@@ -3354,16 +3354,16 @@
         <v>25</v>
       </c>
       <c r="B155" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C155" s="18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D155" s="4">
         <v>3</v>
       </c>
       <c r="E155" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F155" s="3"/>
       <c r="G155" s="5"/>
@@ -3373,16 +3373,16 @@
         <v>26</v>
       </c>
       <c r="B156" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C156" s="18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D156" s="4">
         <v>3</v>
       </c>
       <c r="E156" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F156" s="3"/>
       <c r="G156" s="5"/>
@@ -3392,16 +3392,16 @@
         <v>27</v>
       </c>
       <c r="B157" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C157" s="18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D157" s="4">
         <v>3</v>
       </c>
       <c r="E157" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F157" s="3"/>
       <c r="G157" s="5"/>
@@ -3411,16 +3411,16 @@
         <v>28</v>
       </c>
       <c r="B158" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C158" s="18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D158" s="4">
         <v>3</v>
       </c>
       <c r="E158" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F158" s="3"/>
       <c r="G158" s="5"/>
@@ -3430,16 +3430,16 @@
         <v>29</v>
       </c>
       <c r="B159" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C159" s="18" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D159" s="4">
         <v>4</v>
       </c>
       <c r="E159" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F159" s="3"/>
       <c r="G159" s="5"/>
@@ -3449,16 +3449,16 @@
         <v>30</v>
       </c>
       <c r="B160" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C160" s="18" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D160" s="4">
         <v>5</v>
       </c>
       <c r="E160" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F160" s="3"/>
       <c r="G160" s="5"/>
@@ -3468,16 +3468,16 @@
         <v>31</v>
       </c>
       <c r="B161" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C161" s="18" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D161" s="4">
         <v>6</v>
       </c>
       <c r="E161" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F161" s="3"/>
       <c r="G161" s="5"/>

</xml_diff>

<commit_message>
added: excel column Year Level, Units renamed: Year Level -> Year Level & Department in admin.html
</commit_message>
<xml_diff>
--- a/static/files/subject_data.xlsx
+++ b/static/files/subject_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jenze\Desktop\PROF LOADING CAPSTONE PROJECT\ClassScheduler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3A214B3-AADB-40F6-8BB0-9F427FC84A8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A142928F-E48B-4CB1-8C91-281A9E8675DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -499,7 +499,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -561,14 +561,17 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -853,7 +856,7 @@
   <dimension ref="A1:H161"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -878,7 +881,7 @@
       <c r="C1" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="D1" s="28" t="s">
+      <c r="D1" s="27" t="s">
         <v>114</v>
       </c>
       <c r="E1" s="1" t="s">
@@ -919,7 +922,7 @@
       <c r="C4" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="29" t="s">
+      <c r="D4" s="25" t="s">
         <v>115</v>
       </c>
       <c r="E4" s="4">
@@ -940,7 +943,7 @@
       <c r="C5" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="29" t="s">
+      <c r="D5" s="25" t="s">
         <v>115</v>
       </c>
       <c r="E5" s="4">
@@ -961,7 +964,7 @@
       <c r="C6" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="29" t="s">
+      <c r="D6" s="25" t="s">
         <v>115</v>
       </c>
       <c r="E6" s="4">
@@ -976,7 +979,7 @@
       <c r="A7" s="3"/>
       <c r="B7" s="4"/>
       <c r="C7" s="18"/>
-      <c r="D7" s="29"/>
+      <c r="D7" s="25"/>
       <c r="E7" s="4"/>
       <c r="F7" s="3"/>
       <c r="G7" s="5"/>
@@ -985,6 +988,7 @@
       <c r="A8" s="3"/>
       <c r="B8" s="4"/>
       <c r="C8" s="19"/>
+      <c r="D8" s="30"/>
       <c r="E8" s="4"/>
       <c r="F8" s="3"/>
       <c r="G8" s="5"/>
@@ -999,7 +1003,7 @@
       <c r="C9" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="29" t="s">
+      <c r="D9" s="25" t="s">
         <v>116</v>
       </c>
       <c r="E9" s="4">
@@ -1020,7 +1024,7 @@
       <c r="C10" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="29" t="s">
+      <c r="D10" s="25" t="s">
         <v>116</v>
       </c>
       <c r="E10" s="4">
@@ -1041,7 +1045,7 @@
       <c r="C11" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="29" t="s">
+      <c r="D11" s="25" t="s">
         <v>116</v>
       </c>
       <c r="E11" s="4">
@@ -1056,7 +1060,7 @@
       <c r="A12" s="3"/>
       <c r="B12" s="4"/>
       <c r="C12" s="20"/>
-      <c r="D12" s="29"/>
+      <c r="D12" s="25"/>
       <c r="E12" s="4"/>
       <c r="F12" s="3"/>
       <c r="G12" s="5"/>
@@ -1071,7 +1075,7 @@
       <c r="C13" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="29" t="s">
+      <c r="D13" s="25" t="s">
         <v>116</v>
       </c>
       <c r="E13" s="4">
@@ -1092,7 +1096,7 @@
       <c r="C14" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="D14" s="29" t="s">
+      <c r="D14" s="25" t="s">
         <v>116</v>
       </c>
       <c r="E14" s="4">
@@ -1113,7 +1117,7 @@
       <c r="C15" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="D15" s="29" t="s">
+      <c r="D15" s="25" t="s">
         <v>116</v>
       </c>
       <c r="E15" s="4">
@@ -1128,7 +1132,7 @@
       <c r="A16" s="3"/>
       <c r="B16" s="4"/>
       <c r="C16" s="20"/>
-      <c r="D16" s="29"/>
+      <c r="D16" s="25"/>
       <c r="E16" s="4"/>
       <c r="F16" s="3"/>
       <c r="G16" s="5"/>
@@ -1143,7 +1147,7 @@
       <c r="C17" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="D17" s="29" t="s">
+      <c r="D17" s="25" t="s">
         <v>116</v>
       </c>
       <c r="E17" s="4">
@@ -1164,7 +1168,7 @@
       <c r="C18" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="D18" s="29" t="s">
+      <c r="D18" s="25" t="s">
         <v>116</v>
       </c>
       <c r="E18" s="4">
@@ -1185,7 +1189,7 @@
       <c r="C19" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="D19" s="29" t="s">
+      <c r="D19" s="25" t="s">
         <v>116</v>
       </c>
       <c r="E19" s="4">
@@ -1200,7 +1204,7 @@
       <c r="A20" s="3"/>
       <c r="B20" s="9"/>
       <c r="C20" s="21"/>
-      <c r="D20" s="29"/>
+      <c r="D20" s="25"/>
       <c r="E20" s="4"/>
       <c r="F20" s="3"/>
       <c r="G20" s="5"/>
@@ -1209,7 +1213,7 @@
       <c r="A21" s="3"/>
       <c r="B21" s="4"/>
       <c r="C21" s="17"/>
-      <c r="D21" s="29" t="s">
+      <c r="D21" s="25" t="s">
         <v>117</v>
       </c>
       <c r="E21" s="4"/>
@@ -1226,7 +1230,7 @@
       <c r="C22" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="D22" s="29" t="s">
+      <c r="D22" s="25" t="s">
         <v>117</v>
       </c>
       <c r="E22" s="4">
@@ -1247,7 +1251,7 @@
       <c r="C23" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="D23" s="29" t="s">
+      <c r="D23" s="25" t="s">
         <v>117</v>
       </c>
       <c r="E23" s="4">
@@ -1262,7 +1266,7 @@
       <c r="A24" s="3"/>
       <c r="B24" s="4"/>
       <c r="C24" s="20"/>
-      <c r="D24" s="29"/>
+      <c r="D24" s="25"/>
       <c r="E24" s="4"/>
       <c r="F24" s="3"/>
       <c r="G24" s="5"/>
@@ -1277,7 +1281,7 @@
       <c r="C25" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="D25" s="29" t="s">
+      <c r="D25" s="25" t="s">
         <v>117</v>
       </c>
       <c r="E25" s="4">
@@ -1298,7 +1302,7 @@
       <c r="C26" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="D26" s="29" t="s">
+      <c r="D26" s="25" t="s">
         <v>117</v>
       </c>
       <c r="E26" s="4">
@@ -1313,7 +1317,7 @@
       <c r="A27" s="5"/>
       <c r="B27" s="6"/>
       <c r="C27" s="22"/>
-      <c r="D27" s="29"/>
+      <c r="D27" s="25"/>
       <c r="E27" s="6"/>
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
@@ -1329,7 +1333,7 @@
       <c r="C28" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="D28" s="29" t="s">
+      <c r="D28" s="25" t="s">
         <v>117</v>
       </c>
       <c r="E28" s="4">
@@ -1351,7 +1355,7 @@
       <c r="C29" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="D29" s="29" t="s">
+      <c r="D29" s="25" t="s">
         <v>117</v>
       </c>
       <c r="E29" s="4">
@@ -1367,7 +1371,7 @@
       <c r="A30" s="3"/>
       <c r="B30" s="4"/>
       <c r="C30" s="20"/>
-      <c r="D30" s="29"/>
+      <c r="D30" s="25"/>
       <c r="E30" s="4"/>
       <c r="F30" s="3"/>
       <c r="G30" s="5"/>
@@ -1382,7 +1386,7 @@
       <c r="C31" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="D31" s="29" t="s">
+      <c r="D31" s="25" t="s">
         <v>117</v>
       </c>
       <c r="E31" s="4">
@@ -1403,7 +1407,7 @@
       <c r="C32" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="D32" s="29" t="s">
+      <c r="D32" s="25" t="s">
         <v>117</v>
       </c>
       <c r="E32" s="4">
@@ -1418,7 +1422,7 @@
       <c r="A33" s="3"/>
       <c r="B33" s="9"/>
       <c r="C33" s="18"/>
-      <c r="D33" s="29"/>
+      <c r="D33" s="25"/>
       <c r="E33" s="4"/>
       <c r="F33" s="3"/>
       <c r="G33" s="5"/>
@@ -1427,7 +1431,7 @@
       <c r="A34" s="3"/>
       <c r="B34" s="9"/>
       <c r="C34" s="20"/>
-      <c r="D34" s="29"/>
+      <c r="D34" s="25"/>
       <c r="E34" s="4"/>
       <c r="F34" s="3"/>
       <c r="G34" s="5"/>
@@ -1442,7 +1446,7 @@
       <c r="C35" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="D35" s="29" t="s">
+      <c r="D35" s="25" t="s">
         <v>117</v>
       </c>
       <c r="E35" s="4">
@@ -1463,7 +1467,7 @@
       <c r="C36" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="D36" s="29" t="s">
+      <c r="D36" s="25" t="s">
         <v>117</v>
       </c>
       <c r="E36" s="4">
@@ -1478,7 +1482,7 @@
       <c r="A37" s="3"/>
       <c r="B37" s="4"/>
       <c r="C37" s="20"/>
-      <c r="D37" s="29"/>
+      <c r="D37" s="25"/>
       <c r="E37" s="4"/>
       <c r="F37" s="3"/>
       <c r="G37" s="5"/>
@@ -1493,7 +1497,7 @@
       <c r="C38" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="D38" s="29" t="s">
+      <c r="D38" s="25" t="s">
         <v>117</v>
       </c>
       <c r="E38" s="4">
@@ -1514,7 +1518,7 @@
       <c r="C39" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="D39" s="29" t="s">
+      <c r="D39" s="25" t="s">
         <v>117</v>
       </c>
       <c r="E39" s="4">
@@ -1529,7 +1533,7 @@
       <c r="A40" s="3"/>
       <c r="B40" s="10"/>
       <c r="C40" s="23"/>
-      <c r="D40" s="29"/>
+      <c r="D40" s="25"/>
       <c r="E40" s="4"/>
       <c r="F40" s="3"/>
       <c r="G40" s="5"/>
@@ -1544,7 +1548,7 @@
       <c r="C41" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="D41" s="29" t="s">
+      <c r="D41" s="25" t="s">
         <v>117</v>
       </c>
       <c r="E41" s="4">
@@ -1565,7 +1569,7 @@
       <c r="C42" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="D42" s="29" t="s">
+      <c r="D42" s="25" t="s">
         <v>117</v>
       </c>
       <c r="E42" s="4">
@@ -1580,7 +1584,7 @@
       <c r="A43" s="3"/>
       <c r="B43" s="10"/>
       <c r="C43" s="23"/>
-      <c r="D43" s="29"/>
+      <c r="D43" s="25"/>
       <c r="E43" s="4"/>
       <c r="F43" s="3"/>
       <c r="G43" s="5"/>
@@ -1589,7 +1593,7 @@
       <c r="A44" s="3"/>
       <c r="B44" s="4"/>
       <c r="C44" s="19"/>
-      <c r="D44" s="29"/>
+      <c r="D44" s="25"/>
       <c r="E44" s="4"/>
       <c r="F44" s="3"/>
       <c r="G44" s="5"/>
@@ -1604,7 +1608,7 @@
       <c r="C45" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="D45" s="29" t="s">
+      <c r="D45" s="25" t="s">
         <v>118</v>
       </c>
       <c r="E45" s="4">
@@ -1625,7 +1629,7 @@
       <c r="C46" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="D46" s="29" t="s">
+      <c r="D46" s="25" t="s">
         <v>118</v>
       </c>
       <c r="E46" s="4">
@@ -1646,7 +1650,7 @@
       <c r="C47" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="D47" s="29" t="s">
+      <c r="D47" s="25" t="s">
         <v>118</v>
       </c>
       <c r="E47" s="4">
@@ -1661,7 +1665,7 @@
       <c r="A48" s="3"/>
       <c r="B48" s="4"/>
       <c r="C48" s="20"/>
-      <c r="D48" s="29"/>
+      <c r="D48" s="25"/>
       <c r="E48" s="4"/>
       <c r="F48" s="3"/>
       <c r="G48" s="5"/>
@@ -1676,7 +1680,7 @@
       <c r="C49" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="D49" s="29" t="s">
+      <c r="D49" s="25" t="s">
         <v>118</v>
       </c>
       <c r="E49" s="4">
@@ -1697,7 +1701,7 @@
       <c r="C50" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="D50" s="29" t="s">
+      <c r="D50" s="25" t="s">
         <v>118</v>
       </c>
       <c r="E50" s="4">
@@ -1718,7 +1722,7 @@
       <c r="C51" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="D51" s="29" t="s">
+      <c r="D51" s="25" t="s">
         <v>118</v>
       </c>
       <c r="E51" s="4">
@@ -1733,7 +1737,7 @@
       <c r="A52" s="3"/>
       <c r="B52" s="4"/>
       <c r="C52" s="20"/>
-      <c r="D52" s="29"/>
+      <c r="D52" s="25"/>
       <c r="E52" s="4"/>
       <c r="F52" s="3"/>
       <c r="G52" s="5"/>
@@ -1748,7 +1752,7 @@
       <c r="C53" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="D53" s="29" t="s">
+      <c r="D53" s="25" t="s">
         <v>118</v>
       </c>
       <c r="E53" s="4">
@@ -1769,7 +1773,7 @@
       <c r="C54" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="D54" s="29" t="s">
+      <c r="D54" s="25" t="s">
         <v>118</v>
       </c>
       <c r="E54" s="4">
@@ -1790,7 +1794,7 @@
       <c r="C55" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="D55" s="29" t="s">
+      <c r="D55" s="25" t="s">
         <v>118</v>
       </c>
       <c r="E55" s="4">
@@ -1805,16 +1809,16 @@
       <c r="A56" s="3"/>
       <c r="B56" s="4"/>
       <c r="C56" s="20"/>
-      <c r="D56" s="29"/>
+      <c r="D56" s="25"/>
       <c r="E56" s="4"/>
       <c r="F56" s="3"/>
       <c r="G56" s="5"/>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="3"/>
-      <c r="B57" s="27"/>
-      <c r="C57" s="27"/>
-      <c r="D57" s="29"/>
+      <c r="B57" s="29"/>
+      <c r="C57" s="29"/>
+      <c r="D57" s="25"/>
       <c r="E57" s="4"/>
       <c r="F57" s="3"/>
       <c r="G57" s="5"/>
@@ -1823,7 +1827,7 @@
       <c r="A58" s="3"/>
       <c r="B58" s="4"/>
       <c r="C58" s="19"/>
-      <c r="D58" s="29"/>
+      <c r="D58" s="25"/>
       <c r="E58" s="4"/>
       <c r="F58" s="3"/>
       <c r="G58" s="5"/>
@@ -1838,7 +1842,7 @@
       <c r="C59" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="D59" s="29" t="s">
+      <c r="D59" s="25" t="s">
         <v>119</v>
       </c>
       <c r="E59" s="4">
@@ -1859,7 +1863,7 @@
       <c r="C60" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="D60" s="29" t="s">
+      <c r="D60" s="25" t="s">
         <v>119</v>
       </c>
       <c r="E60" s="4">
@@ -1880,7 +1884,7 @@
       <c r="C61" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="D61" s="29" t="s">
+      <c r="D61" s="25" t="s">
         <v>119</v>
       </c>
       <c r="E61" s="4">
@@ -1895,7 +1899,7 @@
       <c r="A62" s="3"/>
       <c r="B62" s="4"/>
       <c r="C62" s="18"/>
-      <c r="D62" s="29"/>
+      <c r="D62" s="25"/>
       <c r="E62" s="4"/>
       <c r="F62" s="3"/>
       <c r="G62" s="5"/>
@@ -1904,7 +1908,7 @@
       <c r="A63" s="3"/>
       <c r="B63" s="4"/>
       <c r="C63" s="19"/>
-      <c r="D63" s="29"/>
+      <c r="D63" s="25"/>
       <c r="E63" s="4"/>
       <c r="F63" s="3"/>
       <c r="G63" s="5"/>
@@ -1919,7 +1923,7 @@
       <c r="C64" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="D64" s="29" t="s">
+      <c r="D64" s="25" t="s">
         <v>120</v>
       </c>
       <c r="E64" s="4">
@@ -1940,7 +1944,7 @@
       <c r="C65" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="D65" s="29" t="s">
+      <c r="D65" s="25" t="s">
         <v>120</v>
       </c>
       <c r="E65" s="4">
@@ -1961,7 +1965,7 @@
       <c r="C66" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="D66" s="29" t="s">
+      <c r="D66" s="25" t="s">
         <v>120</v>
       </c>
       <c r="E66" s="4">
@@ -1976,7 +1980,7 @@
       <c r="A67" s="3"/>
       <c r="B67" s="9"/>
       <c r="C67" s="18"/>
-      <c r="D67" s="29"/>
+      <c r="D67" s="25"/>
       <c r="E67" s="4"/>
       <c r="F67" s="3"/>
       <c r="G67" s="5"/>
@@ -1985,7 +1989,7 @@
       <c r="A68" s="3"/>
       <c r="B68" s="4"/>
       <c r="C68" s="20"/>
-      <c r="D68" s="29"/>
+      <c r="D68" s="25"/>
       <c r="E68" s="4"/>
       <c r="F68" s="3"/>
       <c r="G68" s="5"/>
@@ -2000,7 +2004,7 @@
       <c r="C69" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="D69" s="29" t="s">
+      <c r="D69" s="25" t="s">
         <v>120</v>
       </c>
       <c r="E69" s="4">
@@ -2021,7 +2025,7 @@
       <c r="C70" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="D70" s="29" t="s">
+      <c r="D70" s="25" t="s">
         <v>120</v>
       </c>
       <c r="E70" s="4">
@@ -2042,7 +2046,7 @@
       <c r="C71" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="D71" s="29" t="s">
+      <c r="D71" s="25" t="s">
         <v>120</v>
       </c>
       <c r="E71" s="4">
@@ -2057,7 +2061,7 @@
       <c r="A72" s="3"/>
       <c r="B72" s="4"/>
       <c r="C72" s="18"/>
-      <c r="D72" s="29"/>
+      <c r="D72" s="25"/>
       <c r="E72" s="4"/>
       <c r="F72" s="3"/>
       <c r="G72" s="5"/>
@@ -2072,7 +2076,7 @@
       <c r="C73" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="D73" s="29" t="s">
+      <c r="D73" s="25" t="s">
         <v>120</v>
       </c>
       <c r="E73" s="4">
@@ -2093,7 +2097,7 @@
       <c r="C74" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="D74" s="29" t="s">
+      <c r="D74" s="25" t="s">
         <v>120</v>
       </c>
       <c r="E74" s="4">
@@ -2114,7 +2118,7 @@
       <c r="C75" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="D75" s="29" t="s">
+      <c r="D75" s="25" t="s">
         <v>120</v>
       </c>
       <c r="E75" s="4">
@@ -2129,7 +2133,7 @@
       <c r="A76" s="3"/>
       <c r="B76" s="4"/>
       <c r="C76" s="20"/>
-      <c r="D76" s="29"/>
+      <c r="D76" s="25"/>
       <c r="E76" s="4"/>
       <c r="F76" s="3"/>
       <c r="G76" s="5"/>
@@ -2138,7 +2142,7 @@
       <c r="A77" s="3"/>
       <c r="B77" s="4"/>
       <c r="C77" s="19"/>
-      <c r="D77" s="29"/>
+      <c r="D77" s="25"/>
       <c r="E77" s="4"/>
       <c r="F77" s="3"/>
       <c r="G77" s="5"/>
@@ -2153,7 +2157,7 @@
       <c r="C78" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="D78" s="29" t="s">
+      <c r="D78" s="25" t="s">
         <v>121</v>
       </c>
       <c r="E78" s="4">
@@ -2174,7 +2178,7 @@
       <c r="C79" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="D79" s="29" t="s">
+      <c r="D79" s="25" t="s">
         <v>121</v>
       </c>
       <c r="E79" s="4">
@@ -2195,7 +2199,7 @@
       <c r="C80" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="D80" s="29" t="s">
+      <c r="D80" s="25" t="s">
         <v>121</v>
       </c>
       <c r="E80" s="4">
@@ -2216,7 +2220,7 @@
       <c r="C81" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="D81" s="29" t="s">
+      <c r="D81" s="25" t="s">
         <v>121</v>
       </c>
       <c r="E81" s="4">
@@ -2231,7 +2235,7 @@
       <c r="A82" s="3"/>
       <c r="B82" s="4"/>
       <c r="C82" s="20"/>
-      <c r="D82" s="29"/>
+      <c r="D82" s="25"/>
       <c r="E82" s="4"/>
       <c r="F82" s="3"/>
       <c r="G82" s="5"/>
@@ -2246,7 +2250,7 @@
       <c r="C83" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="D83" s="29" t="s">
+      <c r="D83" s="25" t="s">
         <v>121</v>
       </c>
       <c r="E83" s="4">
@@ -2267,7 +2271,7 @@
       <c r="C84" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="D84" s="29" t="s">
+      <c r="D84" s="25" t="s">
         <v>121</v>
       </c>
       <c r="E84" s="4">
@@ -2288,7 +2292,7 @@
       <c r="C85" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="D85" s="29" t="s">
+      <c r="D85" s="25" t="s">
         <v>121</v>
       </c>
       <c r="E85" s="4">
@@ -2309,7 +2313,7 @@
       <c r="C86" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="D86" s="29" t="s">
+      <c r="D86" s="25" t="s">
         <v>121</v>
       </c>
       <c r="E86" s="4">
@@ -2324,7 +2328,7 @@
       <c r="A87" s="3"/>
       <c r="B87" s="4"/>
       <c r="C87" s="20"/>
-      <c r="D87" s="29"/>
+      <c r="D87" s="25"/>
       <c r="E87" s="4"/>
       <c r="F87" s="3"/>
       <c r="G87" s="5"/>
@@ -2339,7 +2343,7 @@
       <c r="C88" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="D88" s="29" t="s">
+      <c r="D88" s="25" t="s">
         <v>121</v>
       </c>
       <c r="E88" s="4">
@@ -2360,7 +2364,7 @@
       <c r="C89" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="D89" s="29" t="s">
+      <c r="D89" s="25" t="s">
         <v>121</v>
       </c>
       <c r="E89" s="4">
@@ -2381,7 +2385,7 @@
       <c r="C90" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="D90" s="29" t="s">
+      <c r="D90" s="25" t="s">
         <v>121</v>
       </c>
       <c r="E90" s="4">
@@ -2402,7 +2406,7 @@
       <c r="C91" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="D91" s="29" t="s">
+      <c r="D91" s="25" t="s">
         <v>121</v>
       </c>
       <c r="E91" s="4">
@@ -2417,7 +2421,7 @@
       <c r="A92" s="3"/>
       <c r="B92" s="4"/>
       <c r="C92" s="20"/>
-      <c r="D92" s="29"/>
+      <c r="D92" s="25"/>
       <c r="E92" s="4"/>
       <c r="F92" s="3"/>
       <c r="G92" s="5"/>
@@ -2432,7 +2436,7 @@
       <c r="C93" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="D93" s="29" t="s">
+      <c r="D93" s="25" t="s">
         <v>121</v>
       </c>
       <c r="E93" s="4">
@@ -2453,7 +2457,7 @@
       <c r="C94" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="D94" s="29" t="s">
+      <c r="D94" s="25" t="s">
         <v>121</v>
       </c>
       <c r="E94" s="4">
@@ -2474,7 +2478,7 @@
       <c r="C95" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="D95" s="29" t="s">
+      <c r="D95" s="25" t="s">
         <v>121</v>
       </c>
       <c r="E95" s="4">
@@ -2495,7 +2499,7 @@
       <c r="C96" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="D96" s="29" t="s">
+      <c r="D96" s="25" t="s">
         <v>121</v>
       </c>
       <c r="E96" s="4">
@@ -2510,7 +2514,7 @@
       <c r="A97" s="3"/>
       <c r="B97" s="4"/>
       <c r="C97" s="20"/>
-      <c r="D97" s="29"/>
+      <c r="D97" s="25"/>
       <c r="E97" s="4"/>
       <c r="F97" s="3"/>
       <c r="G97" s="5"/>
@@ -2525,7 +2529,7 @@
       <c r="C98" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="D98" s="29" t="s">
+      <c r="D98" s="25" t="s">
         <v>121</v>
       </c>
       <c r="E98" s="4">
@@ -2546,7 +2550,7 @@
       <c r="C99" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="D99" s="29" t="s">
+      <c r="D99" s="25" t="s">
         <v>121</v>
       </c>
       <c r="E99" s="4">
@@ -2567,7 +2571,7 @@
       <c r="C100" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="D100" s="29" t="s">
+      <c r="D100" s="25" t="s">
         <v>121</v>
       </c>
       <c r="E100" s="4">
@@ -2588,7 +2592,7 @@
       <c r="C101" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="D101" s="29" t="s">
+      <c r="D101" s="25" t="s">
         <v>121</v>
       </c>
       <c r="E101" s="4">
@@ -2603,7 +2607,7 @@
       <c r="A102" s="3"/>
       <c r="B102" s="4"/>
       <c r="C102" s="20"/>
-      <c r="D102" s="29"/>
+      <c r="D102" s="25"/>
       <c r="E102" s="4"/>
       <c r="F102" s="3"/>
       <c r="G102" s="5"/>
@@ -2618,7 +2622,7 @@
       <c r="C103" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="D103" s="29" t="s">
+      <c r="D103" s="25" t="s">
         <v>121</v>
       </c>
       <c r="E103" s="4">
@@ -2639,7 +2643,7 @@
       <c r="C104" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="D104" s="29" t="s">
+      <c r="D104" s="25" t="s">
         <v>121</v>
       </c>
       <c r="E104" s="4">
@@ -2660,7 +2664,7 @@
       <c r="C105" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="D105" s="29" t="s">
+      <c r="D105" s="25" t="s">
         <v>121</v>
       </c>
       <c r="E105" s="4">
@@ -2681,7 +2685,7 @@
       <c r="C106" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="D106" s="29" t="s">
+      <c r="D106" s="25" t="s">
         <v>121</v>
       </c>
       <c r="E106" s="4">
@@ -2696,7 +2700,7 @@
       <c r="A107" s="3"/>
       <c r="B107" s="4"/>
       <c r="C107" s="20"/>
-      <c r="D107" s="29"/>
+      <c r="D107" s="25"/>
       <c r="E107" s="4"/>
       <c r="F107" s="3"/>
       <c r="G107" s="5"/>
@@ -2705,7 +2709,7 @@
       <c r="A108" s="3"/>
       <c r="B108" s="4"/>
       <c r="C108" s="19"/>
-      <c r="D108" s="29"/>
+      <c r="D108" s="25"/>
       <c r="E108" s="4"/>
       <c r="F108" s="3"/>
       <c r="G108" s="5"/>
@@ -2720,7 +2724,7 @@
       <c r="C109" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="D109" s="29" t="s">
+      <c r="D109" s="25" t="s">
         <v>122</v>
       </c>
       <c r="E109" s="4">
@@ -2741,7 +2745,7 @@
       <c r="C110" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="D110" s="29" t="s">
+      <c r="D110" s="25" t="s">
         <v>122</v>
       </c>
       <c r="E110" s="4">
@@ -2762,7 +2766,7 @@
       <c r="C111" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="D111" s="29" t="s">
+      <c r="D111" s="25" t="s">
         <v>122</v>
       </c>
       <c r="E111" s="4">
@@ -2777,7 +2781,7 @@
       <c r="A112" s="3"/>
       <c r="B112" s="4"/>
       <c r="C112" s="20"/>
-      <c r="D112" s="29"/>
+      <c r="D112" s="25"/>
       <c r="E112" s="4"/>
       <c r="F112" s="3"/>
       <c r="G112" s="5"/>
@@ -2792,7 +2796,7 @@
       <c r="C113" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="D113" s="29" t="s">
+      <c r="D113" s="25" t="s">
         <v>122</v>
       </c>
       <c r="E113" s="4">
@@ -2813,7 +2817,7 @@
       <c r="C114" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="D114" s="29" t="s">
+      <c r="D114" s="25" t="s">
         <v>122</v>
       </c>
       <c r="E114" s="4">
@@ -2834,7 +2838,7 @@
       <c r="C115" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="D115" s="29" t="s">
+      <c r="D115" s="25" t="s">
         <v>122</v>
       </c>
       <c r="E115" s="4">
@@ -2849,7 +2853,7 @@
       <c r="A116" s="3"/>
       <c r="B116" s="4"/>
       <c r="C116" s="20"/>
-      <c r="D116" s="29"/>
+      <c r="D116" s="25"/>
       <c r="E116" s="4"/>
       <c r="F116" s="3"/>
       <c r="G116" s="5"/>
@@ -2864,7 +2868,7 @@
       <c r="C117" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="D117" s="29" t="s">
+      <c r="D117" s="25" t="s">
         <v>122</v>
       </c>
       <c r="E117" s="4">
@@ -2885,7 +2889,7 @@
       <c r="C118" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="D118" s="29" t="s">
+      <c r="D118" s="25" t="s">
         <v>122</v>
       </c>
       <c r="E118" s="4">
@@ -2906,7 +2910,7 @@
       <c r="C119" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="D119" s="29" t="s">
+      <c r="D119" s="25" t="s">
         <v>122</v>
       </c>
       <c r="E119" s="4">
@@ -2921,7 +2925,7 @@
       <c r="A120" s="3"/>
       <c r="B120" s="4"/>
       <c r="C120" s="20"/>
-      <c r="D120" s="29"/>
+      <c r="D120" s="25"/>
       <c r="E120" s="4"/>
       <c r="F120" s="3"/>
       <c r="G120" s="5"/>
@@ -2936,7 +2940,7 @@
       <c r="C121" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="D121" s="29" t="s">
+      <c r="D121" s="25" t="s">
         <v>122</v>
       </c>
       <c r="E121" s="4">
@@ -2957,7 +2961,7 @@
       <c r="C122" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="D122" s="29" t="s">
+      <c r="D122" s="25" t="s">
         <v>122</v>
       </c>
       <c r="E122" s="4">
@@ -2978,7 +2982,7 @@
       <c r="C123" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="D123" s="29" t="s">
+      <c r="D123" s="25" t="s">
         <v>122</v>
       </c>
       <c r="E123" s="4">
@@ -2999,7 +3003,7 @@
       <c r="C124" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="D124" s="29" t="s">
+      <c r="D124" s="25" t="s">
         <v>122</v>
       </c>
       <c r="E124" s="4">
@@ -3014,16 +3018,16 @@
       <c r="A125" s="3"/>
       <c r="B125" s="4"/>
       <c r="C125" s="25"/>
-      <c r="D125" s="29"/>
+      <c r="D125" s="28"/>
       <c r="E125" s="4"/>
       <c r="F125" s="3"/>
       <c r="G125" s="5"/>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" s="3"/>
-      <c r="B126" s="27"/>
-      <c r="C126" s="27"/>
-      <c r="D126" s="29"/>
+      <c r="B126" s="29"/>
+      <c r="C126" s="29"/>
+      <c r="D126" s="28"/>
       <c r="E126" s="4"/>
       <c r="F126" s="3"/>
       <c r="G126" s="5"/>
@@ -3032,7 +3036,7 @@
       <c r="A127" s="3"/>
       <c r="B127" s="1"/>
       <c r="C127" s="16"/>
-      <c r="D127" s="29"/>
+      <c r="D127" s="28"/>
       <c r="E127" s="4"/>
       <c r="F127" s="3"/>
       <c r="G127" s="5"/>
@@ -3047,7 +3051,7 @@
       <c r="C128" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="D128" s="29"/>
+      <c r="D128" s="28"/>
       <c r="E128" s="4">
         <v>3</v>
       </c>
@@ -3066,7 +3070,7 @@
       <c r="C129" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="D129" s="29"/>
+      <c r="D129" s="28"/>
       <c r="E129" s="4">
         <v>3</v>
       </c>
@@ -3085,7 +3089,7 @@
       <c r="C130" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="D130" s="29"/>
+      <c r="D130" s="28"/>
       <c r="E130" s="4">
         <v>3</v>
       </c>
@@ -3104,7 +3108,7 @@
       <c r="C131" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="D131" s="29"/>
+      <c r="D131" s="28"/>
       <c r="E131" s="4">
         <v>3</v>
       </c>
@@ -3117,7 +3121,7 @@
       <c r="A132" s="3"/>
       <c r="B132" s="9"/>
       <c r="C132" s="18"/>
-      <c r="D132" s="29"/>
+      <c r="D132" s="28"/>
       <c r="E132" s="4"/>
       <c r="F132" s="7"/>
       <c r="G132" s="5"/>
@@ -3132,7 +3136,7 @@
       <c r="C133" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="D133" s="29"/>
+      <c r="D133" s="28"/>
       <c r="E133" s="4">
         <v>3</v>
       </c>
@@ -3151,7 +3155,7 @@
       <c r="C134" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="D134" s="29"/>
+      <c r="D134" s="28"/>
       <c r="E134" s="4">
         <v>3</v>
       </c>
@@ -3170,7 +3174,7 @@
       <c r="C135" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="D135" s="29"/>
+      <c r="D135" s="28"/>
       <c r="E135" s="4">
         <v>3</v>
       </c>
@@ -3189,7 +3193,7 @@
       <c r="C136" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="D136" s="29"/>
+      <c r="D136" s="28"/>
       <c r="E136" s="4">
         <v>3</v>
       </c>
@@ -3208,7 +3212,7 @@
       <c r="C137" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="D137" s="29"/>
+      <c r="D137" s="28"/>
       <c r="E137" s="4">
         <v>4</v>
       </c>
@@ -3227,7 +3231,7 @@
       <c r="C138" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="D138" s="29"/>
+      <c r="D138" s="28"/>
       <c r="E138" s="4">
         <v>3</v>
       </c>
@@ -3246,7 +3250,7 @@
       <c r="C139" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="D139" s="29"/>
+      <c r="D139" s="28"/>
       <c r="E139" s="4">
         <v>3</v>
       </c>
@@ -3265,7 +3269,7 @@
       <c r="C140" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="D140" s="29"/>
+      <c r="D140" s="28"/>
       <c r="E140" s="4">
         <v>3</v>
       </c>
@@ -3284,7 +3288,7 @@
       <c r="C141" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="D141" s="29"/>
+      <c r="D141" s="28"/>
       <c r="E141" s="4">
         <v>3</v>
       </c>
@@ -3303,7 +3307,7 @@
       <c r="C142" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="D142" s="29"/>
+      <c r="D142" s="28"/>
       <c r="E142" s="4">
         <v>3</v>
       </c>
@@ -3322,7 +3326,7 @@
       <c r="C143" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="D143" s="29"/>
+      <c r="D143" s="28"/>
       <c r="E143" s="4">
         <v>3</v>
       </c>
@@ -3341,7 +3345,7 @@
       <c r="C144" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="D144" s="29"/>
+      <c r="D144" s="28"/>
       <c r="E144" s="4">
         <v>4</v>
       </c>
@@ -3360,7 +3364,7 @@
       <c r="C145" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="D145" s="29"/>
+      <c r="D145" s="28"/>
       <c r="E145" s="4">
         <v>3</v>
       </c>
@@ -3373,7 +3377,7 @@
       <c r="A146" s="3"/>
       <c r="B146" s="1"/>
       <c r="C146" s="16"/>
-      <c r="D146" s="29"/>
+      <c r="D146" s="28"/>
       <c r="E146" s="4"/>
       <c r="F146" s="3"/>
       <c r="G146" s="5"/>
@@ -3388,7 +3392,7 @@
       <c r="C147" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="D147" s="29"/>
+      <c r="D147" s="28"/>
       <c r="E147" s="4">
         <v>3</v>
       </c>
@@ -3407,7 +3411,7 @@
       <c r="C148" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="D148" s="29"/>
+      <c r="D148" s="28"/>
       <c r="E148" s="4">
         <v>3</v>
       </c>
@@ -3426,7 +3430,7 @@
       <c r="C149" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="D149" s="29"/>
+      <c r="D149" s="28"/>
       <c r="E149" s="4">
         <v>3</v>
       </c>
@@ -3445,7 +3449,7 @@
       <c r="C150" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="D150" s="29"/>
+      <c r="D150" s="28"/>
       <c r="E150" s="4">
         <v>3</v>
       </c>
@@ -3464,7 +3468,7 @@
       <c r="C151" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="D151" s="29"/>
+      <c r="D151" s="28"/>
       <c r="E151" s="4">
         <v>3</v>
       </c>
@@ -3483,7 +3487,7 @@
       <c r="C152" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="D152" s="29"/>
+      <c r="D152" s="28"/>
       <c r="E152" s="4">
         <v>3</v>
       </c>
@@ -3496,7 +3500,7 @@
       <c r="A153" s="3"/>
       <c r="B153" s="4"/>
       <c r="C153" s="20"/>
-      <c r="D153" s="29"/>
+      <c r="D153" s="28"/>
       <c r="E153" s="4"/>
       <c r="F153" s="3"/>
       <c r="G153" s="5"/>
@@ -3511,7 +3515,7 @@
       <c r="C154" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="D154" s="29"/>
+      <c r="D154" s="28"/>
       <c r="E154" s="4">
         <v>3</v>
       </c>
@@ -3530,7 +3534,7 @@
       <c r="C155" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="D155" s="29"/>
+      <c r="D155" s="28"/>
       <c r="E155" s="4">
         <v>3</v>
       </c>
@@ -3549,7 +3553,7 @@
       <c r="C156" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="D156" s="29"/>
+      <c r="D156" s="28"/>
       <c r="E156" s="4">
         <v>3</v>
       </c>
@@ -3568,7 +3572,7 @@
       <c r="C157" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="D157" s="29"/>
+      <c r="D157" s="28"/>
       <c r="E157" s="4">
         <v>3</v>
       </c>
@@ -3587,7 +3591,7 @@
       <c r="C158" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="D158" s="29"/>
+      <c r="D158" s="28"/>
       <c r="E158" s="4">
         <v>3</v>
       </c>
@@ -3606,7 +3610,7 @@
       <c r="C159" s="18" t="s">
         <v>110</v>
       </c>
-      <c r="D159" s="29"/>
+      <c r="D159" s="28"/>
       <c r="E159" s="4">
         <v>4</v>
       </c>
@@ -3625,7 +3629,7 @@
       <c r="C160" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="D160" s="29"/>
+      <c r="D160" s="28"/>
       <c r="E160" s="4">
         <v>5</v>
       </c>
@@ -3644,7 +3648,7 @@
       <c r="C161" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="D161" s="29"/>
+      <c r="D161" s="28"/>
       <c r="E161" s="4">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
added: 4:30 - 9:00 PM in 1.5hr increments in table added: new start time options added: course offerings overflow y scroll - thanks Mark added: course delete success message added: file upload success refresh / redirection
</commit_message>
<xml_diff>
--- a/static/files/subject_data.xlsx
+++ b/static/files/subject_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jenze\Desktop\PROF LOADING CAPSTONE PROJECT\ClassScheduler\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jenze\Desktop\PROF LOADING CAPSTONE PROJECT\cbfsls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E93C9516-8119-4259-8EB5-CE7502080D80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4011AC2A-540A-4DF6-942F-666A1C758862}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6810" yWindow="1260" windowWidth="21990" windowHeight="13395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="128">
   <si>
     <t>COURSE CODE</t>
   </si>
@@ -404,6 +404,12 @@
   </si>
   <si>
     <t>FOURTH YEAR - HRDM</t>
+  </si>
+  <si>
+    <t>COURSE TYPE</t>
+  </si>
+  <si>
+    <t>Major</t>
   </si>
 </sst>
 </file>
@@ -853,8 +859,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A102" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="D122" sqref="D122"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -866,10 +872,10 @@
     <col min="5" max="5" width="24.28515625" customWidth="1"/>
     <col min="6" max="6" width="26.28515625" customWidth="1"/>
     <col min="7" max="7" width="28.5703125" style="14" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="13"/>
+    <col min="8" max="8" width="26.7109375" style="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -886,31 +892,36 @@
         <v>6</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="1"/>
       <c r="C2" s="18"/>
       <c r="D2" s="18"/>
       <c r="E2" s="18"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="1"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F2" s="18"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="1"/>
       <c r="C3" s="16"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="1"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F3" s="18"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>1</v>
       </c>
@@ -926,14 +937,17 @@
       <c r="E4" s="4">
         <v>6</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G4" s="6">
         <v>801</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>2</v>
       </c>
@@ -949,14 +963,17 @@
       <c r="E5" s="4">
         <v>6</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G5" s="6">
         <v>802</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="H5" s="3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>3</v>
       </c>
@@ -972,36 +989,41 @@
       <c r="E6" s="4">
         <v>6</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G6" s="6">
         <v>803</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="H6" s="3" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="4"/>
       <c r="C7" s="17"/>
       <c r="D7" s="24"/>
       <c r="E7" s="4"/>
-      <c r="F7" s="6">
+      <c r="F7" s="18"/>
+      <c r="G7" s="6">
         <v>804</v>
       </c>
-      <c r="G7" s="3"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H7" s="3"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="4"/>
       <c r="C8" s="18"/>
       <c r="D8" s="24"/>
       <c r="E8" s="4"/>
-      <c r="F8" s="6">
+      <c r="F8" s="18"/>
+      <c r="G8" s="6">
         <v>805</v>
       </c>
-      <c r="G8" s="3"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H8" s="3"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>4</v>
       </c>
@@ -1017,14 +1039,17 @@
       <c r="E9" s="4">
         <v>6</v>
       </c>
-      <c r="F9" s="6">
+      <c r="F9" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G9" s="6">
         <v>806</v>
       </c>
-      <c r="G9" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H9" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>5</v>
       </c>
@@ -1040,14 +1065,17 @@
       <c r="E10" s="4">
         <v>6</v>
       </c>
-      <c r="F10" s="6">
+      <c r="F10" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G10" s="6">
         <v>807</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="H10" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>6</v>
       </c>
@@ -1063,25 +1091,29 @@
       <c r="E11" s="4">
         <v>6</v>
       </c>
-      <c r="F11" s="6">
+      <c r="F11" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G11" s="6">
         <v>808</v>
       </c>
-      <c r="G11" s="3" t="s">
+      <c r="H11" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="4"/>
       <c r="C12" s="19"/>
       <c r="D12" s="24"/>
       <c r="E12" s="4"/>
-      <c r="F12" s="6">
+      <c r="F12" s="18"/>
+      <c r="G12" s="6">
         <v>809</v>
       </c>
-      <c r="G12" s="3"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H12" s="3"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>7</v>
       </c>
@@ -1097,14 +1129,17 @@
       <c r="E13" s="4">
         <v>3</v>
       </c>
-      <c r="F13" s="6">
+      <c r="F13" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G13" s="6">
         <v>810</v>
       </c>
-      <c r="G13" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H13" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>8</v>
       </c>
@@ -1120,14 +1155,17 @@
       <c r="E14" s="4">
         <v>3</v>
       </c>
-      <c r="F14" s="6">
+      <c r="F14" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G14" s="6">
         <v>811</v>
       </c>
-      <c r="G14" s="3" t="s">
+      <c r="H14" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>9</v>
       </c>
@@ -1143,25 +1181,29 @@
       <c r="E15" s="4">
         <v>3</v>
       </c>
-      <c r="F15" s="6">
+      <c r="F15" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G15" s="6">
         <v>812</v>
       </c>
-      <c r="G15" s="3" t="s">
+      <c r="H15" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="4"/>
       <c r="C16" s="19"/>
       <c r="D16" s="24"/>
       <c r="E16" s="4"/>
-      <c r="F16" s="6">
+      <c r="F16" s="18"/>
+      <c r="G16" s="6">
         <v>813</v>
       </c>
-      <c r="G16" s="3"/>
-    </row>
-    <row r="17" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H16" s="3"/>
+    </row>
+    <row r="17" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>10</v>
       </c>
@@ -1177,14 +1219,17 @@
       <c r="E17" s="4">
         <v>3</v>
       </c>
-      <c r="F17" s="6">
+      <c r="F17" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G17" s="6">
         <v>814</v>
       </c>
-      <c r="G17" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H17" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>11</v>
       </c>
@@ -1200,14 +1245,17 @@
       <c r="E18" s="4">
         <v>3</v>
       </c>
-      <c r="F18" s="6">
+      <c r="F18" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G18" s="6">
         <v>815</v>
       </c>
-      <c r="G18" s="3" t="s">
+      <c r="H18" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>12</v>
       </c>
@@ -1223,36 +1271,41 @@
       <c r="E19" s="4">
         <v>3</v>
       </c>
-      <c r="F19" s="6">
+      <c r="F19" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G19" s="6">
         <v>901</v>
       </c>
-      <c r="G19" s="3" t="s">
+      <c r="H19" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="9"/>
       <c r="C20" s="20"/>
       <c r="D20" s="24"/>
       <c r="E20" s="4"/>
-      <c r="F20" s="6">
+      <c r="F20" s="18"/>
+      <c r="G20" s="6">
         <v>902</v>
       </c>
-      <c r="G20" s="3"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H20" s="3"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="4"/>
       <c r="C21" s="16"/>
       <c r="D21" s="24"/>
       <c r="E21" s="4"/>
-      <c r="F21" s="6">
+      <c r="F21" s="18"/>
+      <c r="G21" s="6">
         <v>903</v>
       </c>
-      <c r="G21" s="3"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H21" s="3"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>13</v>
       </c>
@@ -1268,14 +1321,17 @@
       <c r="E22" s="4">
         <v>4</v>
       </c>
-      <c r="F22" s="6">
+      <c r="F22" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G22" s="6">
         <v>904</v>
       </c>
-      <c r="G22" s="3" t="s">
+      <c r="H22" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>14</v>
       </c>
@@ -1291,25 +1347,29 @@
       <c r="E23" s="4">
         <v>4</v>
       </c>
-      <c r="F23" s="6">
+      <c r="F23" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G23" s="6">
         <v>905</v>
       </c>
-      <c r="G23" s="3" t="s">
+      <c r="H23" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="4"/>
       <c r="C24" s="19"/>
       <c r="D24" s="24"/>
       <c r="E24" s="4"/>
-      <c r="F24" s="6">
+      <c r="F24" s="18"/>
+      <c r="G24" s="6">
         <v>906</v>
       </c>
-      <c r="G24" s="3"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H24" s="3"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>15</v>
       </c>
@@ -1325,14 +1385,17 @@
       <c r="E25" s="4">
         <v>3</v>
       </c>
-      <c r="F25" s="6">
+      <c r="F25" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G25" s="6">
         <v>907</v>
       </c>
-      <c r="G25" s="3" t="s">
+      <c r="H25" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>16</v>
       </c>
@@ -1348,25 +1411,29 @@
       <c r="E26" s="4">
         <v>3</v>
       </c>
-      <c r="F26" s="6">
+      <c r="F26" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G26" s="6">
         <v>908</v>
       </c>
-      <c r="G26" s="3" t="s">
+      <c r="H26" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="27" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
       <c r="B27" s="6"/>
       <c r="C27" s="21"/>
       <c r="D27" s="24"/>
       <c r="E27" s="6"/>
-      <c r="F27" s="6">
+      <c r="F27" s="18"/>
+      <c r="G27" s="6">
         <v>909</v>
       </c>
-      <c r="G27" s="5"/>
-    </row>
-    <row r="28" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H27" s="5"/>
+    </row>
+    <row r="28" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <v>17</v>
       </c>
@@ -1382,14 +1449,17 @@
       <c r="E28" s="4">
         <v>3</v>
       </c>
-      <c r="F28" s="6">
+      <c r="F28" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G28" s="6">
         <v>910</v>
       </c>
-      <c r="G28" s="3" t="s">
+      <c r="H28" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <v>18</v>
       </c>
@@ -1405,25 +1475,29 @@
       <c r="E29" s="4">
         <v>3</v>
       </c>
-      <c r="F29" s="6">
+      <c r="F29" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G29" s="6">
         <v>911</v>
       </c>
-      <c r="G29" s="3" t="s">
+      <c r="H29" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
       <c r="B30" s="4"/>
       <c r="C30" s="19"/>
       <c r="D30" s="24"/>
       <c r="E30" s="4"/>
-      <c r="F30" s="6">
+      <c r="F30" s="18"/>
+      <c r="G30" s="6">
         <v>912</v>
       </c>
-      <c r="G30" s="3"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H30" s="3"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>19</v>
       </c>
@@ -1439,14 +1513,17 @@
       <c r="E31" s="4">
         <v>3</v>
       </c>
-      <c r="F31" s="6">
+      <c r="F31" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G31" s="6">
         <v>913</v>
       </c>
-      <c r="G31" s="3" t="s">
+      <c r="H31" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>20</v>
       </c>
@@ -1462,36 +1539,41 @@
       <c r="E32" s="4">
         <v>3</v>
       </c>
-      <c r="F32" s="6">
+      <c r="F32" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G32" s="6">
         <v>914</v>
       </c>
-      <c r="G32" s="3" t="s">
+      <c r="H32" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="3"/>
       <c r="B33" s="9"/>
       <c r="C33" s="17"/>
       <c r="D33" s="24"/>
       <c r="E33" s="4"/>
-      <c r="F33" s="6">
+      <c r="F33" s="18"/>
+      <c r="G33" s="6">
         <v>915</v>
       </c>
-      <c r="G33" s="3"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H33" s="3"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
       <c r="B34" s="9"/>
       <c r="C34" s="19"/>
       <c r="D34" s="24"/>
       <c r="E34" s="4"/>
-      <c r="F34" s="6">
+      <c r="F34" s="18"/>
+      <c r="G34" s="6">
         <v>1001</v>
       </c>
-      <c r="G34" s="3"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H34" s="3"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>21</v>
       </c>
@@ -1507,14 +1589,17 @@
       <c r="E35" s="4">
         <v>3</v>
       </c>
-      <c r="F35" s="6">
+      <c r="F35" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G35" s="6">
         <v>1002</v>
       </c>
-      <c r="G35" s="3" t="s">
+      <c r="H35" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>22</v>
       </c>
@@ -1530,25 +1615,29 @@
       <c r="E36" s="4">
         <v>3</v>
       </c>
-      <c r="F36" s="6">
+      <c r="F36" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G36" s="6">
         <v>1003</v>
       </c>
-      <c r="G36" s="3" t="s">
+      <c r="H36" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="3"/>
       <c r="B37" s="4"/>
       <c r="C37" s="19"/>
       <c r="D37" s="24"/>
       <c r="E37" s="4"/>
-      <c r="F37" s="6">
+      <c r="F37" s="18"/>
+      <c r="G37" s="6">
         <v>1004</v>
       </c>
-      <c r="G37" s="3"/>
-    </row>
-    <row r="38" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H37" s="3"/>
+    </row>
+    <row r="38" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>23</v>
       </c>
@@ -1564,14 +1653,17 @@
       <c r="E38" s="4">
         <v>3</v>
       </c>
-      <c r="F38" s="6">
+      <c r="F38" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G38" s="6">
         <v>1005</v>
       </c>
-      <c r="G38" s="3" t="s">
+      <c r="H38" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>24</v>
       </c>
@@ -1587,25 +1679,29 @@
       <c r="E39" s="4">
         <v>3</v>
       </c>
-      <c r="F39" s="6">
+      <c r="F39" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G39" s="6">
         <v>1006</v>
       </c>
-      <c r="G39" s="3" t="s">
+      <c r="H39" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="3"/>
       <c r="B40" s="10"/>
       <c r="C40" s="22"/>
       <c r="D40" s="24"/>
       <c r="E40" s="4"/>
-      <c r="F40" s="6">
+      <c r="F40" s="18"/>
+      <c r="G40" s="6">
         <v>1007</v>
       </c>
-      <c r="G40" s="3"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H40" s="3"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>25</v>
       </c>
@@ -1621,14 +1717,17 @@
       <c r="E41" s="4">
         <v>3</v>
       </c>
-      <c r="F41" s="6">
+      <c r="F41" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G41" s="6">
         <v>1008</v>
       </c>
-      <c r="G41" s="3" t="s">
+      <c r="H41" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>26</v>
       </c>
@@ -1644,36 +1743,41 @@
       <c r="E42" s="4">
         <v>3</v>
       </c>
-      <c r="F42" s="6">
+      <c r="F42" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G42" s="6">
         <v>1009</v>
       </c>
-      <c r="G42" s="3" t="s">
+      <c r="H42" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="3"/>
       <c r="B43" s="10"/>
       <c r="C43" s="22"/>
       <c r="D43" s="24"/>
       <c r="E43" s="4"/>
-      <c r="F43" s="6">
+      <c r="F43" s="18"/>
+      <c r="G43" s="6">
         <v>1010</v>
       </c>
-      <c r="G43" s="3"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H43" s="3"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="3"/>
       <c r="B44" s="4"/>
       <c r="C44" s="18"/>
       <c r="D44" s="24"/>
       <c r="E44" s="4"/>
-      <c r="F44" s="6">
+      <c r="F44" s="18"/>
+      <c r="G44" s="6">
         <v>1011</v>
       </c>
-      <c r="G44" s="3"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H44" s="3"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>27</v>
       </c>
@@ -1689,14 +1793,17 @@
       <c r="E45" s="4">
         <v>3</v>
       </c>
-      <c r="F45" s="6">
+      <c r="F45" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G45" s="6">
         <v>1012</v>
       </c>
-      <c r="G45" s="3" t="s">
+      <c r="H45" s="3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <v>28</v>
       </c>
@@ -1712,14 +1819,17 @@
       <c r="E46" s="4">
         <v>3</v>
       </c>
-      <c r="F46" s="6">
+      <c r="F46" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G46" s="6">
         <v>1013</v>
       </c>
-      <c r="G46" s="3" t="s">
+      <c r="H46" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>29</v>
       </c>
@@ -1735,25 +1845,29 @@
       <c r="E47" s="4">
         <v>3</v>
       </c>
-      <c r="F47" s="6">
+      <c r="F47" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G47" s="6">
         <v>1014</v>
       </c>
-      <c r="G47" s="3" t="s">
+      <c r="H47" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="3"/>
       <c r="B48" s="4"/>
       <c r="C48" s="19"/>
       <c r="D48" s="24"/>
       <c r="E48" s="4"/>
-      <c r="F48" s="6">
+      <c r="F48" s="18"/>
+      <c r="G48" s="6">
         <v>1015</v>
       </c>
-      <c r="G48" s="3"/>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H48" s="3"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
         <v>30</v>
       </c>
@@ -1769,12 +1883,15 @@
       <c r="E49" s="4">
         <v>3</v>
       </c>
-      <c r="F49" s="5"/>
-      <c r="G49" s="3" t="s">
+      <c r="F49" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G49" s="5"/>
+      <c r="H49" s="3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
         <v>31</v>
       </c>
@@ -1790,12 +1907,15 @@
       <c r="E50" s="4">
         <v>3</v>
       </c>
-      <c r="F50" s="5"/>
-      <c r="G50" s="3" t="s">
+      <c r="F50" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G50" s="5"/>
+      <c r="H50" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
         <v>32</v>
       </c>
@@ -1811,21 +1931,25 @@
       <c r="E51" s="4">
         <v>3</v>
       </c>
-      <c r="F51" s="5"/>
-      <c r="G51" s="3" t="s">
+      <c r="F51" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G51" s="5"/>
+      <c r="H51" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="3"/>
       <c r="B52" s="4"/>
       <c r="C52" s="19"/>
       <c r="D52" s="24"/>
       <c r="E52" s="4"/>
-      <c r="F52" s="5"/>
-      <c r="G52" s="3"/>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F52" s="18"/>
+      <c r="G52" s="5"/>
+      <c r="H52" s="3"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
         <v>33</v>
       </c>
@@ -1841,12 +1965,15 @@
       <c r="E53" s="4">
         <v>3</v>
       </c>
-      <c r="F53" s="5"/>
-      <c r="G53" s="3" t="s">
+      <c r="F53" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G53" s="5"/>
+      <c r="H53" s="3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
         <v>34</v>
       </c>
@@ -1862,12 +1989,15 @@
       <c r="E54" s="4">
         <v>3</v>
       </c>
-      <c r="F54" s="5"/>
-      <c r="G54" s="3" t="s">
+      <c r="F54" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G54" s="5"/>
+      <c r="H54" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
         <v>36</v>
       </c>
@@ -1883,39 +2013,45 @@
       <c r="E55" s="4">
         <v>3</v>
       </c>
-      <c r="F55" s="5"/>
-      <c r="G55" s="3" t="s">
+      <c r="F55" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G55" s="5"/>
+      <c r="H55" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="3"/>
       <c r="B56" s="4"/>
       <c r="C56" s="19"/>
       <c r="D56" s="24"/>
       <c r="E56" s="4"/>
-      <c r="F56" s="5"/>
-      <c r="G56" s="3"/>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F56" s="18"/>
+      <c r="G56" s="5"/>
+      <c r="H56" s="3"/>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="3"/>
       <c r="B57" s="26"/>
       <c r="C57" s="26"/>
       <c r="D57" s="24"/>
       <c r="E57" s="4"/>
-      <c r="F57" s="5"/>
-      <c r="G57" s="3"/>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F57" s="18"/>
+      <c r="G57" s="5"/>
+      <c r="H57" s="3"/>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="3"/>
       <c r="B58" s="4"/>
       <c r="C58" s="18"/>
       <c r="D58" s="24"/>
       <c r="E58" s="4"/>
-      <c r="F58" s="5"/>
-      <c r="G58" s="3"/>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F58" s="18"/>
+      <c r="G58" s="5"/>
+      <c r="H58" s="3"/>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="3">
         <v>37</v>
       </c>
@@ -1931,12 +2067,15 @@
       <c r="E59" s="4">
         <v>3</v>
       </c>
-      <c r="F59" s="5"/>
-      <c r="G59" s="3" t="s">
+      <c r="F59" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G59" s="5"/>
+      <c r="H59" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="3">
         <v>38</v>
       </c>
@@ -1952,12 +2091,15 @@
       <c r="E60" s="4">
         <v>3</v>
       </c>
-      <c r="F60" s="5"/>
-      <c r="G60" s="3" t="s">
+      <c r="F60" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G60" s="5"/>
+      <c r="H60" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="3">
         <v>39</v>
       </c>
@@ -1973,30 +2115,35 @@
       <c r="E61" s="4">
         <v>3</v>
       </c>
-      <c r="F61" s="5"/>
-      <c r="G61" s="3" t="s">
+      <c r="F61" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G61" s="5"/>
+      <c r="H61" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="3"/>
       <c r="B62" s="4"/>
       <c r="C62" s="17"/>
       <c r="D62" s="24"/>
       <c r="E62" s="4"/>
-      <c r="F62" s="5"/>
-      <c r="G62" s="3"/>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F62" s="18"/>
+      <c r="G62" s="5"/>
+      <c r="H62" s="3"/>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="3"/>
       <c r="B63" s="4"/>
       <c r="C63" s="18"/>
       <c r="D63" s="24"/>
       <c r="E63" s="4"/>
-      <c r="F63" s="5"/>
-      <c r="G63" s="3"/>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F63" s="18"/>
+      <c r="G63" s="5"/>
+      <c r="H63" s="3"/>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="3">
         <v>40</v>
       </c>
@@ -2012,12 +2159,15 @@
       <c r="E64" s="4">
         <v>3</v>
       </c>
-      <c r="F64" s="5"/>
-      <c r="G64" s="3" t="s">
+      <c r="F64" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G64" s="5"/>
+      <c r="H64" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="3">
         <v>41</v>
       </c>
@@ -2033,12 +2183,15 @@
       <c r="E65" s="4">
         <v>3</v>
       </c>
-      <c r="F65" s="5"/>
-      <c r="G65" s="3" t="s">
+      <c r="F65" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G65" s="5"/>
+      <c r="H65" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="3">
         <v>42</v>
       </c>
@@ -2054,30 +2207,35 @@
       <c r="E66" s="4">
         <v>3</v>
       </c>
-      <c r="F66" s="5"/>
-      <c r="G66" s="3" t="s">
+      <c r="F66" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G66" s="5"/>
+      <c r="H66" s="3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="3"/>
       <c r="B67" s="9"/>
       <c r="C67" s="17"/>
       <c r="D67" s="24"/>
       <c r="E67" s="4"/>
-      <c r="F67" s="5"/>
-      <c r="G67" s="3"/>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F67" s="18"/>
+      <c r="G67" s="5"/>
+      <c r="H67" s="3"/>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="3"/>
       <c r="B68" s="4"/>
       <c r="C68" s="19"/>
       <c r="D68" s="24"/>
       <c r="E68" s="4"/>
-      <c r="F68" s="5"/>
-      <c r="G68" s="3"/>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F68" s="18"/>
+      <c r="G68" s="5"/>
+      <c r="H68" s="3"/>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="3">
         <v>43</v>
       </c>
@@ -2093,12 +2251,15 @@
       <c r="E69" s="4">
         <v>3</v>
       </c>
-      <c r="F69" s="5"/>
-      <c r="G69" s="3" t="s">
+      <c r="F69" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G69" s="5"/>
+      <c r="H69" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="3">
         <v>44</v>
       </c>
@@ -2114,12 +2275,15 @@
       <c r="E70" s="4">
         <v>3</v>
       </c>
-      <c r="F70" s="5"/>
-      <c r="G70" s="3" t="s">
+      <c r="F70" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G70" s="5"/>
+      <c r="H70" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="3">
         <v>45</v>
       </c>
@@ -2135,21 +2299,25 @@
       <c r="E71" s="4">
         <v>3</v>
       </c>
-      <c r="F71" s="5"/>
-      <c r="G71" s="3" t="s">
+      <c r="F71" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G71" s="5"/>
+      <c r="H71" s="3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="3"/>
       <c r="B72" s="4"/>
       <c r="C72" s="17"/>
       <c r="D72" s="24"/>
       <c r="E72" s="4"/>
-      <c r="F72" s="5"/>
-      <c r="G72" s="3"/>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F72" s="18"/>
+      <c r="G72" s="5"/>
+      <c r="H72" s="3"/>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="3">
         <v>46</v>
       </c>
@@ -2165,12 +2333,15 @@
       <c r="E73" s="4">
         <v>3</v>
       </c>
-      <c r="F73" s="5"/>
-      <c r="G73" s="3" t="s">
+      <c r="F73" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G73" s="5"/>
+      <c r="H73" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="3">
         <v>47</v>
       </c>
@@ -2186,12 +2357,15 @@
       <c r="E74" s="4">
         <v>3</v>
       </c>
-      <c r="F74" s="5"/>
-      <c r="G74" s="3" t="s">
+      <c r="F74" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G74" s="5"/>
+      <c r="H74" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="3">
         <v>48</v>
       </c>
@@ -2207,30 +2381,35 @@
       <c r="E75" s="4">
         <v>3</v>
       </c>
-      <c r="F75" s="5"/>
-      <c r="G75" s="3" t="s">
+      <c r="F75" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G75" s="5"/>
+      <c r="H75" s="3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="3"/>
       <c r="B76" s="4"/>
       <c r="C76" s="19"/>
       <c r="D76" s="24"/>
       <c r="E76" s="4"/>
-      <c r="F76" s="5"/>
-      <c r="G76" s="3"/>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F76" s="18"/>
+      <c r="G76" s="5"/>
+      <c r="H76" s="3"/>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="3"/>
       <c r="B77" s="4"/>
       <c r="C77" s="18"/>
       <c r="D77" s="24"/>
       <c r="E77" s="4"/>
-      <c r="F77" s="5"/>
-      <c r="G77" s="3"/>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F77" s="18"/>
+      <c r="G77" s="5"/>
+      <c r="H77" s="3"/>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="3">
         <v>49</v>
       </c>
@@ -2246,12 +2425,15 @@
       <c r="E78" s="4">
         <v>3</v>
       </c>
-      <c r="F78" s="5"/>
-      <c r="G78" s="3" t="s">
+      <c r="F78" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G78" s="5"/>
+      <c r="H78" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="3">
         <v>50</v>
       </c>
@@ -2267,12 +2449,15 @@
       <c r="E79" s="4">
         <v>3</v>
       </c>
-      <c r="F79" s="5"/>
-      <c r="G79" s="3" t="s">
+      <c r="F79" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G79" s="5"/>
+      <c r="H79" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="3">
         <v>51</v>
       </c>
@@ -2288,12 +2473,15 @@
       <c r="E80" s="4">
         <v>3</v>
       </c>
-      <c r="F80" s="5"/>
-      <c r="G80" s="3" t="s">
+      <c r="F80" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G80" s="5"/>
+      <c r="H80" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="3">
         <v>52</v>
       </c>
@@ -2309,21 +2497,25 @@
       <c r="E81" s="4">
         <v>3</v>
       </c>
-      <c r="F81" s="5"/>
-      <c r="G81" s="3" t="s">
+      <c r="F81" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G81" s="5"/>
+      <c r="H81" s="3" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="3"/>
       <c r="B82" s="4"/>
       <c r="C82" s="19"/>
       <c r="D82" s="24"/>
       <c r="E82" s="4"/>
-      <c r="F82" s="5"/>
-      <c r="G82" s="3"/>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F82" s="18"/>
+      <c r="G82" s="5"/>
+      <c r="H82" s="3"/>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="3">
         <v>53</v>
       </c>
@@ -2339,12 +2531,15 @@
       <c r="E83" s="4">
         <v>3</v>
       </c>
-      <c r="F83" s="5"/>
-      <c r="G83" s="3" t="s">
+      <c r="F83" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G83" s="5"/>
+      <c r="H83" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="3">
         <v>54</v>
       </c>
@@ -2360,12 +2555,15 @@
       <c r="E84" s="4">
         <v>3</v>
       </c>
-      <c r="F84" s="5"/>
-      <c r="G84" s="3" t="s">
+      <c r="F84" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G84" s="5"/>
+      <c r="H84" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="3">
         <v>55</v>
       </c>
@@ -2381,12 +2579,15 @@
       <c r="E85" s="4">
         <v>3</v>
       </c>
-      <c r="F85" s="5"/>
-      <c r="G85" s="3" t="s">
+      <c r="F85" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G85" s="5"/>
+      <c r="H85" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="3">
         <v>56</v>
       </c>
@@ -2402,21 +2603,25 @@
       <c r="E86" s="4">
         <v>3</v>
       </c>
-      <c r="F86" s="5"/>
-      <c r="G86" s="3" t="s">
+      <c r="F86" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G86" s="5"/>
+      <c r="H86" s="3" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="3"/>
       <c r="B87" s="4"/>
       <c r="C87" s="19"/>
       <c r="D87" s="24"/>
       <c r="E87" s="4"/>
-      <c r="F87" s="5"/>
-      <c r="G87" s="3"/>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F87" s="18"/>
+      <c r="G87" s="5"/>
+      <c r="H87" s="3"/>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="3">
         <v>57</v>
       </c>
@@ -2432,12 +2637,15 @@
       <c r="E88" s="4">
         <v>3</v>
       </c>
-      <c r="F88" s="5"/>
-      <c r="G88" s="3" t="s">
+      <c r="F88" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G88" s="5"/>
+      <c r="H88" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="3">
         <v>58</v>
       </c>
@@ -2453,12 +2661,15 @@
       <c r="E89" s="4">
         <v>3</v>
       </c>
-      <c r="F89" s="5"/>
-      <c r="G89" s="3" t="s">
+      <c r="F89" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G89" s="5"/>
+      <c r="H89" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="3">
         <v>59</v>
       </c>
@@ -2474,12 +2685,15 @@
       <c r="E90" s="4">
         <v>3</v>
       </c>
-      <c r="F90" s="5"/>
-      <c r="G90" s="3" t="s">
+      <c r="F90" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G90" s="5"/>
+      <c r="H90" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="3">
         <v>60</v>
       </c>
@@ -2495,21 +2709,25 @@
       <c r="E91" s="4">
         <v>3</v>
       </c>
-      <c r="F91" s="5"/>
-      <c r="G91" s="3" t="s">
+      <c r="F91" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G91" s="5"/>
+      <c r="H91" s="3" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="3"/>
       <c r="B92" s="4"/>
       <c r="C92" s="19"/>
       <c r="D92" s="24"/>
       <c r="E92" s="4"/>
-      <c r="F92" s="5"/>
-      <c r="G92" s="3"/>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F92" s="18"/>
+      <c r="G92" s="5"/>
+      <c r="H92" s="3"/>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="3">
         <v>61</v>
       </c>
@@ -2525,12 +2743,15 @@
       <c r="E93" s="4">
         <v>3</v>
       </c>
-      <c r="F93" s="5"/>
-      <c r="G93" s="3" t="s">
+      <c r="F93" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G93" s="5"/>
+      <c r="H93" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="3">
         <v>62</v>
       </c>
@@ -2546,12 +2767,15 @@
       <c r="E94" s="4">
         <v>3</v>
       </c>
-      <c r="F94" s="5"/>
-      <c r="G94" s="3" t="s">
+      <c r="F94" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G94" s="5"/>
+      <c r="H94" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="3">
         <v>63</v>
       </c>
@@ -2567,12 +2791,15 @@
       <c r="E95" s="4">
         <v>3</v>
       </c>
-      <c r="F95" s="5"/>
-      <c r="G95" s="3" t="s">
+      <c r="F95" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G95" s="5"/>
+      <c r="H95" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="3">
         <v>64</v>
       </c>
@@ -2588,21 +2815,25 @@
       <c r="E96" s="4">
         <v>3</v>
       </c>
-      <c r="F96" s="5"/>
-      <c r="G96" s="3" t="s">
+      <c r="F96" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G96" s="5"/>
+      <c r="H96" s="3" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="3"/>
       <c r="B97" s="4"/>
       <c r="C97" s="19"/>
       <c r="D97" s="24"/>
       <c r="E97" s="4"/>
-      <c r="F97" s="5"/>
-      <c r="G97" s="3"/>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F97" s="18"/>
+      <c r="G97" s="5"/>
+      <c r="H97" s="3"/>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="3">
         <v>65</v>
       </c>
@@ -2618,12 +2849,15 @@
       <c r="E98" s="4">
         <v>3</v>
       </c>
-      <c r="F98" s="5"/>
-      <c r="G98" s="3" t="s">
+      <c r="F98" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G98" s="5"/>
+      <c r="H98" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="3">
         <v>66</v>
       </c>
@@ -2639,12 +2873,15 @@
       <c r="E99" s="4">
         <v>3</v>
       </c>
-      <c r="F99" s="5"/>
-      <c r="G99" s="3" t="s">
+      <c r="F99" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G99" s="5"/>
+      <c r="H99" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="3">
         <v>67</v>
       </c>
@@ -2660,12 +2897,15 @@
       <c r="E100" s="4">
         <v>3</v>
       </c>
-      <c r="F100" s="5"/>
-      <c r="G100" s="3" t="s">
+      <c r="F100" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G100" s="5"/>
+      <c r="H100" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="3">
         <v>68</v>
       </c>
@@ -2681,21 +2921,25 @@
       <c r="E101" s="4">
         <v>3</v>
       </c>
-      <c r="F101" s="5"/>
-      <c r="G101" s="3" t="s">
+      <c r="F101" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G101" s="5"/>
+      <c r="H101" s="3" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" s="3"/>
       <c r="B102" s="4"/>
       <c r="C102" s="19"/>
       <c r="D102" s="24"/>
       <c r="E102" s="4"/>
-      <c r="F102" s="5"/>
-      <c r="G102" s="3"/>
-    </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F102" s="18"/>
+      <c r="G102" s="5"/>
+      <c r="H102" s="3"/>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" s="3">
         <v>69</v>
       </c>
@@ -2711,12 +2955,15 @@
       <c r="E103" s="4">
         <v>3</v>
       </c>
-      <c r="F103" s="5"/>
-      <c r="G103" s="3" t="s">
+      <c r="F103" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G103" s="5"/>
+      <c r="H103" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" s="3">
         <v>70</v>
       </c>
@@ -2732,12 +2979,15 @@
       <c r="E104" s="4">
         <v>3</v>
       </c>
-      <c r="F104" s="5"/>
-      <c r="G104" s="3" t="s">
+      <c r="F104" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G104" s="5"/>
+      <c r="H104" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" s="3">
         <v>71</v>
       </c>
@@ -2753,12 +3003,15 @@
       <c r="E105" s="4">
         <v>3</v>
       </c>
-      <c r="F105" s="5"/>
-      <c r="G105" s="3" t="s">
+      <c r="F105" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G105" s="5"/>
+      <c r="H105" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" s="3">
         <v>72</v>
       </c>
@@ -2774,30 +3027,35 @@
       <c r="E106" s="4">
         <v>3</v>
       </c>
-      <c r="F106" s="5"/>
-      <c r="G106" s="3" t="s">
+      <c r="F106" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G106" s="5"/>
+      <c r="H106" s="3" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" s="3"/>
       <c r="B107" s="4"/>
       <c r="C107" s="19"/>
       <c r="D107" s="24"/>
       <c r="E107" s="4"/>
-      <c r="F107" s="5"/>
-      <c r="G107" s="3"/>
-    </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F107" s="18"/>
+      <c r="G107" s="5"/>
+      <c r="H107" s="3"/>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" s="3"/>
       <c r="B108" s="4"/>
       <c r="C108" s="18"/>
       <c r="D108" s="24"/>
       <c r="E108" s="4"/>
-      <c r="F108" s="5"/>
-      <c r="G108" s="3"/>
-    </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F108" s="18"/>
+      <c r="G108" s="5"/>
+      <c r="H108" s="3"/>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" s="3">
         <v>73</v>
       </c>
@@ -2813,12 +3071,15 @@
       <c r="E109" s="4">
         <v>3</v>
       </c>
-      <c r="F109" s="5"/>
-      <c r="G109" s="3" t="s">
+      <c r="F109" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G109" s="5"/>
+      <c r="H109" s="3" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" s="3">
         <v>74</v>
       </c>
@@ -2834,12 +3095,15 @@
       <c r="E110" s="4">
         <v>3</v>
       </c>
-      <c r="F110" s="5"/>
-      <c r="G110" s="3" t="s">
+      <c r="F110" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G110" s="5"/>
+      <c r="H110" s="3" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" s="3">
         <v>75</v>
       </c>
@@ -2855,12 +3119,15 @@
       <c r="E111" s="4">
         <v>3</v>
       </c>
-      <c r="F111" s="5"/>
-      <c r="G111" s="3" t="s">
+      <c r="F111" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G111" s="5"/>
+      <c r="H111" s="3" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" s="3"/>
       <c r="B112" s="4"/>
       <c r="C112" s="19"/>
@@ -2868,10 +3135,11 @@
         <v>125</v>
       </c>
       <c r="E112" s="4"/>
-      <c r="F112" s="5"/>
-      <c r="G112" s="3"/>
-    </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F112" s="18"/>
+      <c r="G112" s="5"/>
+      <c r="H112" s="3"/>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" s="3">
         <v>76</v>
       </c>
@@ -2887,12 +3155,15 @@
       <c r="E113" s="4">
         <v>3</v>
       </c>
-      <c r="F113" s="5"/>
-      <c r="G113" s="3" t="s">
+      <c r="F113" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G113" s="5"/>
+      <c r="H113" s="3" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" s="3">
         <v>77</v>
       </c>
@@ -2908,12 +3179,15 @@
       <c r="E114" s="4">
         <v>3</v>
       </c>
-      <c r="F114" s="5"/>
-      <c r="G114" s="3" t="s">
+      <c r="F114" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G114" s="5"/>
+      <c r="H114" s="3" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" s="3">
         <v>78</v>
       </c>
@@ -2929,12 +3203,15 @@
       <c r="E115" s="4">
         <v>3</v>
       </c>
-      <c r="F115" s="5"/>
-      <c r="G115" s="3" t="s">
+      <c r="F115" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G115" s="5"/>
+      <c r="H115" s="3" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116" s="3"/>
       <c r="B116" s="4"/>
       <c r="C116" s="19"/>
@@ -2942,10 +3219,11 @@
         <v>125</v>
       </c>
       <c r="E116" s="4"/>
-      <c r="F116" s="5"/>
-      <c r="G116" s="3"/>
-    </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F116" s="18"/>
+      <c r="G116" s="5"/>
+      <c r="H116" s="3"/>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117" s="3">
         <v>79</v>
       </c>
@@ -2961,12 +3239,15 @@
       <c r="E117" s="4">
         <v>3</v>
       </c>
-      <c r="F117" s="5"/>
-      <c r="G117" s="3" t="s">
+      <c r="F117" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G117" s="5"/>
+      <c r="H117" s="3" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118" s="3">
         <v>80</v>
       </c>
@@ -2982,12 +3263,15 @@
       <c r="E118" s="4">
         <v>3</v>
       </c>
-      <c r="F118" s="5"/>
-      <c r="G118" s="3" t="s">
+      <c r="F118" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G118" s="5"/>
+      <c r="H118" s="3" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119" s="3">
         <v>81</v>
       </c>
@@ -3003,12 +3287,15 @@
       <c r="E119" s="4">
         <v>3</v>
       </c>
-      <c r="F119" s="5"/>
-      <c r="G119" s="3" t="s">
+      <c r="F119" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G119" s="5"/>
+      <c r="H119" s="3" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120" s="3"/>
       <c r="B120" s="4"/>
       <c r="C120" s="19"/>
@@ -3016,10 +3303,11 @@
         <v>125</v>
       </c>
       <c r="E120" s="4"/>
-      <c r="F120" s="5"/>
-      <c r="G120" s="3"/>
-    </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F120" s="18"/>
+      <c r="G120" s="5"/>
+      <c r="H120" s="3"/>
+    </row>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121" s="3">
         <v>82</v>
       </c>
@@ -3035,12 +3323,15 @@
       <c r="E121" s="4">
         <v>3</v>
       </c>
-      <c r="F121" s="5"/>
-      <c r="G121" s="3" t="s">
+      <c r="F121" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G121" s="5"/>
+      <c r="H121" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122" s="3">
         <v>83</v>
       </c>
@@ -3056,12 +3347,15 @@
       <c r="E122" s="4">
         <v>3</v>
       </c>
-      <c r="F122" s="5"/>
-      <c r="G122" s="3" t="s">
+      <c r="F122" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G122" s="5"/>
+      <c r="H122" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123" s="3">
         <v>84</v>
       </c>
@@ -3077,12 +3371,15 @@
       <c r="E123" s="4">
         <v>3</v>
       </c>
-      <c r="F123" s="5"/>
-      <c r="G123" s="3" t="s">
+      <c r="F123" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G123" s="5"/>
+      <c r="H123" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124" s="3">
         <v>85</v>
       </c>
@@ -3098,39 +3395,45 @@
       <c r="E124" s="4">
         <v>3</v>
       </c>
-      <c r="F124" s="5"/>
-      <c r="G124" s="3" t="s">
+      <c r="F124" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G124" s="5"/>
+      <c r="H124" s="3" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125" s="3"/>
       <c r="B125" s="4"/>
       <c r="C125" s="24"/>
       <c r="D125" s="24"/>
       <c r="E125" s="4"/>
-      <c r="F125" s="5"/>
-      <c r="G125" s="3"/>
-    </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F125" s="18"/>
+      <c r="G125" s="5"/>
+      <c r="H125" s="3"/>
+    </row>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126" s="3"/>
       <c r="B126" s="26"/>
       <c r="C126" s="26"/>
       <c r="D126" s="24"/>
       <c r="E126" s="4"/>
-      <c r="F126" s="5"/>
-      <c r="G126" s="3"/>
-    </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F126" s="18"/>
+      <c r="G126" s="5"/>
+      <c r="H126" s="3"/>
+    </row>
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127" s="3"/>
       <c r="B127" s="1"/>
       <c r="C127" s="15"/>
       <c r="D127" s="24"/>
       <c r="E127" s="4"/>
-      <c r="F127" s="5"/>
-      <c r="G127" s="3"/>
-    </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F127" s="18"/>
+      <c r="G127" s="5"/>
+      <c r="H127" s="3"/>
+    </row>
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128" s="3">
         <v>1</v>
       </c>
@@ -3144,12 +3447,15 @@
       <c r="E128" s="4">
         <v>3</v>
       </c>
-      <c r="F128" s="5"/>
-      <c r="G128" s="8" t="s">
+      <c r="F128" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G128" s="5"/>
+      <c r="H128" s="8" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A129" s="3">
         <v>2</v>
       </c>
@@ -3163,12 +3469,15 @@
       <c r="E129" s="4">
         <v>3</v>
       </c>
-      <c r="F129" s="5"/>
-      <c r="G129" s="8" t="s">
+      <c r="F129" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G129" s="5"/>
+      <c r="H129" s="8" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A130" s="3">
         <v>3</v>
       </c>
@@ -3182,12 +3491,15 @@
       <c r="E130" s="4">
         <v>3</v>
       </c>
-      <c r="F130" s="5"/>
-      <c r="G130" s="8" t="s">
+      <c r="F130" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G130" s="5"/>
+      <c r="H130" s="8" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A131" s="3">
         <v>4</v>
       </c>
@@ -3201,21 +3513,25 @@
       <c r="E131" s="4">
         <v>3</v>
       </c>
-      <c r="F131" s="5"/>
-      <c r="G131" s="7" t="s">
+      <c r="F131" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G131" s="5"/>
+      <c r="H131" s="7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A132" s="3"/>
       <c r="B132" s="9"/>
       <c r="C132" s="17"/>
       <c r="D132" s="24"/>
       <c r="E132" s="4"/>
-      <c r="F132" s="5"/>
-      <c r="G132" s="7"/>
-    </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F132" s="18"/>
+      <c r="G132" s="5"/>
+      <c r="H132" s="7"/>
+    </row>
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A133" s="3">
         <v>5</v>
       </c>
@@ -3229,12 +3545,15 @@
       <c r="E133" s="4">
         <v>3</v>
       </c>
-      <c r="F133" s="5"/>
-      <c r="G133" s="8" t="s">
+      <c r="F133" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G133" s="5"/>
+      <c r="H133" s="8" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A134" s="3">
         <v>6</v>
       </c>
@@ -3248,12 +3567,15 @@
       <c r="E134" s="4">
         <v>3</v>
       </c>
-      <c r="F134" s="5"/>
-      <c r="G134" s="8" t="s">
+      <c r="F134" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G134" s="5"/>
+      <c r="H134" s="8" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A135" s="3">
         <v>7</v>
       </c>
@@ -3267,12 +3589,15 @@
       <c r="E135" s="4">
         <v>3</v>
       </c>
-      <c r="F135" s="5"/>
-      <c r="G135" s="8" t="s">
+      <c r="F135" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G135" s="5"/>
+      <c r="H135" s="8" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A136" s="3">
         <v>8</v>
       </c>
@@ -3286,12 +3611,15 @@
       <c r="E136" s="4">
         <v>3</v>
       </c>
-      <c r="F136" s="5"/>
-      <c r="G136" s="11" t="s">
+      <c r="F136" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G136" s="5"/>
+      <c r="H136" s="11" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A137" s="3">
         <v>9</v>
       </c>
@@ -3305,12 +3633,15 @@
       <c r="E137" s="4">
         <v>4</v>
       </c>
-      <c r="F137" s="5"/>
-      <c r="G137" s="8" t="s">
+      <c r="F137" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G137" s="5"/>
+      <c r="H137" s="8" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A138" s="3">
         <v>10</v>
       </c>
@@ -3324,12 +3655,15 @@
       <c r="E138" s="4">
         <v>3</v>
       </c>
-      <c r="F138" s="5"/>
-      <c r="G138" s="8" t="s">
+      <c r="F138" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G138" s="5"/>
+      <c r="H138" s="8" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A139" s="3">
         <v>11</v>
       </c>
@@ -3343,12 +3677,15 @@
       <c r="E139" s="4">
         <v>3</v>
       </c>
-      <c r="F139" s="5"/>
-      <c r="G139" s="7" t="s">
+      <c r="F139" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G139" s="5"/>
+      <c r="H139" s="7" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A140" s="3">
         <v>12</v>
       </c>
@@ -3362,12 +3699,15 @@
       <c r="E140" s="4">
         <v>3</v>
       </c>
-      <c r="F140" s="5"/>
-      <c r="G140" s="8" t="s">
+      <c r="F140" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G140" s="5"/>
+      <c r="H140" s="8" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A141" s="3">
         <v>13</v>
       </c>
@@ -3381,12 +3721,15 @@
       <c r="E141" s="4">
         <v>3</v>
       </c>
-      <c r="F141" s="5"/>
-      <c r="G141" s="8" t="s">
+      <c r="F141" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G141" s="5"/>
+      <c r="H141" s="8" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A142" s="3">
         <v>14</v>
       </c>
@@ -3400,12 +3743,15 @@
       <c r="E142" s="4">
         <v>3</v>
       </c>
-      <c r="F142" s="5"/>
-      <c r="G142" s="8" t="s">
+      <c r="F142" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G142" s="5"/>
+      <c r="H142" s="8" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A143" s="3">
         <v>15</v>
       </c>
@@ -3419,12 +3765,15 @@
       <c r="E143" s="4">
         <v>3</v>
       </c>
-      <c r="F143" s="5"/>
-      <c r="G143" s="8" t="s">
+      <c r="F143" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G143" s="5"/>
+      <c r="H143" s="8" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A144" s="3">
         <v>16</v>
       </c>
@@ -3438,12 +3787,15 @@
       <c r="E144" s="4">
         <v>4</v>
       </c>
-      <c r="F144" s="5"/>
-      <c r="G144" s="8" t="s">
+      <c r="F144" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G144" s="5"/>
+      <c r="H144" s="8" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A145" s="3">
         <v>17</v>
       </c>
@@ -3457,21 +3809,25 @@
       <c r="E145" s="4">
         <v>3</v>
       </c>
-      <c r="F145" s="5"/>
-      <c r="G145" s="8" t="s">
+      <c r="F145" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G145" s="5"/>
+      <c r="H145" s="8" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A146" s="3"/>
       <c r="B146" s="1"/>
       <c r="C146" s="15"/>
       <c r="D146" s="24"/>
       <c r="E146" s="4"/>
-      <c r="F146" s="5"/>
-      <c r="G146" s="3"/>
-    </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F146" s="18"/>
+      <c r="G146" s="5"/>
+      <c r="H146" s="3"/>
+    </row>
+    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A147" s="3">
         <v>18</v>
       </c>
@@ -3485,12 +3841,15 @@
       <c r="E147" s="4">
         <v>3</v>
       </c>
-      <c r="F147" s="5"/>
-      <c r="G147" s="8" t="s">
+      <c r="F147" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G147" s="5"/>
+      <c r="H147" s="8" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A148" s="3">
         <v>19</v>
       </c>
@@ -3504,12 +3863,15 @@
       <c r="E148" s="4">
         <v>3</v>
       </c>
-      <c r="F148" s="5"/>
-      <c r="G148" s="8" t="s">
+      <c r="F148" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G148" s="5"/>
+      <c r="H148" s="8" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A149" s="3">
         <v>20</v>
       </c>
@@ -3523,12 +3885,15 @@
       <c r="E149" s="4">
         <v>3</v>
       </c>
-      <c r="F149" s="5"/>
-      <c r="G149" s="8" t="s">
+      <c r="F149" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G149" s="5"/>
+      <c r="H149" s="8" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A150" s="3">
         <v>21</v>
       </c>
@@ -3542,12 +3907,15 @@
       <c r="E150" s="4">
         <v>3</v>
       </c>
-      <c r="F150" s="5"/>
-      <c r="G150" s="8" t="s">
+      <c r="F150" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G150" s="5"/>
+      <c r="H150" s="8" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A151" s="3">
         <v>22</v>
       </c>
@@ -3561,12 +3929,15 @@
       <c r="E151" s="4">
         <v>3</v>
       </c>
-      <c r="F151" s="5"/>
-      <c r="G151" s="8" t="s">
+      <c r="F151" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G151" s="5"/>
+      <c r="H151" s="8" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A152" s="3">
         <v>23</v>
       </c>
@@ -3580,21 +3951,25 @@
       <c r="E152" s="4">
         <v>3</v>
       </c>
-      <c r="F152" s="5"/>
-      <c r="G152" s="8" t="s">
+      <c r="F152" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G152" s="5"/>
+      <c r="H152" s="8" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A153" s="3"/>
       <c r="B153" s="4"/>
       <c r="C153" s="19"/>
       <c r="D153" s="24"/>
       <c r="E153" s="4"/>
-      <c r="F153" s="5"/>
-      <c r="G153" s="3"/>
-    </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F153" s="18"/>
+      <c r="G153" s="5"/>
+      <c r="H153" s="3"/>
+    </row>
+    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A154" s="3">
         <v>24</v>
       </c>
@@ -3608,12 +3983,15 @@
       <c r="E154" s="4">
         <v>3</v>
       </c>
-      <c r="F154" s="5"/>
-      <c r="G154" s="11" t="s">
+      <c r="F154" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G154" s="5"/>
+      <c r="H154" s="11" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A155" s="3">
         <v>25</v>
       </c>
@@ -3627,12 +4005,15 @@
       <c r="E155" s="4">
         <v>3</v>
       </c>
-      <c r="F155" s="5"/>
-      <c r="G155" s="11" t="s">
+      <c r="F155" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G155" s="5"/>
+      <c r="H155" s="11" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A156" s="3">
         <v>26</v>
       </c>
@@ -3646,12 +4027,15 @@
       <c r="E156" s="4">
         <v>3</v>
       </c>
-      <c r="F156" s="5"/>
-      <c r="G156" s="11" t="s">
+      <c r="F156" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G156" s="5"/>
+      <c r="H156" s="11" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A157" s="3">
         <v>27</v>
       </c>
@@ -3665,12 +4049,15 @@
       <c r="E157" s="4">
         <v>3</v>
       </c>
-      <c r="F157" s="5"/>
-      <c r="G157" s="8" t="s">
+      <c r="F157" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G157" s="5"/>
+      <c r="H157" s="8" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A158" s="3">
         <v>28</v>
       </c>
@@ -3684,12 +4071,15 @@
       <c r="E158" s="4">
         <v>3</v>
       </c>
-      <c r="F158" s="5"/>
-      <c r="G158" s="8" t="s">
+      <c r="F158" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G158" s="5"/>
+      <c r="H158" s="8" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A159" s="3">
         <v>29</v>
       </c>
@@ -3705,12 +4095,15 @@
       <c r="E159" s="4">
         <v>2</v>
       </c>
-      <c r="F159" s="5"/>
-      <c r="G159" s="8" t="s">
+      <c r="F159" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G159" s="5"/>
+      <c r="H159" s="8" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A160" s="3">
         <v>30</v>
       </c>
@@ -3726,12 +4119,15 @@
       <c r="E160" s="4">
         <v>4</v>
       </c>
-      <c r="F160" s="5"/>
-      <c r="G160" s="8" t="s">
+      <c r="F160" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G160" s="5"/>
+      <c r="H160" s="8" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A161" s="3">
         <v>31</v>
       </c>
@@ -3747,8 +4143,11 @@
       <c r="E161" s="4">
         <v>6</v>
       </c>
-      <c r="F161" s="5"/>
-      <c r="G161" s="8" t="s">
+      <c r="F161" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G161" s="5"/>
+      <c r="H161" s="8" t="s">
         <v>93</v>
       </c>
     </row>

</xml_diff>